<commit_message>
Importing more of the Excel template
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF765DAF-A4BC-4B14-BC8A-06693F1623A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA05D7B2-E72C-4D31-8722-51288DE03044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30360" yWindow="0" windowWidth="21240" windowHeight="21000" tabRatio="1000" activeTab="7" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="22260" yWindow="0" windowWidth="29340" windowHeight="21000" tabRatio="1000" firstSheet="4" activeTab="17" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="solve_sequence" sheetId="11" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="220">
   <si>
     <t>commodity</t>
   </si>
@@ -677,12 +677,6 @@
     <t>profile</t>
   </si>
   <si>
-    <t>i2020</t>
-  </si>
-  <si>
-    <t>i2025</t>
-  </si>
-  <si>
     <t>Wind1</t>
   </si>
   <si>
@@ -732,6 +726,12 @@
   </si>
   <si>
     <t>A flag whether the node has a balance constraint.</t>
+  </si>
+  <si>
+    <t>Gas_node</t>
+  </si>
+  <si>
+    <t>Gas</t>
   </si>
 </sst>
 </file>
@@ -1240,11 +1240,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F74504-C20F-4059-A948-7FE0BCADBAA0}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1287,6 +1285,414 @@
         <v>79</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>10000</v>
+      </c>
+      <c r="E3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4">
+        <v>10000</v>
+      </c>
+      <c r="E4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5">
+        <v>10000</v>
+      </c>
+      <c r="E5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6">
+        <v>10000</v>
+      </c>
+      <c r="E6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7">
+        <v>10000</v>
+      </c>
+      <c r="E7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
+        <v>10000</v>
+      </c>
+      <c r="E8">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9">
+        <v>10000</v>
+      </c>
+      <c r="E9">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10">
+        <v>10000</v>
+      </c>
+      <c r="E10">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11">
+        <v>10000</v>
+      </c>
+      <c r="E11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12">
+        <v>10000</v>
+      </c>
+      <c r="E12">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13">
+        <v>10000</v>
+      </c>
+      <c r="E13">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14">
+        <v>10000</v>
+      </c>
+      <c r="E14">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15">
+        <v>10000</v>
+      </c>
+      <c r="E15">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16">
+        <v>10000</v>
+      </c>
+      <c r="E16">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17">
+        <v>10000</v>
+      </c>
+      <c r="E17">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18">
+        <v>10000</v>
+      </c>
+      <c r="E18">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19">
+        <v>10000</v>
+      </c>
+      <c r="E19">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20">
+        <v>10000</v>
+      </c>
+      <c r="E20">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21">
+        <v>10000</v>
+      </c>
+      <c r="E21">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22">
+        <v>10000</v>
+      </c>
+      <c r="E22">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23">
+        <v>10000</v>
+      </c>
+      <c r="E23">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24">
+        <v>10000</v>
+      </c>
+      <c r="E24">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25">
+        <v>10000</v>
+      </c>
+      <c r="E25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26">
+        <v>10000</v>
+      </c>
+      <c r="E26">
+        <v>10000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1294,10 +1700,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99DA432-9F88-4927-B437-CA09DA61AB93}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,10 +1736,21 @@
         <v>39</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C3">
         <v>0.34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C4">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -1400,10 +1817,10 @@
         <v>39</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -1416,7 +1833,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C8DA1-A436-4EFF-909D-4060C6CDB560}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1473,6 +1890,40 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1482,9 +1933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D44D2B2-1DE7-400D-8C40-2CD59BEE6EC3}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1619,9 +2068,6 @@
       <c r="B3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C3">
-        <v>0.99</v>
-      </c>
       <c r="D3">
         <v>100</v>
       </c>
@@ -1647,7 +2093,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C5CDA4-FFE3-4938-9213-CC2F8772241C}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1755,7 +2203,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F877950-BDFF-4B0B-89C1-36AC76A9D30A}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1794,6 +2242,342 @@
       </c>
       <c r="E2" s="9" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26">
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>
@@ -1840,10 +2624,10 @@
         <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -1853,10 +2637,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE19B28-F2BE-409F-B1A6-1F5F2146177E}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U42" sqref="U42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1866,8 +2650,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>46</v>
+      <c r="A1" s="9" t="s">
+        <v>200</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -1877,96 +2661,99 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>3</v>
+      <c r="A2" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>200</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>38</v>
+      <c r="A3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3">
+        <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C4">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="C5">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C6">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C9">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C10">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C11">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C12">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C13">
         <v>0.25</v>
@@ -1974,7 +2761,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C14">
         <v>0.25</v>
@@ -1982,7 +2769,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C15">
         <v>0.25</v>
@@ -1990,7 +2777,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C16">
         <v>0.25</v>
@@ -1998,7 +2785,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C17">
         <v>0.25</v>
@@ -2006,7 +2793,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C18">
         <v>0.25</v>
@@ -2014,7 +2801,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C19">
         <v>0.25</v>
@@ -2022,7 +2809,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C20">
         <v>0.25</v>
@@ -2030,7 +2817,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C21">
         <v>0.25</v>
@@ -2038,7 +2825,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C22">
         <v>0.25</v>
@@ -2046,7 +2833,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C23">
         <v>0.25</v>
@@ -2054,7 +2841,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C24">
         <v>0.25</v>
@@ -2062,7 +2849,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C25">
         <v>0.25</v>
@@ -2070,17 +2857,9 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C26">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C27">
         <v>0.25</v>
       </c>
     </row>
@@ -2093,9 +2872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6619729E-584E-41E3-B72E-7B2979330C88}">
   <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2277,7 +3054,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E3">
         <v>0.4</v>
@@ -2301,7 +3078,7 @@
         <v>39</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2313,7 +3090,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2351,7 +3128,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>115</v>
@@ -2468,10 +3245,10 @@
         <v>39</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>201</v>
+        <v>102</v>
       </c>
       <c r="H3">
         <v>100</v>
@@ -2482,10 +3259,10 @@
         <v>39</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>202</v>
+        <v>103</v>
       </c>
       <c r="H4">
         <v>100</v>
@@ -2572,10 +3349,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2836,7 +3613,7 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -2853,10 +3630,10 @@
         <v>199</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -2994,9 +3771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C14DBC-6D65-48AD-9110-D1593FB205E8}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3474,7 +4249,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -3595,10 +4370,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -4041,7 +4816,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>139</v>
@@ -4064,9 +4839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE8329C-91C4-4EB7-BC1D-5B4592D8DD79}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4197,10 +4970,10 @@
         <v>43</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4261,10 +5034,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4280,7 +5053,7 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D1" t="s">
         <v>82</v>
@@ -4289,7 +5062,7 @@
         <v>83</v>
       </c>
       <c r="F1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G1" t="s">
         <v>84</v>
@@ -4401,13 +5174,13 @@
         <v>39</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I3">
         <v>150</v>
@@ -4418,16 +5191,32 @@
         <v>39</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I4">
         <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -4437,11 +5226,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51F2ED7-E82A-4D3D-A4CE-E6A52C2211BA}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4527,6 +5314,34 @@
         <v>15</v>
       </c>
     </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
All Excel input data imported to FlexTool3
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA05D7B2-E72C-4D31-8722-51288DE03044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974FE648-7C6F-4EBB-92CA-3C2975D5C085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22260" yWindow="0" windowWidth="29340" windowHeight="21000" tabRatio="1000" firstSheet="4" activeTab="17" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="22260" yWindow="0" windowWidth="29340" windowHeight="21000" tabRatio="1000" firstSheet="4" activeTab="7" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="solve_sequence" sheetId="11" r:id="rId1"/>
@@ -2639,9 +2639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE19B28-F2BE-409F-B1A6-1F5F2146177E}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5036,8 +5034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Moved ramps to unit__nodes
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974FE648-7C6F-4EBB-92CA-3C2975D5C085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2C5BD5-948F-43F5-9D35-25486596BB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22260" yWindow="0" windowWidth="29340" windowHeight="21000" tabRatio="1000" firstSheet="4" activeTab="7" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="22260" yWindow="0" windowWidth="29340" windowHeight="21000" tabRatio="1000" firstSheet="16" activeTab="18" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="solve_sequence" sheetId="11" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="220">
   <si>
     <t>commodity</t>
   </si>
@@ -2868,9 +2868,9 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6619729E-584E-41E3-B72E-7B2979330C88}">
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2879,7 +2879,7 @@
     <col min="3" max="14" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -2934,34 +2934,22 @@
         <v>157</v>
       </c>
       <c r="T1" t="s">
-        <v>173</v>
+        <v>33</v>
       </c>
       <c r="U1" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="V1" t="s">
-        <v>162</v>
+        <v>34</v>
       </c>
       <c r="W1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="X1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>174</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>165</v>
-      </c>
-      <c r="AB1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -3020,34 +3008,22 @@
         <v>156</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>158</v>
+        <v>16</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>159</v>
+        <v>17</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>161</v>
+        <v>18</v>
       </c>
       <c r="W2" s="9" t="s">
-        <v>163</v>
+        <v>20</v>
       </c>
       <c r="X2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB2" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
@@ -3071,7 +3047,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -3362,7 +3338,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C13F0C3-2BD2-4859-9713-8823A445C2E8}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3382,9 +3360,18 @@
       <c r="E1" t="s">
         <v>198</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="F1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" t="s">
+        <v>164</v>
+      </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -3405,9 +3392,18 @@
       <c r="E2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="F2" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>163</v>
+      </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -3421,7 +3417,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5426421-1769-4717-A94E-940B9D37985D}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3441,9 +3439,18 @@
       <c r="E1" t="s">
         <v>198</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="F1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" t="s">
+        <v>164</v>
+      </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -3464,9 +3471,18 @@
       <c r="E2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="F2" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>163</v>
+      </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -5034,7 +5050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Good progress in getting the new data structures to work
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13494725-4C70-4760-B4A4-5E1BBF7E3394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503A1430-E3CE-441B-BC43-1E4A90F42D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="1000" firstSheet="16" activeTab="23" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="solve_sequence" sheetId="11" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="timeblocks_timeline" sheetId="16" r:id="rId7"/>
     <sheet name="node_c" sheetId="7" r:id="rId8"/>
     <sheet name="node_p" sheetId="19" r:id="rId9"/>
-    <sheet name="node_t" sheetId="20" r:id="rId10"/>
+    <sheet name="node_t" sheetId="47" r:id="rId10"/>
     <sheet name="commodity_c" sheetId="1" r:id="rId11"/>
     <sheet name="commodity_p" sheetId="45" r:id="rId12"/>
     <sheet name="commodity_node" sheetId="23" r:id="rId13"/>
@@ -33,26 +33,23 @@
     <sheet name="profile_t" sheetId="10" r:id="rId18"/>
     <sheet name="unit_c" sheetId="18" r:id="rId19"/>
     <sheet name="unit_p" sheetId="21" r:id="rId20"/>
-    <sheet name="unit_t" sheetId="22" r:id="rId21"/>
-    <sheet name="unit_sourceProfile" sheetId="41" r:id="rId22"/>
-    <sheet name="unit_sourceNode_c" sheetId="38" r:id="rId23"/>
-    <sheet name="unit_sinkNode_c" sheetId="35" r:id="rId24"/>
-    <sheet name="unit_sourceNode_t" sheetId="39" r:id="rId25"/>
-    <sheet name="unit_sinkNode_t" sheetId="36" r:id="rId26"/>
-    <sheet name="constraint_sense_c" sheetId="44" r:id="rId27"/>
-    <sheet name="unit_sourceNode_constraint_c" sheetId="40" r:id="rId28"/>
-    <sheet name="unit_sinkNode_constraint_c" sheetId="37" r:id="rId29"/>
-    <sheet name="group_c" sheetId="6" r:id="rId30"/>
-    <sheet name="group_p" sheetId="46" r:id="rId31"/>
-    <sheet name="group_connection" sheetId="26" r:id="rId32"/>
-    <sheet name="group_connection_node" sheetId="28" r:id="rId33"/>
-    <sheet name="group_node" sheetId="27" r:id="rId34"/>
-    <sheet name="group_unit" sheetId="29" r:id="rId35"/>
-    <sheet name="group_unit_node" sheetId="30" r:id="rId36"/>
-    <sheet name="reserve_connection_node_c" sheetId="31" r:id="rId37"/>
-    <sheet name="reserve_group_c" sheetId="32" r:id="rId38"/>
-    <sheet name="reserve_group_t" sheetId="34" r:id="rId39"/>
-    <sheet name="reserve_unit_node_c" sheetId="33" r:id="rId40"/>
+    <sheet name="unit_t" sheetId="48" r:id="rId21"/>
+    <sheet name="unit_profile_c" sheetId="41" r:id="rId22"/>
+    <sheet name="unit_node_c" sheetId="38" r:id="rId23"/>
+    <sheet name="unit_node_t" sheetId="49" r:id="rId24"/>
+    <sheet name="constraint_sense_c" sheetId="44" r:id="rId25"/>
+    <sheet name="unit_node_constraint_c" sheetId="40" r:id="rId26"/>
+    <sheet name="group_c" sheetId="6" r:id="rId27"/>
+    <sheet name="group_p" sheetId="46" r:id="rId28"/>
+    <sheet name="group_connection" sheetId="26" r:id="rId29"/>
+    <sheet name="group_connection_node" sheetId="28" r:id="rId30"/>
+    <sheet name="group_node" sheetId="27" r:id="rId31"/>
+    <sheet name="group_unit" sheetId="29" r:id="rId32"/>
+    <sheet name="group_unit_node" sheetId="30" r:id="rId33"/>
+    <sheet name="reserve_connection_node_c" sheetId="31" r:id="rId34"/>
+    <sheet name="reserve_group_c" sheetId="32" r:id="rId35"/>
+    <sheet name="reserve_group_t" sheetId="34" r:id="rId36"/>
+    <sheet name="reserve_unit_node_c" sheetId="33" r:id="rId37"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -72,8 +69,112 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Kiviluoma Juha</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{9A6B41AD-099E-4AAD-B13D-62784A5D6AFD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Possible parameters
+inflow: [MWh] Inflow into the node (negative is outflow). Constant or time.
+penalty_up: [€/MW] Penalty cost for increasing consumption in the node. Constant or time.
+penalty_down: [€/MW] Penalty cost for decreasing consumption in the node. Constant or time.
+self_discharge_loss: [e.g. 0.01 means 1% every hour] Loss of stored energy over time. Constant or time.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Kiviluoma Juha</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{D8E7EB74-D2C2-4376-88D2-853C920671FD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Possible parameters
+efficiency: [factor] Efficiency of a unit. Constant or time.
+variable_cost: [CUR/MWh] Variable operating cost. Fuel and CO2 cost can be given through separate means. Constant or time.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Kiviluoma Juha</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{FF4C7C05-3B74-4BCA-B836-EBC67CC1C968}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Possible parameters
+efficiency: [factor] Efficiency of a unit. Constant or time.
+variable_cost: [CUR/MWh] Variable operating cost. Fuel and CO2 cost can be given through separate means. Constant or time.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Kiviluoma Juha</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{7A34832B-70DA-420B-8847-70DC4A2B17D3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Possible parameters
+variable_cost: [CUR/MWh] Variable operating cost. Fuel and CO2 cost can be given through separate means. Constant or time.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="234">
   <si>
     <t>commodity</t>
   </si>
@@ -748,13 +849,40 @@
   </si>
   <si>
     <t>no_startup</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>source_sink</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>sink</t>
+  </si>
+  <si>
+    <t>profile_method</t>
+  </si>
+  <si>
+    <t>upper_limit</t>
+  </si>
+  <si>
+    <t>Choice of profile method (upper_limit, lower_limit, fixed). Negative values also possible.</t>
+  </si>
+  <si>
+    <t>c01</t>
+  </si>
+  <si>
+    <t>greater_than</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -762,8 +890,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -836,6 +978,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE088C1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEBCDC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -849,7 +1021,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -865,12 +1037,24 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEEBCDC"/>
+      <color rgb="FFE088C1"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -880,6 +1064,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1181,7 +1369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9640D032-37A5-47CC-8407-C4F7168BB93B}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1255,471 +1443,326 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F74504-C20F-4059-A948-7FE0BCADBAA0}">
-  <dimension ref="A1:G26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56195B5-58E5-4A49-9514-C11CC17CB482}">
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>38</v>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E3">
-        <v>10000</v>
-      </c>
-      <c r="F3">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4">
+        <v>-10</v>
+      </c>
+      <c r="D4">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E4">
-        <v>10000</v>
-      </c>
-      <c r="F4">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5">
+        <v>-20</v>
+      </c>
+      <c r="D5">
+        <v>-100</v>
+      </c>
+      <c r="K5" s="16"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E5">
-        <v>10000</v>
-      </c>
-      <c r="F5">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6">
+        <v>-30</v>
+      </c>
+      <c r="D6">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E6">
-        <v>10000</v>
-      </c>
-      <c r="F6">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7">
+        <v>-40</v>
+      </c>
+      <c r="D7">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E7">
-        <v>10000</v>
-      </c>
-      <c r="F7">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8">
+        <v>-50</v>
+      </c>
+      <c r="D8">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E8">
-        <v>10000</v>
-      </c>
-      <c r="F8">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9">
+        <v>-60</v>
+      </c>
+      <c r="D9">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E9">
-        <v>10000</v>
-      </c>
-      <c r="F9">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10">
+        <v>-70</v>
+      </c>
+      <c r="D10">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E10">
-        <v>10000</v>
-      </c>
-      <c r="F10">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11">
+        <v>-80</v>
+      </c>
+      <c r="D11">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E11">
-        <v>10000</v>
-      </c>
-      <c r="F11">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12">
+        <v>-90</v>
+      </c>
+      <c r="D12">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E12">
-        <v>10000</v>
-      </c>
-      <c r="F12">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13">
+        <v>-100</v>
+      </c>
+      <c r="D13">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E13">
-        <v>10000</v>
-      </c>
-      <c r="F13">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14">
+        <v>-110</v>
+      </c>
+      <c r="D14">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E14">
-        <v>10000</v>
-      </c>
-      <c r="F14">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15">
+        <v>-120</v>
+      </c>
+      <c r="D15">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E15">
-        <v>10000</v>
-      </c>
-      <c r="F15">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16">
+        <v>-130</v>
+      </c>
+      <c r="D16">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E16">
-        <v>10000</v>
-      </c>
-      <c r="F16">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17">
+        <v>-140</v>
+      </c>
+      <c r="D17">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E17">
-        <v>10000</v>
-      </c>
-      <c r="F17">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18">
+        <v>-150</v>
+      </c>
+      <c r="D18">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E18">
-        <v>10000</v>
-      </c>
-      <c r="F18">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19">
+        <v>-160</v>
+      </c>
+      <c r="D19">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E19">
-        <v>10000</v>
-      </c>
-      <c r="F19">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20">
+        <v>-170</v>
+      </c>
+      <c r="D20">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E20">
-        <v>10000</v>
-      </c>
-      <c r="F20">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21">
+        <v>-180</v>
+      </c>
+      <c r="D21">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E21">
-        <v>10000</v>
-      </c>
-      <c r="F21">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22">
+        <v>-190</v>
+      </c>
+      <c r="D22">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E22">
-        <v>10000</v>
-      </c>
-      <c r="F22">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23">
+        <v>-200</v>
+      </c>
+      <c r="D23">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E23">
-        <v>10000</v>
-      </c>
-      <c r="F23">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24">
+        <v>-210</v>
+      </c>
+      <c r="D24">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E24">
-        <v>10000</v>
-      </c>
-      <c r="F24">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25">
+        <v>-220</v>
+      </c>
+      <c r="D25">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E25">
-        <v>10000</v>
-      </c>
-      <c r="F25">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26">
+        <v>-230</v>
+      </c>
+      <c r="D26">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E26">
-        <v>10000</v>
-      </c>
-      <c r="F26">
-        <v>10000</v>
+      <c r="C27">
+        <v>-240</v>
+      </c>
+      <c r="D27">
+        <v>-100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1727,9 +1770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99DA432-9F88-4927-B437-CA09DA61AB93}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1796,9 +1837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E20CFBA-1F92-463C-919B-31F910121997}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1866,9 +1905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EFF0A7-3963-4998-9482-2033971B0C97}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2085,9 +2122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C5CDA4-FFE3-4938-9213-CC2F8772241C}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2194,386 +2229,247 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F877950-BDFF-4B0B-89C1-36AC76A9D30A}">
-  <dimension ref="A1:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F877950-BDFF-4B0B-89C1-36AC76A9D30A}">
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D3">
+      <c r="C4">
         <v>0.99</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="4" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D4">
+      <c r="C5">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="K5" s="16"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D5">
+      <c r="C6">
         <v>0.99</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="4" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D6">
+      <c r="C7">
         <v>0.99</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="4" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D7">
+      <c r="C8">
         <v>0.99</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="4" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D8">
+      <c r="C9">
         <v>0.99</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="4" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D9">
+      <c r="C10">
         <v>0.99</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="4" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D10">
+      <c r="C11">
         <v>0.99</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="4" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D11">
+      <c r="C12">
         <v>0.99</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="4" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D12">
+      <c r="C13">
         <v>0.99</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="4" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D13">
+      <c r="C14">
         <v>0.99</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="4" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D14">
+      <c r="C15">
         <v>0.99</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="4" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D15">
+      <c r="C16">
         <v>0.99</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="4" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D16">
+      <c r="C17">
         <v>0.99</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="4" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D17">
+      <c r="C18">
         <v>0.99</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="4" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D18">
+      <c r="C19">
         <v>0.99</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="4" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D19">
+      <c r="C20">
         <v>0.99</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="4" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D20">
+      <c r="C21">
         <v>0.99</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="4" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D21">
+      <c r="C22">
         <v>0.99</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="4" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D22">
+      <c r="C23">
         <v>0.99</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="4" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D23">
+      <c r="C24">
         <v>0.99</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="4" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D24">
+      <c r="C25">
         <v>0.99</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="4" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D25">
+      <c r="C26">
         <v>0.99</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="4" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D26">
+      <c r="C27">
         <v>0.99</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2631,14 +2527,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE19B28-F2BE-409F-B1A6-1F5F2146177E}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2864,9 +2758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6619729E-584E-41E3-B72E-7B2979330C88}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3035,6 +2927,9 @@
       <c r="F3" s="5"/>
       <c r="G3">
         <v>100</v>
+      </c>
+      <c r="J3">
+        <v>0.08</v>
       </c>
       <c r="K3">
         <v>1000</v>
@@ -3204,9 +3099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F519FEB-FCA9-4C11-88F7-D4EA23EF6482}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3320,423 +3213,304 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B01DC28-9F07-4853-988E-EB648783EBC1}">
-  <dimension ref="A1:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A4A219-02B1-4261-8559-589A0949A31B}">
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E3">
+      <c r="C4">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C4" s="4" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E4">
+      <c r="C5">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="K5" s="16"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E5">
+      <c r="C6">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C6" s="4" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E6">
+      <c r="C7">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C7" s="4" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E7">
+      <c r="C8">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C8" s="4" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E8">
+      <c r="C9">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C9" s="4" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E9">
+      <c r="C10">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C10" s="4" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E10">
+      <c r="C11">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C11" s="4" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E11">
+      <c r="C12">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C12" s="4" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E12">
+      <c r="C13">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C13" s="4" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E13">
+      <c r="C14">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C14" s="4" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E14">
+      <c r="C15">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C15" s="4" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E15">
+      <c r="C16">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C16" s="4" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E16">
+      <c r="C17">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C17" s="4" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E17">
+      <c r="C18">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C18" s="4" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E18">
+      <c r="C19">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C19" s="4" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E19">
+      <c r="C20">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C20" s="4" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E20">
+      <c r="C21">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C21" s="4" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E21">
+      <c r="C22">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C22" s="4" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E22">
+      <c r="C23">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C23" s="4" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E23">
+      <c r="C24">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C24" s="4" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E24">
+      <c r="C25">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C25" s="4" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E25">
+      <c r="C26">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C26" s="4" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E26">
+      <c r="C27">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1EE4BC-08B3-4CC5-9A8F-D2957036E873}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="4" customWidth="1"/>
-    <col min="3" max="6" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
+    <col min="4" max="7" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="D2" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>193</v>
+      </c>
+      <c r="D3" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3746,241 +3520,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C13F0C3-2BD2-4859-9713-8823A445C2E8}">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="9" width="11.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F1" t="s">
-        <v>165</v>
-      </c>
-      <c r="G1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I1" t="s">
-        <v>156</v>
-      </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5426421-1769-4717-A94E-940B9D37985D}">
-  <dimension ref="A1:L5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="9" width="11.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F1" t="s">
-        <v>165</v>
-      </c>
-      <c r="G1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I1" t="s">
-        <v>156</v>
-      </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827EC50C-6D87-4D05-B8DC-67E9650A815B}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3989,26 +3529,38 @@
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="11" customWidth="1"/>
-    <col min="5" max="9" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="20" customWidth="1"/>
+    <col min="5" max="10" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F1" t="s">
         <v>190</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="G1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J1" t="s">
+        <v>156</v>
+      </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -4018,497 +3570,395 @@
       <c r="C2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>38</v>
+      <c r="D2" s="19" t="s">
+        <v>226</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="G2" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>155</v>
+      </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA05E91-39CC-4A40-94F0-72A13CA8A05E}">
-  <dimension ref="A1:L26"/>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54CEF76-2D28-40D4-A5BB-1AAB8A75E52F}">
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O54" sqref="O54"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="11" customWidth="1"/>
-    <col min="5" max="9" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C3" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="C4" s="18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="B5" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E3">
+      <c r="C6">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D4" s="11" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E4">
+      <c r="C7">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="K7" s="16"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E5">
+      <c r="C8">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D6" s="11" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E6">
+      <c r="C9">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D7" s="11" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E7">
+      <c r="C10">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D8" s="11" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E8">
+      <c r="C11">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D9" s="11" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E9">
+      <c r="C12">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D10" s="11" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E10">
+      <c r="C13">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D11" s="11" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E11">
+      <c r="C14">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D12" s="11" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E12">
+      <c r="C15">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D13" s="11" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E13">
+      <c r="C16">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D14" s="11" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E14">
+      <c r="C17">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D15" s="11" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E15">
+      <c r="C18">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D16" s="11" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E16">
+      <c r="C19">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D17" s="11" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E17">
+      <c r="C20">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D18" s="11" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E18">
+      <c r="C21">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D19" s="11" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E19">
+      <c r="C22">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D20" s="11" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E20">
+      <c r="C23">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D21" s="11" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E21">
+      <c r="C24">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D22" s="11" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E22">
+      <c r="C25">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D23" s="11" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E23">
+      <c r="C26">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D24" s="11" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E24">
+      <c r="C27">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D25" s="11" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E25">
+      <c r="C28">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D26" s="11" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E26">
+      <c r="C29">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C017E3-B844-46CF-8B82-D76F5D9D7ACD}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4552,65 +4002,338 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA1124C-4BD2-46D2-BD33-99ED754CAC73}">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="20" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="11" customWidth="1"/>
+    <col min="6" max="10" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="F4">
+        <v>-0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
+    <col min="3" max="15" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA1124C-4BD2-46D2-BD33-99ED754CAC73}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA54FD9A-FB2F-4111-AC75-F20843B34F53}">
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA52" sqref="AA52"/>
+      <selection activeCell="E3" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="11" customWidth="1"/>
-    <col min="5" max="9" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="4" customWidth="1"/>
+    <col min="4" max="10" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
       <c r="E1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>159</v>
+        <v>69</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>191</v>
+        <v>43</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+        <v>49</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4618,59 +4341,34 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD02974-D8C8-4B94-8C2E-2D6F98B9973B}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B745B3BE-1539-44A7-9F68-00D8AEBADA46}">
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="11" customWidth="1"/>
-    <col min="5" max="9" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="4" customWidth="1"/>
+    <col min="3" max="8" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" t="s">
-        <v>189</v>
-      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4796,233 +4494,6 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
-  <dimension ref="A1:N3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
-    <col min="3" max="15" width="11.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA54FD9A-FB2F-4111-AC75-F20843B34F53}">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
-    <col min="3" max="9" width="11.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B745B3BE-1539-44A7-9F68-00D8AEBADA46}">
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="4" customWidth="1"/>
-    <col min="3" max="8" width="11.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C65105-DA47-40FD-BED9-039766CD67C2}">
   <dimension ref="A1:L1"/>
   <sheetViews>
@@ -5063,7 +4534,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6F0B0-C8D9-4343-9EA4-859E87C9AF78}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -5116,7 +4587,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5455887B-7914-47A3-A368-88187BB1082B}">
   <dimension ref="A1:K1"/>
   <sheetViews>
@@ -5153,7 +4624,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8ED891B-8A85-405F-972C-9B1BFE92F9B9}">
   <dimension ref="A1:L1"/>
   <sheetViews>
@@ -5192,7 +4663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB87FF22-BB83-4D5E-B38D-455D581CF757}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -5273,7 +4744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{866244AD-1571-447F-BAEE-EFE2B5B3F812}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -5343,7 +4814,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E05E786-69CB-4CBA-9E06-4DF215E87C9C}">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -5400,6 +4871,87 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8C0D5E-7DB2-4BCF-8A8C-24C978AAECC4}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="13" customWidth="1"/>
+    <col min="6" max="12" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5478,87 +5030,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8C0D5E-7DB2-4BCF-8A8C-24C978AAECC4}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="13" customWidth="1"/>
-    <col min="6" max="12" width="11.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G1" t="s">
-        <v>184</v>
-      </c>
-      <c r="H1" t="s">
-        <v>175</v>
-      </c>
-      <c r="I1" t="s">
-        <v>177</v>
-      </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C14DBC-6D65-48AD-9110-D1593FB205E8}">
   <dimension ref="A1:D26"/>
@@ -5992,9 +5463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D727460B-F1B2-42C2-90E2-38E181F7AFC8}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6028,9 +5497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6174,8 +5641,11 @@
       <c r="G3" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="I3">
-        <v>150</v>
+      <c r="P3">
+        <v>10000</v>
+      </c>
+      <c r="Q3">
+        <v>10000</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -6191,8 +5661,11 @@
       <c r="G4" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="I4">
-        <v>150</v>
+      <c r="P4">
+        <v>10000</v>
+      </c>
+      <c r="Q4">
+        <v>10000</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -6202,6 +5675,12 @@
       <c r="B5" s="2" t="s">
         <v>197</v>
       </c>
+      <c r="P5">
+        <v>10000</v>
+      </c>
+      <c r="Q5">
+        <v>10000</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -6209,6 +5688,12 @@
       </c>
       <c r="B6" s="2" t="s">
         <v>210</v>
+      </c>
+      <c r="P6">
+        <v>10000</v>
+      </c>
+      <c r="Q6">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
@@ -6220,9 +5705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51F2ED7-E82A-4D3D-A4CE-E6A52C2211BA}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Start of unit testing
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,48 +8,49 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4483859-F815-4D0B-97D3-2645B4C98E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC17BD83-42F1-4100-875F-02300997AC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7530" yWindow="2220" windowWidth="25080" windowHeight="16200" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-28920" yWindow="5145" windowWidth="29040" windowHeight="16440" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
-    <sheet name="solve_sequence" sheetId="11" r:id="rId1"/>
-    <sheet name="solve" sheetId="12" r:id="rId2"/>
-    <sheet name="solve_period" sheetId="13" r:id="rId3"/>
-    <sheet name="timeblocks" sheetId="14" r:id="rId4"/>
-    <sheet name="timeline_t" sheetId="15" r:id="rId5"/>
-    <sheet name="timeline_s" sheetId="17" r:id="rId6"/>
-    <sheet name="timeblocks_timeline" sheetId="16" r:id="rId7"/>
-    <sheet name="node_c" sheetId="7" r:id="rId8"/>
-    <sheet name="node_p" sheetId="19" r:id="rId9"/>
-    <sheet name="node_t" sheetId="47" r:id="rId10"/>
-    <sheet name="commodity_c" sheetId="1" r:id="rId11"/>
-    <sheet name="commodity_p" sheetId="45" r:id="rId12"/>
-    <sheet name="commodity_node" sheetId="23" r:id="rId13"/>
-    <sheet name="connection_c" sheetId="2" r:id="rId14"/>
-    <sheet name="connection_p" sheetId="42" r:id="rId15"/>
-    <sheet name="connection_t" sheetId="43" r:id="rId16"/>
-    <sheet name="connection_node_node" sheetId="25" r:id="rId17"/>
-    <sheet name="profile_t" sheetId="10" r:id="rId18"/>
-    <sheet name="unit_c" sheetId="18" r:id="rId19"/>
-    <sheet name="unit_p" sheetId="21" r:id="rId20"/>
-    <sheet name="unit_t" sheetId="48" r:id="rId21"/>
-    <sheet name="unit_profile_c" sheetId="41" r:id="rId22"/>
-    <sheet name="unit_node_c" sheetId="38" r:id="rId23"/>
-    <sheet name="unit_node_t" sheetId="49" r:id="rId24"/>
-    <sheet name="constraint_sense_c" sheetId="44" r:id="rId25"/>
-    <sheet name="unit_node_constraint_c" sheetId="40" r:id="rId26"/>
-    <sheet name="group_c" sheetId="6" r:id="rId27"/>
-    <sheet name="group_p" sheetId="46" r:id="rId28"/>
-    <sheet name="group_connection" sheetId="26" r:id="rId29"/>
-    <sheet name="group_connection_node" sheetId="28" r:id="rId30"/>
-    <sheet name="group_node" sheetId="27" r:id="rId31"/>
-    <sheet name="group_unit" sheetId="29" r:id="rId32"/>
-    <sheet name="group_unit_node" sheetId="30" r:id="rId33"/>
-    <sheet name="reserve_connection_node_c" sheetId="31" r:id="rId34"/>
-    <sheet name="reserve_group_c" sheetId="32" r:id="rId35"/>
-    <sheet name="reserve_group_t" sheetId="50" r:id="rId36"/>
-    <sheet name="reserve_unit_node_c" sheetId="33" r:id="rId37"/>
+    <sheet name="version" sheetId="51" r:id="rId1"/>
+    <sheet name="solve_sequence" sheetId="11" r:id="rId2"/>
+    <sheet name="solve" sheetId="12" r:id="rId3"/>
+    <sheet name="solve_period" sheetId="13" r:id="rId4"/>
+    <sheet name="timeblocks" sheetId="14" r:id="rId5"/>
+    <sheet name="timeline_t" sheetId="15" r:id="rId6"/>
+    <sheet name="timeline_s" sheetId="17" r:id="rId7"/>
+    <sheet name="timeblocks_timeline" sheetId="16" r:id="rId8"/>
+    <sheet name="node_c" sheetId="7" r:id="rId9"/>
+    <sheet name="node_p" sheetId="19" r:id="rId10"/>
+    <sheet name="node_t" sheetId="47" r:id="rId11"/>
+    <sheet name="commodity_c" sheetId="1" r:id="rId12"/>
+    <sheet name="commodity_p" sheetId="45" r:id="rId13"/>
+    <sheet name="commodity_node" sheetId="23" r:id="rId14"/>
+    <sheet name="connection_c" sheetId="2" r:id="rId15"/>
+    <sheet name="connection_p" sheetId="42" r:id="rId16"/>
+    <sheet name="connection_t" sheetId="43" r:id="rId17"/>
+    <sheet name="connection_node_node" sheetId="25" r:id="rId18"/>
+    <sheet name="profile_t" sheetId="10" r:id="rId19"/>
+    <sheet name="unit_c" sheetId="18" r:id="rId20"/>
+    <sheet name="unit_p" sheetId="21" r:id="rId21"/>
+    <sheet name="unit_t" sheetId="48" r:id="rId22"/>
+    <sheet name="unit_profile_c" sheetId="41" r:id="rId23"/>
+    <sheet name="unit_node_c" sheetId="38" r:id="rId24"/>
+    <sheet name="unit_node_t" sheetId="49" r:id="rId25"/>
+    <sheet name="constraint_sense_c" sheetId="44" r:id="rId26"/>
+    <sheet name="unit_node_constraint_c" sheetId="40" r:id="rId27"/>
+    <sheet name="group_c" sheetId="6" r:id="rId28"/>
+    <sheet name="group_p" sheetId="46" r:id="rId29"/>
+    <sheet name="group_connection" sheetId="26" r:id="rId30"/>
+    <sheet name="group_connection_node" sheetId="28" r:id="rId31"/>
+    <sheet name="group_node" sheetId="27" r:id="rId32"/>
+    <sheet name="group_unit" sheetId="29" r:id="rId33"/>
+    <sheet name="group_unit_node" sheetId="30" r:id="rId34"/>
+    <sheet name="reserve_connection_node_c" sheetId="31" r:id="rId35"/>
+    <sheet name="reserve_group_c" sheetId="32" r:id="rId36"/>
+    <sheet name="reserve_group_t" sheetId="50" r:id="rId37"/>
+    <sheet name="reserve_unit_node_c" sheetId="33" r:id="rId38"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -198,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="249">
   <si>
     <t>commodity</t>
   </si>
@@ -500,9 +501,6 @@
     <t>timestep</t>
   </si>
   <si>
-    <t>duration</t>
-  </si>
-  <si>
     <t>t0003</t>
   </si>
   <si>
@@ -659,9 +657,6 @@
     <t>[MWs/MW] Inertia constant for a synchronously connected unit. Constant.</t>
   </si>
   <si>
-    <t>[hours] Constant.</t>
-  </si>
-  <si>
     <t>[€/MW] Cost of ramping the unit. Constant or period.</t>
   </si>
   <si>
@@ -912,6 +907,45 @@
   </si>
   <si>
     <t>A choice of solve mode (invest, dispatch_single, dispatch_rolling)</t>
+  </si>
+  <si>
+    <t>Version number</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Juha Kiviluoma</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>First working set for the data template</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>time_steps</t>
+  </si>
+  <si>
+    <t>Version numbering: When the number before the dot changes, then the old template will not work with the latest FlexTool. When the latter number changes, then there are only data changes that don't break the functioning.</t>
+  </si>
+  <si>
+    <t>[hours] When unit turns off, how many hours it must stay turned off. Constant.</t>
+  </si>
+  <si>
+    <t>[hours] When unit turns on, how many hours it must stay turned on. Constant.</t>
+  </si>
+  <si>
+    <t>Sheet timeline_t: parameter name duration to time_steps (works better in the database). Improved description of unit/min_downtime and unit/min_uptime.</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1091,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1091,6 +1125,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1410,78 +1445,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9640D032-37A5-47CC-8407-C4F7168BB93B}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="15" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>201</v>
+      <c r="B4" s="25">
+        <v>44594</v>
       </c>
       <c r="C4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>240</v>
+      </c>
+      <c r="D4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5" s="25">
+        <v>44595</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>240</v>
+      </c>
+      <c r="D5" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -1490,6 +1511,141 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51F2ED7-E82A-4D3D-A4CE-E6A52C2211BA}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3">
+        <v>500</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4">
+        <v>550</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56195B5-58E5-4A49-9514-C11CC17CB482}">
   <dimension ref="A1:K27"/>
   <sheetViews>
@@ -1497,7 +1653,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,7 +1679,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>71</v>
@@ -1540,10 +1696,10 @@
         <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1571,7 +1727,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>-30</v>
@@ -1582,7 +1738,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7">
         <v>-40</v>
@@ -1593,7 +1749,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8">
         <v>-50</v>
@@ -1604,7 +1760,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9">
         <v>-60</v>
@@ -1615,7 +1771,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10">
         <v>-70</v>
@@ -1626,7 +1782,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11">
         <v>-80</v>
@@ -1637,7 +1793,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12">
         <v>-90</v>
@@ -1648,7 +1804,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13">
         <v>-100</v>
@@ -1659,7 +1815,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14">
         <v>-110</v>
@@ -1670,7 +1826,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15">
         <v>-120</v>
@@ -1681,7 +1837,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16">
         <v>-130</v>
@@ -1692,7 +1848,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17">
         <v>-140</v>
@@ -1703,7 +1859,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C18">
         <v>-150</v>
@@ -1714,7 +1870,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C19">
         <v>-160</v>
@@ -1725,7 +1881,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20">
         <v>-170</v>
@@ -1736,7 +1892,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C21">
         <v>-180</v>
@@ -1747,7 +1903,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C22">
         <v>-190</v>
@@ -1758,7 +1914,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C23">
         <v>-200</v>
@@ -1769,7 +1925,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C24">
         <v>-210</v>
@@ -1780,7 +1936,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25">
         <v>-220</v>
@@ -1791,7 +1947,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C26">
         <v>-230</v>
@@ -1802,7 +1958,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C27">
         <v>-240</v>
@@ -1818,7 +1974,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99DA432-9F88-4927-B437-CA09DA61AB93}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1843,7 +1999,7 @@
         <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1857,7 +2013,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1865,7 +2021,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C3">
         <v>0.34</v>
@@ -1879,7 +2035,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C4">
         <v>0.2</v>
@@ -1890,7 +2046,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E20CFBA-1F92-463C-919B-31F910121997}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1913,7 +2069,7 @@
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1927,7 +2083,7 @@
         <v>39</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1935,7 +2091,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>94</v>
@@ -1949,7 +2105,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>95</v>
@@ -1963,7 +2119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EFF0A7-3963-4998-9482-2033971B0C97}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -1998,18 +2154,18 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2017,7 +2173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D44D2B2-1DE7-400D-8C40-2CD59BEE6EC3}">
   <dimension ref="A1:P3"/>
   <sheetViews>
@@ -2050,19 +2206,19 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F1" t="s">
         <v>222</v>
       </c>
-      <c r="D1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E1" t="s">
-        <v>232</v>
-      </c>
-      <c r="F1" t="s">
-        <v>224</v>
-      </c>
       <c r="G1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H1" t="s">
         <v>22</v>
@@ -2150,13 +2306,13 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H3">
         <v>100</v>
@@ -2179,7 +2335,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C5CDA4-FFE3-4938-9213-CC2F8772241C}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -2210,7 +2366,7 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E1" t="s">
         <v>26</v>
@@ -2302,7 +2458,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F877950-BDFF-4B0B-89C1-36AC76A9D30A}">
   <dimension ref="A1:K27"/>
   <sheetViews>
@@ -2333,7 +2489,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
@@ -2369,7 +2525,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>0.99</v>
@@ -2377,7 +2533,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7">
         <v>0.99</v>
@@ -2385,7 +2541,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8">
         <v>0.99</v>
@@ -2393,7 +2549,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9">
         <v>0.99</v>
@@ -2401,7 +2557,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10">
         <v>0.99</v>
@@ -2409,7 +2565,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11">
         <v>0.99</v>
@@ -2417,7 +2573,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12">
         <v>0.99</v>
@@ -2425,7 +2581,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13">
         <v>0.99</v>
@@ -2433,7 +2589,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14">
         <v>0.99</v>
@@ -2441,7 +2597,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15">
         <v>0.99</v>
@@ -2449,7 +2605,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16">
         <v>0.99</v>
@@ -2457,7 +2613,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17">
         <v>0.99</v>
@@ -2465,7 +2621,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C18">
         <v>0.99</v>
@@ -2473,7 +2629,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C19">
         <v>0.99</v>
@@ -2481,7 +2637,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20">
         <v>0.99</v>
@@ -2489,7 +2645,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C21">
         <v>0.99</v>
@@ -2497,7 +2653,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C22">
         <v>0.99</v>
@@ -2505,7 +2661,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C23">
         <v>0.99</v>
@@ -2513,7 +2669,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C24">
         <v>0.99</v>
@@ -2521,7 +2677,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25">
         <v>0.99</v>
@@ -2529,7 +2685,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C26">
         <v>0.99</v>
@@ -2537,7 +2693,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C27">
         <v>0.99</v>
@@ -2550,7 +2706,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22779BFC-2A05-4741-ADBE-AFE66F77AC46}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -2592,10 +2748,10 @@
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2603,7 +2759,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE19B28-F2BE-409F-B1A6-1F5F2146177E}">
   <dimension ref="A1:C26"/>
   <sheetViews>
@@ -2611,7 +2767,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2622,7 +2778,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -2636,10 +2792,10 @@
         <v>34</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2660,7 +2816,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5">
         <v>0.7</v>
@@ -2668,7 +2824,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6">
         <v>0.9</v>
@@ -2676,7 +2832,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7">
         <v>0.5</v>
@@ -2684,7 +2840,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8">
         <v>0.4</v>
@@ -2692,7 +2848,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9">
         <v>0.3</v>
@@ -2700,7 +2856,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10">
         <v>0.2</v>
@@ -2708,7 +2864,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11">
         <v>0.1</v>
@@ -2716,7 +2872,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12">
         <v>0.25</v>
@@ -2724,7 +2880,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C13">
         <v>0.25</v>
@@ -2732,7 +2888,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C14">
         <v>0.25</v>
@@ -2740,7 +2896,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C15">
         <v>0.25</v>
@@ -2748,7 +2904,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C16">
         <v>0.25</v>
@@ -2756,7 +2912,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C17">
         <v>0.25</v>
@@ -2764,7 +2920,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C18">
         <v>0.25</v>
@@ -2772,7 +2928,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19">
         <v>0.25</v>
@@ -2780,7 +2936,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C20">
         <v>0.25</v>
@@ -2788,7 +2944,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C21">
         <v>0.25</v>
@@ -2796,7 +2952,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C22">
         <v>0.25</v>
@@ -2804,7 +2960,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C23">
         <v>0.25</v>
@@ -2812,7 +2968,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C24">
         <v>0.25</v>
@@ -2820,7 +2976,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C25">
         <v>0.25</v>
@@ -2828,7 +2984,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C26">
         <v>0.25</v>
@@ -2839,7 +2995,87 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9640D032-37A5-47CC-8407-C4F7168BB93B}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="15" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6619729E-584E-41E3-B72E-7B2979330C88}">
   <dimension ref="A1:W5"/>
   <sheetViews>
@@ -2847,7 +3083,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2880,16 +3116,16 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G1" t="s">
         <v>22</v>
@@ -2901,7 +3137,7 @@
         <v>31</v>
       </c>
       <c r="J1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K1" t="s">
         <v>24</v>
@@ -2913,34 +3149,34 @@
         <v>23</v>
       </c>
       <c r="N1" t="s">
+        <v>145</v>
+      </c>
+      <c r="O1" t="s">
+        <v>208</v>
+      </c>
+      <c r="P1" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S1" t="s">
+        <v>246</v>
+      </c>
+      <c r="T1" t="s">
+        <v>247</v>
+      </c>
+      <c r="U1" t="s">
+        <v>151</v>
+      </c>
+      <c r="V1" t="s">
+        <v>127</v>
+      </c>
+      <c r="W1" t="s">
         <v>146</v>
-      </c>
-      <c r="O1" t="s">
-        <v>210</v>
-      </c>
-      <c r="P1" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>132</v>
-      </c>
-      <c r="R1" t="s">
-        <v>136</v>
-      </c>
-      <c r="S1" t="s">
-        <v>153</v>
-      </c>
-      <c r="T1" t="s">
-        <v>153</v>
-      </c>
-      <c r="U1" t="s">
-        <v>152</v>
-      </c>
-      <c r="V1" t="s">
-        <v>128</v>
-      </c>
-      <c r="W1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2948,16 +3184,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F2" s="24" t="s">
         <v>12</v>
@@ -2993,22 +3229,22 @@
         <v>3</v>
       </c>
       <c r="Q2" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R2" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S2" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T2" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="U2" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V2" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W2" s="24" t="s">
         <v>75</v>
@@ -3019,16 +3255,16 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -3055,16 +3291,16 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -3078,16 +3314,16 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G5">
         <v>50</v>
@@ -3101,107 +3337,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE8329C-91C4-4EB7-BC1D-5B4592D8DD79}">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="14" width="11.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F519FEB-FCA9-4C11-88F7-D4EA23EF6482}">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -3245,7 +3381,7 @@
         <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I1" t="s">
         <v>24</v>
@@ -3257,7 +3393,7 @@
         <v>23</v>
       </c>
       <c r="L1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3265,7 +3401,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>39</v>
@@ -3303,7 +3439,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>94</v>
@@ -3317,7 +3453,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>95</v>
@@ -3331,7 +3467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A4A219-02B1-4261-8559-589A0949A31B}">
   <dimension ref="A1:K27"/>
   <sheetViews>
@@ -3362,7 +3498,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>20</v>
@@ -3373,10 +3509,10 @@
         <v>34</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3398,7 +3534,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -3406,7 +3542,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -3414,7 +3550,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -3422,7 +3558,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -3430,7 +3566,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -3438,7 +3574,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -3446,7 +3582,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -3454,7 +3590,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -3462,7 +3598,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -3470,7 +3606,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -3478,7 +3614,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -3486,7 +3622,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -3494,7 +3630,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C18">
         <v>5</v>
@@ -3502,7 +3638,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -3510,7 +3646,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -3518,7 +3654,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -3526,7 +3662,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -3534,7 +3670,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -3542,7 +3678,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -3550,7 +3686,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25">
         <v>5</v>
@@ -3558,7 +3694,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C26">
         <v>5</v>
@@ -3566,7 +3702,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -3579,7 +3715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1EE4BC-08B3-4CC5-9A8F-D2957036E873}">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -3604,7 +3740,7 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3612,13 +3748,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -3632,13 +3768,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3646,7 +3782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C13F0C3-2BD2-4859-9713-8823A445C2E8}">
   <dimension ref="A1:O7"/>
   <sheetViews>
@@ -3679,22 +3815,22 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" t="s">
         <v>177</v>
       </c>
-      <c r="F1" t="s">
-        <v>179</v>
-      </c>
       <c r="G1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -3705,31 +3841,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -3740,19 +3876,19 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -3763,13 +3899,13 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -3780,13 +3916,13 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -3797,13 +3933,13 @@
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -3814,13 +3950,13 @@
         <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -3831,7 +3967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54CEF76-2D28-40D4-A5BB-1AAB8A75E52F}">
   <dimension ref="A1:K29"/>
   <sheetViews>
@@ -3862,7 +3998,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>20</v>
@@ -3871,10 +4007,10 @@
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -3883,7 +4019,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -3891,10 +4027,10 @@
         <v>34</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3916,7 +4052,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -3924,7 +4060,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -3932,7 +4068,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -3940,7 +4076,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -3948,7 +4084,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -3956,7 +4092,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -3964,7 +4100,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -3972,7 +4108,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -3980,7 +4116,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -3988,7 +4124,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -3996,7 +4132,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C18">
         <v>5</v>
@@ -4004,7 +4140,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -4012,7 +4148,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -4020,7 +4156,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -4028,7 +4164,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -4036,7 +4172,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -4044,7 +4180,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -4052,7 +4188,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C25">
         <v>5</v>
@@ -4060,7 +4196,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26">
         <v>5</v>
@@ -4068,7 +4204,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -4076,7 +4212,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C28">
         <v>5</v>
@@ -4084,7 +4220,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C29">
         <v>5</v>
@@ -4097,7 +4233,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C017E3-B844-46CF-8B82-D76F5D9D7ACD}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -4121,7 +4257,7 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -4135,13 +4271,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -4155,10 +4291,10 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -4169,7 +4305,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA1124C-4BD2-46D2-BD33-99ED754CAC73}">
   <dimension ref="A1:M4"/>
   <sheetViews>
@@ -4198,7 +4334,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -4212,19 +4348,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -4238,16 +4374,16 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -4258,16 +4394,16 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F4">
         <v>-0.1</v>
@@ -4278,7 +4414,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -4388,7 +4524,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -4399,7 +4535,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA54FD9A-FB2F-4111-AC75-F20843B34F53}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -4480,7 +4616,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>94</v>
@@ -4494,7 +4630,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>95</v>
@@ -4508,7 +4644,107 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE8329C-91C4-4EB7-BC1D-5B4592D8DD79}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="14" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B745B3BE-1539-44A7-9F68-00D8AEBADA46}">
   <dimension ref="A1:K1"/>
   <sheetViews>
@@ -4546,129 +4782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23963C17-7280-4F39-8524-0DD641A631A4}">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="14" width="11.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" t="s">
-        <v>205</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" t="s">
-        <v>205</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" t="s">
-        <v>204</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C65105-DA47-40FD-BED9-039766CD67C2}">
   <dimension ref="A1:L1"/>
   <sheetViews>
@@ -4710,7 +4824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6F0B0-C8D9-4343-9EA4-859E87C9AF78}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -4745,18 +4859,18 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4764,7 +4878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5455887B-7914-47A3-A368-88187BB1082B}">
   <dimension ref="A1:K1"/>
   <sheetViews>
@@ -4785,7 +4899,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -4802,7 +4916,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8ED891B-8A85-405F-972C-9B1BFE92F9B9}">
   <dimension ref="A1:L1"/>
   <sheetViews>
@@ -4824,7 +4938,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>66</v>
@@ -4844,7 +4958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB87FF22-BB83-4D5E-B38D-455D581CF757}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -4875,19 +4989,19 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J1" t="s">
         <v>164</v>
-      </c>
-      <c r="J1" t="s">
-        <v>166</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -4901,10 +5015,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>33</v>
@@ -4913,19 +5027,19 @@
         <v>66</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G2" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>162</v>
-      </c>
       <c r="I2" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>163</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -4939,7 +5053,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{866244AD-1571-447F-BAEE-EFE2B5B3F812}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -4969,13 +5083,13 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -4989,22 +5103,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>65</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -5018,7 +5132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E57CD72E-4345-442F-8DFC-A799FEED107D}">
   <dimension ref="A1:K29"/>
   <sheetViews>
@@ -5046,13 +5160,13 @@
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -5066,7 +5180,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -5082,114 +5196,114 @@
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="17"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -5199,7 +5313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8C0D5E-7DB2-4BCF-8A8C-24C978AAECC4}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -5231,19 +5345,19 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J1" t="s">
         <v>164</v>
-      </c>
-      <c r="J1" t="s">
-        <v>166</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -5257,31 +5371,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G2" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>162</v>
-      </c>
       <c r="I2" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>163</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -5296,6 +5410,128 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23963C17-7280-4F39-8524-0DD641A631A4}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="14" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC750BDA-1B66-4AC2-A2C1-8E80C5AE8DE0}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -5328,7 +5564,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>99</v>
@@ -5342,7 +5578,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>36</v>
@@ -5356,7 +5592,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>36</v>
@@ -5370,7 +5606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C14DBC-6D65-48AD-9110-D1593FB205E8}">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -5378,7 +5614,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5395,7 +5631,7 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5403,13 +5639,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>99</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>100</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5417,7 +5653,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>36</v>
@@ -5431,7 +5667,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>37</v>
@@ -5445,10 +5681,10 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -5459,10 +5695,10 @@
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -5473,10 +5709,10 @@
         <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -5487,10 +5723,10 @@
         <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -5501,10 +5737,10 @@
         <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -5515,10 +5751,10 @@
         <v>35</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -5529,10 +5765,10 @@
         <v>35</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -5543,10 +5779,10 @@
         <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -5557,10 +5793,10 @@
         <v>35</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -5571,10 +5807,10 @@
         <v>35</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -5585,10 +5821,10 @@
         <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -5599,10 +5835,10 @@
         <v>35</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -5613,10 +5849,10 @@
         <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -5627,10 +5863,10 @@
         <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -5641,10 +5877,10 @@
         <v>35</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -5655,10 +5891,10 @@
         <v>35</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -5669,10 +5905,10 @@
         <v>35</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -5683,10 +5919,10 @@
         <v>35</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -5697,10 +5933,10 @@
         <v>35</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -5711,10 +5947,10 @@
         <v>35</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -5725,10 +5961,10 @@
         <v>35</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -5739,10 +5975,10 @@
         <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -5753,7 +5989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD7B3D9-76DA-4A96-8BE2-2966A08AF799}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -5776,7 +6012,7 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5784,10 +6020,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5795,7 +6031,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C3">
         <f>24/8760</f>
@@ -5807,7 +6043,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D727460B-F1B2-42C2-90E2-38E181F7AFC8}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -5825,26 +6061,26 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -5852,7 +6088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:S6"/>
   <sheetViews>
@@ -5860,7 +6096,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5890,28 +6126,28 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1" t="s">
         <v>225</v>
       </c>
-      <c r="D1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" t="s">
-        <v>227</v>
-      </c>
       <c r="F1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I1" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1" t="s">
         <v>150</v>
-      </c>
-      <c r="J1" t="s">
-        <v>151</v>
       </c>
       <c r="K1" t="s">
         <v>77</v>
@@ -6005,17 +6241,17 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I3">
         <v>10000</v>
@@ -6029,17 +6265,17 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I4">
         <v>10000</v>
@@ -6053,10 +6289,10 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I5">
         <v>10000</v>
@@ -6070,151 +6306,16 @@
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I6">
         <v>10000</v>
       </c>
       <c r="J6">
         <v>10000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51F2ED7-E82A-4D3D-A4CE-E6A52C2211BA}">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I3">
-        <v>500</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="I4">
-        <v>550</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some changes to input file Excel and model structure.
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,49 +8,48 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC17BD83-42F1-4100-875F-02300997AC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60526844-3275-4971-BBEC-563391FD9B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5145" windowWidth="29040" windowHeight="16440" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="1575" yWindow="885" windowWidth="28800" windowHeight="15600" tabRatio="1000" activeTab="4" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="version" sheetId="51" r:id="rId1"/>
-    <sheet name="solve_sequence" sheetId="11" r:id="rId2"/>
-    <sheet name="solve" sheetId="12" r:id="rId3"/>
-    <sheet name="solve_period" sheetId="13" r:id="rId4"/>
-    <sheet name="timeblocks" sheetId="14" r:id="rId5"/>
-    <sheet name="timeline_t" sheetId="15" r:id="rId6"/>
-    <sheet name="timeline_s" sheetId="17" r:id="rId7"/>
-    <sheet name="timeblocks_timeline" sheetId="16" r:id="rId8"/>
-    <sheet name="node_c" sheetId="7" r:id="rId9"/>
-    <sheet name="node_p" sheetId="19" r:id="rId10"/>
-    <sheet name="node_t" sheetId="47" r:id="rId11"/>
-    <sheet name="commodity_c" sheetId="1" r:id="rId12"/>
-    <sheet name="commodity_p" sheetId="45" r:id="rId13"/>
-    <sheet name="commodity_node" sheetId="23" r:id="rId14"/>
-    <sheet name="connection_c" sheetId="2" r:id="rId15"/>
-    <sheet name="connection_p" sheetId="42" r:id="rId16"/>
-    <sheet name="connection_t" sheetId="43" r:id="rId17"/>
-    <sheet name="connection_node_node" sheetId="25" r:id="rId18"/>
-    <sheet name="profile_t" sheetId="10" r:id="rId19"/>
-    <sheet name="unit_c" sheetId="18" r:id="rId20"/>
-    <sheet name="unit_p" sheetId="21" r:id="rId21"/>
-    <sheet name="unit_t" sheetId="48" r:id="rId22"/>
-    <sheet name="unit_profile_c" sheetId="41" r:id="rId23"/>
-    <sheet name="unit_node_c" sheetId="38" r:id="rId24"/>
-    <sheet name="unit_node_t" sheetId="49" r:id="rId25"/>
-    <sheet name="constraint_sense_c" sheetId="44" r:id="rId26"/>
-    <sheet name="unit_node_constraint_c" sheetId="40" r:id="rId27"/>
-    <sheet name="group_c" sheetId="6" r:id="rId28"/>
-    <sheet name="group_p" sheetId="46" r:id="rId29"/>
-    <sheet name="group_connection" sheetId="26" r:id="rId30"/>
-    <sheet name="group_connection_node" sheetId="28" r:id="rId31"/>
-    <sheet name="group_node" sheetId="27" r:id="rId32"/>
-    <sheet name="group_unit" sheetId="29" r:id="rId33"/>
-    <sheet name="group_unit_node" sheetId="30" r:id="rId34"/>
-    <sheet name="reserve_connection_node_c" sheetId="31" r:id="rId35"/>
-    <sheet name="reserve_group_c" sheetId="32" r:id="rId36"/>
-    <sheet name="reserve_group_t" sheetId="50" r:id="rId37"/>
-    <sheet name="reserve_unit_node_c" sheetId="33" r:id="rId38"/>
+    <sheet name="solve_period" sheetId="53" r:id="rId2"/>
+    <sheet name="solve_sequence" sheetId="11" r:id="rId3"/>
+    <sheet name="timeblockSet" sheetId="14" r:id="rId4"/>
+    <sheet name="timeline_t" sheetId="15" r:id="rId5"/>
+    <sheet name="timeline_s" sheetId="17" r:id="rId6"/>
+    <sheet name="timeblockSet_timeline" sheetId="16" r:id="rId7"/>
+    <sheet name="node_c" sheetId="7" r:id="rId8"/>
+    <sheet name="node_p" sheetId="19" r:id="rId9"/>
+    <sheet name="node_t" sheetId="47" r:id="rId10"/>
+    <sheet name="commodity_c" sheetId="1" r:id="rId11"/>
+    <sheet name="commodity_p" sheetId="45" r:id="rId12"/>
+    <sheet name="commodity_node" sheetId="23" r:id="rId13"/>
+    <sheet name="connection_c" sheetId="2" r:id="rId14"/>
+    <sheet name="connection_p" sheetId="42" r:id="rId15"/>
+    <sheet name="connection_t" sheetId="43" r:id="rId16"/>
+    <sheet name="connection_node_node" sheetId="25" r:id="rId17"/>
+    <sheet name="profile_t" sheetId="10" r:id="rId18"/>
+    <sheet name="unit_c" sheetId="18" r:id="rId19"/>
+    <sheet name="unit_p" sheetId="21" r:id="rId20"/>
+    <sheet name="unit_t" sheetId="48" r:id="rId21"/>
+    <sheet name="unit_profile_c" sheetId="41" r:id="rId22"/>
+    <sheet name="unit_node_c" sheetId="38" r:id="rId23"/>
+    <sheet name="unit_node_t" sheetId="49" r:id="rId24"/>
+    <sheet name="constraint_sense_c" sheetId="44" r:id="rId25"/>
+    <sheet name="unit_node_constraint_c" sheetId="40" r:id="rId26"/>
+    <sheet name="group_c" sheetId="6" r:id="rId27"/>
+    <sheet name="group_p" sheetId="46" r:id="rId28"/>
+    <sheet name="group_connection" sheetId="26" r:id="rId29"/>
+    <sheet name="group_connection_node" sheetId="28" r:id="rId30"/>
+    <sheet name="group_node" sheetId="27" r:id="rId31"/>
+    <sheet name="group_unit" sheetId="29" r:id="rId32"/>
+    <sheet name="group_unit_node" sheetId="30" r:id="rId33"/>
+    <sheet name="reserve_connection_node_c" sheetId="31" r:id="rId34"/>
+    <sheet name="reserve_group_c" sheetId="32" r:id="rId35"/>
+    <sheet name="reserve_group_t" sheetId="50" r:id="rId36"/>
+    <sheet name="reserve_unit_node_c" sheetId="33" r:id="rId37"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -199,7 +198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="257">
   <si>
     <t>commodity</t>
   </si>
@@ -468,12 +467,6 @@
     <t>[CO2 ton per MWh] Constant.</t>
   </si>
   <si>
-    <t>invest_periods</t>
-  </si>
-  <si>
-    <t>realized_periods</t>
-  </si>
-  <si>
     <t>Array of periods where investments are allowed.</t>
   </si>
   <si>
@@ -492,9 +485,6 @@
     <t>invest</t>
   </si>
   <si>
-    <t>block_durations</t>
-  </si>
-  <si>
     <t>Map of block durations. Index: timestep name where the block starts, value: block duration in time steps.</t>
   </si>
   <si>
@@ -780,9 +770,6 @@
     <t>Constraints and the sense of the constraint (greater_than, equal, less_than) as well as a constant factor for the constraint equation.</t>
   </si>
   <si>
-    <t>timeblocks</t>
-  </si>
-  <si>
     <t>discount_years</t>
   </si>
   <si>
@@ -816,9 +803,6 @@
     <t>solve_mode</t>
   </si>
   <si>
-    <t>period_timeblocks_in_solve</t>
-  </si>
-  <si>
     <t>dispatch_single</t>
   </si>
   <si>
@@ -933,9 +917,6 @@
     <t>2.0</t>
   </si>
   <si>
-    <t>time_steps</t>
-  </si>
-  <si>
     <t>Version numbering: When the number before the dot changes, then the old template will not work with the latest FlexTool. When the latter number changes, then there are only data changes that don't break the functioning.</t>
   </si>
   <si>
@@ -946,6 +927,48 @@
   </si>
   <si>
     <t>Sheet timeline_t: parameter name duration to time_steps (works better in the database). Improved description of unit/min_downtime and unit/min_uptime.</t>
+  </si>
+  <si>
+    <t>y2025_dispatch</t>
+  </si>
+  <si>
+    <t>y2000_12h</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>p2030</t>
+  </si>
+  <si>
+    <t>Added y2025_dispatch to solve_sequence, solve and solve_period. Added y2000_12h to timeline_s. Added year 2030 to y2025 investment solve and data to different parameters for year 2030.</t>
+  </si>
+  <si>
+    <t>is_realized</t>
+  </si>
+  <si>
+    <t>can_invest</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>timeblockSet</t>
+  </si>
+  <si>
+    <t>period_timeblockSet</t>
+  </si>
+  <si>
+    <t>block_duration</t>
+  </si>
+  <si>
+    <t>timesteps</t>
+  </si>
+  <si>
+    <t>timestep_name</t>
+  </si>
+  <si>
+    <t>Combined sheet 'solve' and sheet 'solve_period' into one sheet 'solve_period'. Changed timeblocks to timeblockSet in sheet names and inside sheets. In timeline_t 'time_steps' was changed to 'timesteps'.</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1126,6 +1149,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1147,6 +1171,459 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5153014" cy="1395318"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71E1ADD2-894E-4CC9-8911-C865343C1FFF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7419975" y="676275"/>
+          <a:ext cx="5153014" cy="1395318"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Define periods</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> in </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>each</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> solve</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- One solve can have multiple rows (one row for each period in the solve)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- period_timeblockSet: Choose what timeblockSet the period uses</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- discount_years: How many years from the solve to the period</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- realised_periods: Results are kept only from these</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- invest_periods: Investments are allowed only from these</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- Maintain the order of periods (top to bottom &gt;&gt; first to last in the solve)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5573770" cy="1581459"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A5E5855-F888-4056-977F-0750AE55CB00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3743325" y="590550"/>
+          <a:ext cx="5573770" cy="1581459"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Define the sequence of solves:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- Can just be one solve for a single shot model</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- Solve order is based on top to bottom order</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fi-FI" sz="1200" baseline="0">
+            <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Solve_mode:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- invest mode allows investments for investable units, connections and storages</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- dispatch_single performs a single perfect foresight dispatch solve</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- dispatch_rolling is not funtional yet</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4227055" cy="836896"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E22C936-BB03-4C73-9567-773323C7FAC6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3848100" y="466725"/>
+          <a:ext cx="4227055" cy="836896"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Define the</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> timeblockSets</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- one timeblockSet can have multiple rows (multiple blocks)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- timestep: starting time step for the block</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- block_duration: duration of the block counted in time steps</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5942332" cy="836896"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{186E89B8-8326-47C9-9577-3DCA0AEADD69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3905250" y="495300"/>
+          <a:ext cx="5942332" cy="836896"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Define the</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> timelines the timeblockSets can use</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- There can be multiple timelines</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- timestep_name: name of the time step (this is read as a string - datetime also works)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fi-FI" sz="1200" baseline="0">
+              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>- timesteps: duration of each time step (in hours)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1446,10 +1923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1460,49 +1937,77 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D3" t="s">
         <v>236</v>
-      </c>
-      <c r="B3" t="s">
-        <v>238</v>
-      </c>
-      <c r="C3" t="s">
-        <v>239</v>
-      </c>
-      <c r="D3" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B4" s="25">
         <v>44594</v>
       </c>
       <c r="C4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D4" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B5" s="25">
         <v>44595</v>
       </c>
       <c r="C5" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D5" t="s">
-        <v>248</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B6" s="25">
+        <v>44600</v>
+      </c>
+      <c r="C6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B7" s="25">
+        <v>44602</v>
+      </c>
+      <c r="C7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D7" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -1511,141 +2016,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51F2ED7-E82A-4D3D-A4CE-E6A52C2211BA}">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I3">
-        <v>500</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="I4">
-        <v>550</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56195B5-58E5-4A49-9514-C11CC17CB482}">
   <dimension ref="A1:K27"/>
   <sheetViews>
@@ -1653,7 +2023,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,7 +2049,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>71</v>
@@ -1696,10 +2066,10 @@
         <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1727,7 +2097,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C6">
         <v>-30</v>
@@ -1738,7 +2108,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C7">
         <v>-40</v>
@@ -1749,7 +2119,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C8">
         <v>-50</v>
@@ -1760,7 +2130,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C9">
         <v>-60</v>
@@ -1771,7 +2141,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C10">
         <v>-70</v>
@@ -1782,7 +2152,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C11">
         <v>-80</v>
@@ -1793,7 +2163,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C12">
         <v>-90</v>
@@ -1804,7 +2174,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C13">
         <v>-100</v>
@@ -1815,7 +2185,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C14">
         <v>-110</v>
@@ -1826,7 +2196,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C15">
         <v>-120</v>
@@ -1837,7 +2207,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C16">
         <v>-130</v>
@@ -1848,7 +2218,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C17">
         <v>-140</v>
@@ -1859,7 +2229,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C18">
         <v>-150</v>
@@ -1870,7 +2240,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C19">
         <v>-160</v>
@@ -1881,7 +2251,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C20">
         <v>-170</v>
@@ -1892,7 +2262,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C21">
         <v>-180</v>
@@ -1903,7 +2273,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C22">
         <v>-190</v>
@@ -1914,7 +2284,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C23">
         <v>-200</v>
@@ -1925,7 +2295,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C24">
         <v>-210</v>
@@ -1936,7 +2306,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C25">
         <v>-220</v>
@@ -1947,7 +2317,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C26">
         <v>-230</v>
@@ -1958,7 +2328,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C27">
         <v>-240</v>
@@ -1974,7 +2344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99DA432-9F88-4927-B437-CA09DA61AB93}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1999,7 +2369,7 @@
         <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2013,7 +2383,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2021,7 +2391,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C3">
         <v>0.34</v>
@@ -2035,7 +2405,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C4">
         <v>0.2</v>
@@ -2046,15 +2416,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E20CFBA-1F92-463C-919B-31F910121997}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2069,7 +2439,7 @@
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2083,7 +2453,7 @@
         <v>39</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2091,10 +2461,10 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -2105,13 +2475,27 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D4">
         <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D5">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2119,7 +2503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EFF0A7-3963-4998-9482-2033971B0C97}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -2154,18 +2538,18 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2173,7 +2557,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D44D2B2-1DE7-400D-8C40-2CD59BEE6EC3}">
   <dimension ref="A1:P3"/>
   <sheetViews>
@@ -2206,19 +2590,19 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H1" t="s">
         <v>22</v>
@@ -2306,13 +2690,13 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="H3">
         <v>100</v>
@@ -2335,15 +2719,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C5CDA4-FFE3-4938-9213-CC2F8772241C}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2366,7 +2750,7 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E1" t="s">
         <v>26</v>
@@ -2433,7 +2817,7 @@
         <v>38</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -2447,9 +2831,23 @@
         <v>38</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5">
         <v>150</v>
       </c>
     </row>
@@ -2458,7 +2856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F877950-BDFF-4B0B-89C1-36AC76A9D30A}">
   <dimension ref="A1:K27"/>
   <sheetViews>
@@ -2489,7 +2887,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
@@ -2525,7 +2923,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C6">
         <v>0.99</v>
@@ -2533,7 +2931,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C7">
         <v>0.99</v>
@@ -2541,7 +2939,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C8">
         <v>0.99</v>
@@ -2549,7 +2947,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C9">
         <v>0.99</v>
@@ -2557,7 +2955,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C10">
         <v>0.99</v>
@@ -2565,7 +2963,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C11">
         <v>0.99</v>
@@ -2573,7 +2971,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C12">
         <v>0.99</v>
@@ -2581,7 +2979,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C13">
         <v>0.99</v>
@@ -2589,7 +2987,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C14">
         <v>0.99</v>
@@ -2597,7 +2995,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C15">
         <v>0.99</v>
@@ -2605,7 +3003,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C16">
         <v>0.99</v>
@@ -2613,7 +3011,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C17">
         <v>0.99</v>
@@ -2621,7 +3019,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C18">
         <v>0.99</v>
@@ -2629,7 +3027,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C19">
         <v>0.99</v>
@@ -2637,7 +3035,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C20">
         <v>0.99</v>
@@ -2645,7 +3043,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C21">
         <v>0.99</v>
@@ -2653,7 +3051,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C22">
         <v>0.99</v>
@@ -2661,7 +3059,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C23">
         <v>0.99</v>
@@ -2669,7 +3067,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C24">
         <v>0.99</v>
@@ -2677,7 +3075,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C25">
         <v>0.99</v>
@@ -2685,7 +3083,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C26">
         <v>0.99</v>
@@ -2693,7 +3091,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C27">
         <v>0.99</v>
@@ -2706,7 +3104,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22779BFC-2A05-4741-ADBE-AFE66F77AC46}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -2748,10 +3146,10 @@
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2759,7 +3157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE19B28-F2BE-409F-B1A6-1F5F2146177E}">
   <dimension ref="A1:C26"/>
   <sheetViews>
@@ -2778,7 +3176,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -2792,10 +3190,10 @@
         <v>34</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2816,7 +3214,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C5">
         <v>0.7</v>
@@ -2824,7 +3222,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C6">
         <v>0.9</v>
@@ -2832,7 +3230,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C7">
         <v>0.5</v>
@@ -2840,7 +3238,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C8">
         <v>0.4</v>
@@ -2848,7 +3246,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C9">
         <v>0.3</v>
@@ -2856,7 +3254,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C10">
         <v>0.2</v>
@@ -2864,7 +3262,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C11">
         <v>0.1</v>
@@ -2872,7 +3270,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C12">
         <v>0.25</v>
@@ -2880,7 +3278,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C13">
         <v>0.25</v>
@@ -2888,7 +3286,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C14">
         <v>0.25</v>
@@ -2896,7 +3294,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C15">
         <v>0.25</v>
@@ -2904,7 +3302,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C16">
         <v>0.25</v>
@@ -2912,7 +3310,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C17">
         <v>0.25</v>
@@ -2920,7 +3318,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C18">
         <v>0.25</v>
@@ -2928,7 +3326,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C19">
         <v>0.25</v>
@@ -2936,7 +3334,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C20">
         <v>0.25</v>
@@ -2944,7 +3342,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C21">
         <v>0.25</v>
@@ -2952,7 +3350,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C22">
         <v>0.25</v>
@@ -2960,7 +3358,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C23">
         <v>0.25</v>
@@ -2968,7 +3366,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C24">
         <v>0.25</v>
@@ -2976,7 +3374,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C25">
         <v>0.25</v>
@@ -2984,7 +3382,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C26">
         <v>0.25</v>
@@ -2995,87 +3393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9640D032-37A5-47CC-8407-C4F7168BB93B}">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="15" width="11.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6619729E-584E-41E3-B72E-7B2979330C88}">
   <dimension ref="A1:W5"/>
   <sheetViews>
@@ -3116,16 +3434,16 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="G1" t="s">
         <v>22</v>
@@ -3137,7 +3455,7 @@
         <v>31</v>
       </c>
       <c r="J1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K1" t="s">
         <v>24</v>
@@ -3149,34 +3467,34 @@
         <v>23</v>
       </c>
       <c r="N1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="O1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="P1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Q1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="R1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="S1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="T1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="U1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="V1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="W1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3184,16 +3502,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F2" s="24" t="s">
         <v>12</v>
@@ -3229,22 +3547,22 @@
         <v>3</v>
       </c>
       <c r="Q2" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="S2" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="R2" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="S2" s="24" t="s">
+      <c r="T2" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="T2" s="24" t="s">
-        <v>136</v>
-      </c>
       <c r="U2" s="24" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="V2" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="W2" s="24" t="s">
         <v>75</v>
@@ -3255,16 +3573,16 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -3291,16 +3609,16 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -3314,16 +3632,16 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G5">
         <v>50</v>
@@ -3337,9 +3655,204 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F0779D-09F6-4BFC-A27B-5A43B3911876}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="14" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" t="s">
+        <v>198</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F519FEB-FCA9-4C11-88F7-D4EA23EF6482}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
@@ -3381,7 +3894,7 @@
         <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I1" t="s">
         <v>24</v>
@@ -3393,7 +3906,7 @@
         <v>23</v>
       </c>
       <c r="L1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3401,7 +3914,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>39</v>
@@ -3439,13 +3952,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E3">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3453,13 +3966,27 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E4">
-        <v>100</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -3467,7 +3994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A4A219-02B1-4261-8559-589A0949A31B}">
   <dimension ref="A1:K27"/>
   <sheetViews>
@@ -3498,7 +4025,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>20</v>
@@ -3509,10 +4036,10 @@
         <v>34</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3534,7 +4061,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -3542,7 +4069,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -3550,7 +4077,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -3558,7 +4085,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -3566,7 +4093,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -3574,7 +4101,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -3582,7 +4109,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -3590,7 +4117,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -3598,7 +4125,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -3606,7 +4133,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -3614,7 +4141,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -3622,7 +4149,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -3630,7 +4157,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C18">
         <v>5</v>
@@ -3638,7 +4165,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -3646,7 +4173,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -3654,7 +4181,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -3662,7 +4189,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -3670,7 +4197,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -3678,7 +4205,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -3686,7 +4213,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C25">
         <v>5</v>
@@ -3694,7 +4221,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C26">
         <v>5</v>
@@ -3702,7 +4229,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -3715,7 +4242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1EE4BC-08B3-4CC5-9A8F-D2957036E873}">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -3740,7 +4267,7 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3748,13 +4275,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -3768,13 +4295,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -3782,7 +4309,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C13F0C3-2BD2-4859-9713-8823A445C2E8}">
   <dimension ref="A1:O7"/>
   <sheetViews>
@@ -3815,22 +4342,22 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -3841,31 +4368,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>141</v>
-      </c>
       <c r="J2" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -3876,19 +4403,19 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -3899,13 +4426,13 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -3916,13 +4443,13 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -3933,13 +4460,13 @@
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -3950,13 +4477,13 @@
         <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -3967,7 +4494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54CEF76-2D28-40D4-A5BB-1AAB8A75E52F}">
   <dimension ref="A1:K29"/>
   <sheetViews>
@@ -3975,7 +4502,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3998,7 +4525,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>20</v>
@@ -4007,10 +4534,10 @@
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -4019,7 +4546,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4027,10 +4554,10 @@
         <v>34</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -4052,7 +4579,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -4060,7 +4587,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -4068,7 +4595,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -4076,7 +4603,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -4084,7 +4611,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -4092,7 +4619,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -4100,7 +4627,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -4108,7 +4635,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -4116,7 +4643,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -4124,7 +4651,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -4132,7 +4659,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C18">
         <v>5</v>
@@ -4140,7 +4667,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -4148,7 +4675,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -4156,7 +4683,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -4164,7 +4691,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -4172,7 +4699,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -4180,7 +4707,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -4188,7 +4715,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C25">
         <v>5</v>
@@ -4196,7 +4723,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C26">
         <v>5</v>
@@ -4204,7 +4731,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -4212,7 +4739,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C28">
         <v>5</v>
@@ -4220,7 +4747,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C29">
         <v>5</v>
@@ -4233,7 +4760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C017E3-B844-46CF-8B82-D76F5D9D7ACD}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -4257,7 +4784,7 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -4271,13 +4798,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -4291,10 +4818,10 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -4305,7 +4832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA1124C-4BD2-46D2-BD33-99ED754CAC73}">
   <dimension ref="A1:M4"/>
   <sheetViews>
@@ -4313,7 +4840,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4334,7 +4861,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -4348,19 +4875,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -4374,16 +4901,16 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D3" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>213</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>218</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -4394,16 +4921,16 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F4">
         <v>-0.1</v>
@@ -4414,7 +4941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -4524,7 +5051,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -4535,15 +5062,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA54FD9A-FB2F-4111-AC75-F20843B34F53}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4616,10 +5143,10 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G3">
         <v>20</v>
@@ -4630,12 +5157,26 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G5">
         <v>20</v>
       </c>
     </row>
@@ -4644,107 +5185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE8329C-91C4-4EB7-BC1D-5B4592D8DD79}">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="14" width="11.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B745B3BE-1539-44A7-9F68-00D8AEBADA46}">
   <dimension ref="A1:K1"/>
   <sheetViews>
@@ -4782,7 +5223,97 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9640D032-37A5-47CC-8407-C4F7168BB93B}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="15" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C65105-DA47-40FD-BED9-039766CD67C2}">
   <dimension ref="A1:L1"/>
   <sheetViews>
@@ -4824,7 +5355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6F0B0-C8D9-4343-9EA4-859E87C9AF78}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -4859,18 +5390,18 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -4878,7 +5409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5455887B-7914-47A3-A368-88187BB1082B}">
   <dimension ref="A1:K1"/>
   <sheetViews>
@@ -4899,7 +5430,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -4916,7 +5447,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8ED891B-8A85-405F-972C-9B1BFE92F9B9}">
   <dimension ref="A1:L1"/>
   <sheetViews>
@@ -4938,7 +5469,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>66</v>
@@ -4958,7 +5489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB87FF22-BB83-4D5E-B38D-455D581CF757}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -4989,19 +5520,19 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="G1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" t="s">
         <v>159</v>
       </c>
-      <c r="H1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I1" t="s">
-        <v>162</v>
-      </c>
       <c r="J1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -5015,10 +5546,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>33</v>
@@ -5027,19 +5558,19 @@
         <v>66</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="G2" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -5053,7 +5584,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{866244AD-1571-447F-BAEE-EFE2B5B3F812}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -5083,13 +5614,13 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -5103,22 +5634,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>65</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -5132,7 +5663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E57CD72E-4345-442F-8DFC-A799FEED107D}">
   <dimension ref="A1:K29"/>
   <sheetViews>
@@ -5160,13 +5691,13 @@
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -5180,7 +5711,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -5196,114 +5727,114 @@
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B9" s="17"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -5313,7 +5844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8C0D5E-7DB2-4BCF-8A8C-24C978AAECC4}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -5345,19 +5876,19 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" t="s">
         <v>159</v>
       </c>
-      <c r="H1" t="s">
-        <v>171</v>
-      </c>
-      <c r="I1" t="s">
-        <v>162</v>
-      </c>
       <c r="J1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -5371,31 +5902,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="G2" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -5410,128 +5941,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23963C17-7280-4F39-8524-0DD641A631A4}">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="14" width="11.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" t="s">
-        <v>203</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" t="s">
-        <v>203</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" t="s">
-        <v>203</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" t="s">
-        <v>202</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC750BDA-1B66-4AC2-A2C1-8E80C5AE8DE0}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -5539,13 +5948,13 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="13" width="11.5703125" customWidth="1"/>
@@ -5556,7 +5965,7 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5564,13 +5973,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>193</v>
+        <v>251</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>97</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5578,7 +5987,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>36</v>
@@ -5592,7 +6001,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>36</v>
@@ -5603,25 +6012,26 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C14DBC-6D65-48AD-9110-D1593FB205E8}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="13" width="11.5703125" customWidth="1"/>
   </cols>
@@ -5631,7 +6041,7 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5639,13 +6049,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>99</v>
+        <v>255</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5653,7 +6063,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>36</v>
@@ -5667,7 +6077,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>37</v>
@@ -5681,10 +6091,10 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -5695,10 +6105,10 @@
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -5709,10 +6119,10 @@
         <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -5723,10 +6133,10 @@
         <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -5737,10 +6147,10 @@
         <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -5751,10 +6161,10 @@
         <v>35</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -5765,10 +6175,10 @@
         <v>35</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -5779,10 +6189,10 @@
         <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -5793,10 +6203,10 @@
         <v>35</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -5807,10 +6217,10 @@
         <v>35</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -5821,10 +6231,10 @@
         <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -5835,10 +6245,10 @@
         <v>35</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -5849,10 +6259,10 @@
         <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -5863,10 +6273,10 @@
         <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -5877,10 +6287,10 @@
         <v>35</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -5891,10 +6301,10 @@
         <v>35</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -5905,10 +6315,10 @@
         <v>35</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -5919,10 +6329,10 @@
         <v>35</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -5933,10 +6343,10 @@
         <v>35</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -5947,10 +6357,10 @@
         <v>35</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -5961,10 +6371,10 @@
         <v>35</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -5975,23 +6385,27 @@
         <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="26"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD7B3D9-76DA-4A96-8BE2-2966A08AF799}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -6012,7 +6426,7 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -6020,10 +6434,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -6031,11 +6445,23 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C3">
         <f>24/8760</f>
         <v>2.7397260273972603E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4">
+        <f>12/8760</f>
+        <v>1.3698630136986301E-3</v>
       </c>
     </row>
   </sheetData>
@@ -6043,7 +6469,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D727460B-F1B2-42C2-90E2-38E181F7AFC8}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -6054,33 +6480,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="4" customWidth="1"/>
     <col min="3" max="11" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>193</v>
+        <v>251</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -6088,7 +6514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:S6"/>
   <sheetViews>
@@ -6126,28 +6552,28 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1" t="s">
         <v>225</v>
       </c>
-      <c r="F1" t="s">
-        <v>230</v>
-      </c>
       <c r="G1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="I1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="K1" t="s">
         <v>77</v>
@@ -6241,17 +6667,17 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I3">
         <v>10000</v>
@@ -6265,17 +6691,17 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I4">
         <v>10000</v>
@@ -6289,10 +6715,10 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I5">
         <v>10000</v>
@@ -6306,16 +6732,132 @@
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I6">
         <v>10000</v>
       </c>
       <c r="J6">
         <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51F2ED7-E82A-4D3D-A4CE-E6A52C2211BA}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D3">
+        <f>3000*8760/24*1.1</f>
+        <v>1204500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added inflow_method and made annual_flow scaling to work also on the model side.
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0C5ED5-0048-44B5-9E45-111C2B1D253D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEF3D56-065D-4B80-BDCD-C8277D41C1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" activeTab="1" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="315">
   <si>
     <t>commodity</t>
   </si>
@@ -410,9 +410,6 @@
     <t>has_balance</t>
   </si>
   <si>
-    <t>has_inflow</t>
-  </si>
-  <si>
     <t>has_state</t>
   </si>
   <si>
@@ -854,9 +851,6 @@
     <t>A flag whether the node has a balance constraint. If empty, then not true. Use 'yes' to indicate true.</t>
   </si>
   <si>
-    <t>A flag whether node has inflow. If empty, then not true. Use 'yes' to indicate true.</t>
-  </si>
-  <si>
     <t>A flag whether has a state variable (storage). If empty, then not true. Use 'yes' to indicate true.</t>
   </si>
   <si>
@@ -929,9 +923,6 @@
     <t>y2025_dispatch</t>
   </si>
   <si>
-    <t>y2000_12h</t>
-  </si>
-  <si>
     <t>2.1</t>
   </si>
   <si>
@@ -1131,6 +1122,30 @@
   </si>
   <si>
     <t>- time series (sheets ends with '_t') - These parameters can be defined separately for each timestep. Overrides any constant value. Time series are typically used to give profiles, often based in history (e.g., VRE profile).</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>Removed timeline 'y2000_12h'</t>
+  </si>
+  <si>
+    <t>inflow_method</t>
+  </si>
+  <si>
+    <t>use_original</t>
+  </si>
+  <si>
+    <t>Choice how to treat inflow time series. Empty defaults to 'use_original', which does not scale the time series. 'no_inflow' ignores the inflow time series. 'scale_to_annual_flow' will scale the time series to match the 'annual_flow' when the sum of inflow is multiplied by 8760/'hours_in_solve'.</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>Changed 'has_inflow' in node to 'inflow_method'. This also changes what parameters are allowed in there.</t>
+  </si>
+  <si>
+    <t>scale_to_annual_flow</t>
   </si>
 </sst>
 </file>
@@ -1386,16 +1401,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2746,7 +2761,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A2:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2754,147 +2771,147 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
-        <v>254</v>
-      </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
+      <c r="A2" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
-        <v>255</v>
-      </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
+      <c r="A3" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
       <c r="E3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
-        <v>256</v>
-      </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
+      <c r="A4" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
       <c r="E4" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
-        <v>249</v>
-      </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
+      <c r="A5" s="42" t="s">
+        <v>246</v>
+      </c>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
       <c r="E5" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="29" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
-        <v>258</v>
-      </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
+      <c r="A7" s="42" t="s">
+        <v>255</v>
+      </c>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="27"/>
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
       <c r="E8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C10" s="32"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
-        <v>264</v>
-      </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
+      <c r="A11" s="43" t="s">
+        <v>261</v>
+      </c>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
         <v>265</v>
       </c>
-      <c r="B12" s="31" t="s">
-        <v>266</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
-        <v>268</v>
-      </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="31" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
-        <v>271</v>
-      </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
+      <c r="A16" s="43" t="s">
+        <v>268</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
-        <v>272</v>
-      </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
+      <c r="A17" s="43" t="s">
+        <v>269</v>
+      </c>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="33"/>
@@ -2905,29 +2922,29 @@
       <c r="A19" s="39"/>
       <c r="B19" s="39"/>
       <c r="C19" s="40" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
-        <v>306</v>
-      </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
+      <c r="A20" s="44" t="s">
+        <v>303</v>
+      </c>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
-        <v>305</v>
-      </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
+      <c r="A21" s="44" t="s">
+        <v>302</v>
+      </c>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
-        <v>270</v>
-      </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
+      <c r="A22" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="33"/>
@@ -2936,45 +2953,45 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C24" s="34"/>
       <c r="D24" s="28"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="41"/>
@@ -2985,30 +3002,35 @@
       <c r="C30" s="27"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="42" t="s">
-        <v>278</v>
-      </c>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
+      <c r="A31" s="45" t="s">
+        <v>275</v>
+      </c>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B32" s="36"/>
       <c r="C32" s="35" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="42" t="s">
-        <v>281</v>
-      </c>
-      <c r="B33" s="42"/>
-      <c r="C33" s="42"/>
+      <c r="A33" s="45" t="s">
+        <v>278</v>
+      </c>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A33:C33"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="A2:C2"/>
@@ -3023,11 +3045,6 @@
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A33:C33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A31" location="reserve_unit_node_c!A1" display="reserve_connection_node_c" xr:uid="{3F855114-4A57-4E0A-A766-0317F980F4BF}"/>
@@ -3084,7 +3101,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3105,30 +3122,30 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
         <v>80</v>
       </c>
-      <c r="F1" t="s">
-        <v>81</v>
-      </c>
       <c r="G1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" t="s">
         <v>83</v>
       </c>
-      <c r="H1" t="s">
-        <v>84</v>
-      </c>
       <c r="I1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="K1" t="s">
         <v>24</v>
@@ -3137,7 +3154,7 @@
         <v>28</v>
       </c>
       <c r="M1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3169,7 +3186,7 @@
         <v>8</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>7</v>
@@ -3186,10 +3203,10 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D3">
         <f>3000*8760/24*1.1</f>
@@ -3225,7 +3242,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -3240,13 +3257,13 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3257,10 +3274,10 @@
         <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3288,7 +3305,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6">
         <v>-30</v>
@@ -3299,7 +3316,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7">
         <v>-40</v>
@@ -3310,7 +3327,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8">
         <v>-50</v>
@@ -3321,7 +3338,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9">
         <v>-60</v>
@@ -3332,7 +3349,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10">
         <v>-70</v>
@@ -3343,7 +3360,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11">
         <v>-80</v>
@@ -3354,7 +3371,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12">
         <v>-90</v>
@@ -3365,7 +3382,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C13">
         <v>-100</v>
@@ -3376,7 +3393,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14">
         <v>-110</v>
@@ -3387,7 +3404,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15">
         <v>-120</v>
@@ -3398,7 +3415,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16">
         <v>-130</v>
@@ -3409,7 +3426,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17">
         <v>-140</v>
@@ -3420,7 +3437,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18">
         <v>-150</v>
@@ -3431,7 +3448,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19">
         <v>-160</v>
@@ -3442,7 +3459,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20">
         <v>-170</v>
@@ -3453,7 +3470,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21">
         <v>-180</v>
@@ -3464,7 +3481,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C22">
         <v>-190</v>
@@ -3475,7 +3492,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C23">
         <v>-200</v>
@@ -3486,7 +3503,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C24">
         <v>-210</v>
@@ -3497,7 +3514,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C25">
         <v>-220</v>
@@ -3508,7 +3525,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C26">
         <v>-230</v>
@@ -3519,7 +3536,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27">
         <v>-240</v>
@@ -3558,14 +3575,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1"/>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3579,7 +3596,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3587,7 +3604,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C3">
         <v>0.34</v>
@@ -3601,7 +3618,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C4">
         <v>0.2</v>
@@ -3636,12 +3653,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3655,7 +3672,7 @@
         <v>39</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3663,10 +3680,10 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -3677,10 +3694,10 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4">
         <v>21</v>
@@ -3691,10 +3708,10 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D5">
         <v>22</v>
@@ -3743,18 +3760,18 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -3770,7 +3787,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3793,23 +3810,23 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1" t="s">
         <v>213</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1" t="s">
         <v>214</v>
       </c>
-      <c r="E1" t="s">
-        <v>223</v>
-      </c>
-      <c r="F1" t="s">
-        <v>215</v>
-      </c>
       <c r="G1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H1" t="s">
         <v>22</v>
@@ -3824,7 +3841,7 @@
         <v>42</v>
       </c>
       <c r="L1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="M1" t="s">
         <v>24</v>
@@ -3877,7 +3894,7 @@
         <v>8</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>7</v>
@@ -3903,13 +3920,13 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" t="s">
         <v>203</v>
       </c>
-      <c r="D3" t="s">
-        <v>204</v>
-      </c>
       <c r="E3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H3">
         <v>100</v>
@@ -3965,12 +3982,12 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E1" t="s">
         <v>26</v>
@@ -3985,7 +4002,7 @@
         <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="J1" t="s">
         <v>24</v>
@@ -4023,7 +4040,7 @@
         <v>8</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
@@ -4043,7 +4060,7 @@
         <v>38</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -4057,7 +4074,7 @@
         <v>38</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E4">
         <v>150</v>
@@ -4071,7 +4088,7 @@
         <v>38</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E5">
         <v>150</v>
@@ -4106,7 +4123,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -4118,7 +4135,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
@@ -4154,7 +4171,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6">
         <v>0.99</v>
@@ -4162,7 +4179,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7">
         <v>0.99</v>
@@ -4170,7 +4187,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8">
         <v>0.99</v>
@@ -4178,7 +4195,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9">
         <v>0.99</v>
@@ -4186,7 +4203,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10">
         <v>0.99</v>
@@ -4194,7 +4211,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11">
         <v>0.99</v>
@@ -4202,7 +4219,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12">
         <v>0.99</v>
@@ -4210,7 +4227,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C13">
         <v>0.99</v>
@@ -4218,7 +4235,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14">
         <v>0.99</v>
@@ -4226,7 +4243,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15">
         <v>0.99</v>
@@ -4234,7 +4251,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16">
         <v>0.99</v>
@@ -4242,7 +4259,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17">
         <v>0.99</v>
@@ -4250,7 +4267,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18">
         <v>0.99</v>
@@ -4258,7 +4275,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19">
         <v>0.99</v>
@@ -4266,7 +4283,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20">
         <v>0.99</v>
@@ -4274,7 +4291,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21">
         <v>0.99</v>
@@ -4282,7 +4299,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C22">
         <v>0.99</v>
@@ -4290,7 +4307,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C23">
         <v>0.99</v>
@@ -4298,7 +4315,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C24">
         <v>0.99</v>
@@ -4306,7 +4323,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C25">
         <v>0.99</v>
@@ -4314,7 +4331,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C26">
         <v>0.99</v>
@@ -4322,7 +4339,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27">
         <v>0.99</v>
@@ -4380,10 +4397,10 @@
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>178</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -4430,20 +4447,20 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G1" t="s">
         <v>22</v>
@@ -4455,10 +4472,10 @@
         <v>31</v>
       </c>
       <c r="J1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="L1" t="s">
         <v>24</v>
@@ -4470,31 +4487,31 @@
         <v>23</v>
       </c>
       <c r="O1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P1" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>125</v>
+      </c>
+      <c r="R1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S1" t="s">
+        <v>131</v>
+      </c>
+      <c r="T1" t="s">
+        <v>236</v>
+      </c>
+      <c r="U1" t="s">
+        <v>237</v>
+      </c>
+      <c r="V1" t="s">
+        <v>123</v>
+      </c>
+      <c r="W1" t="s">
         <v>142</v>
-      </c>
-      <c r="P1" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>126</v>
-      </c>
-      <c r="R1" t="s">
-        <v>128</v>
-      </c>
-      <c r="S1" t="s">
-        <v>132</v>
-      </c>
-      <c r="T1" t="s">
-        <v>238</v>
-      </c>
-      <c r="U1" t="s">
-        <v>239</v>
-      </c>
-      <c r="V1" t="s">
-        <v>124</v>
-      </c>
-      <c r="W1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4502,16 +4519,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F2" s="24" t="s">
         <v>12</v>
@@ -4529,7 +4546,7 @@
         <v>8</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="L2" s="24" t="s">
         <v>7</v>
@@ -4550,22 +4567,22 @@
         <v>3</v>
       </c>
       <c r="R2" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S2" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="T2" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="U2" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V2" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="W2" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -4573,16 +4590,16 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -4609,16 +4626,16 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -4632,16 +4649,16 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G5">
         <v>50</v>
@@ -4660,11 +4677,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4674,105 +4689,133 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" t="s">
         <v>229</v>
       </c>
-      <c r="B3" t="s">
-        <v>231</v>
-      </c>
       <c r="C3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" t="s">
         <v>232</v>
-      </c>
-      <c r="D3" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B4" s="25">
         <v>44594</v>
       </c>
       <c r="C4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D4" t="s">
         <v>233</v>
-      </c>
-      <c r="D4" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B5" s="25">
         <v>44595</v>
       </c>
       <c r="C5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B6" s="25">
         <v>44600</v>
       </c>
       <c r="C6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D6" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B7" s="25">
         <v>44602</v>
       </c>
       <c r="C7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D7" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B8" s="25">
         <v>44602</v>
       </c>
       <c r="C8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D8" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B9" s="25">
         <v>44602</v>
       </c>
       <c r="C9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D9" t="s">
-        <v>304</v>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="B10" s="25">
+        <v>44602</v>
+      </c>
+      <c r="C10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D10" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B11" s="25">
+        <v>44603</v>
+      </c>
+      <c r="C11" t="s">
+        <v>231</v>
+      </c>
+      <c r="D11" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -4810,7 +4853,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4827,10 +4870,10 @@
         <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="J1" t="s">
         <v>24</v>
@@ -4842,7 +4885,7 @@
         <v>23</v>
       </c>
       <c r="M1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4850,7 +4893,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>39</v>
@@ -4871,7 +4914,7 @@
         <v>8</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
@@ -4891,10 +4934,10 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3">
         <v>75</v>
@@ -4905,10 +4948,10 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E4">
         <v>75</v>
@@ -4919,10 +4962,10 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E5">
         <v>75</v>
@@ -4957,7 +5000,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -4969,7 +5012,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>20</v>
@@ -4980,10 +5023,10 @@
         <v>34</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -5005,7 +5048,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -5013,7 +5056,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -5021,7 +5064,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -5029,7 +5072,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -5037,7 +5080,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -5045,7 +5088,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -5053,7 +5096,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -5061,7 +5104,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -5069,7 +5112,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -5077,7 +5120,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -5085,7 +5128,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -5093,7 +5136,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -5101,7 +5144,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18">
         <v>5</v>
@@ -5109,7 +5152,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -5117,7 +5160,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -5125,7 +5168,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -5133,7 +5176,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -5141,7 +5184,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -5149,7 +5192,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -5157,7 +5200,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C25">
         <v>5</v>
@@ -5165,7 +5208,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C26">
         <v>5</v>
@@ -5173,7 +5216,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -5220,34 +5263,34 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="I1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -5258,37 +5301,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -5299,19 +5342,19 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -5322,19 +5365,19 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H4">
         <v>5</v>
@@ -5345,13 +5388,13 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -5362,19 +5405,19 @@
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -5385,13 +5428,13 @@
         <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -5426,7 +5469,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5438,7 +5481,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>20</v>
@@ -5447,10 +5490,10 @@
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -5459,7 +5502,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -5467,10 +5510,10 @@
         <v>34</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>206</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -5492,7 +5535,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -5500,7 +5543,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -5508,7 +5551,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -5516,7 +5559,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -5524,7 +5567,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -5532,7 +5575,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -5540,7 +5583,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -5548,7 +5591,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -5556,7 +5599,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -5564,7 +5607,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -5572,7 +5615,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18">
         <v>5</v>
@@ -5580,7 +5623,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -5588,7 +5631,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -5596,7 +5639,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -5604,7 +5647,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -5612,7 +5655,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -5620,7 +5663,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -5628,7 +5671,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C25">
         <v>5</v>
@@ -5636,7 +5679,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C26">
         <v>5</v>
@@ -5644,7 +5687,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -5652,7 +5695,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C28">
         <v>5</v>
@@ -5660,7 +5703,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C29">
         <v>5</v>
@@ -5695,7 +5738,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5709,10 +5752,10 @@
         <v>34</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5733,7 +5776,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C5">
         <v>0.7</v>
@@ -5741,7 +5784,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C6">
         <v>0.9</v>
@@ -5749,7 +5792,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7">
         <v>0.5</v>
@@ -5757,7 +5800,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8">
         <v>0.4</v>
@@ -5765,7 +5808,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C9">
         <v>0.3</v>
@@ -5773,7 +5816,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10">
         <v>0.2</v>
@@ -5781,7 +5824,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C11">
         <v>0.1</v>
@@ -5789,7 +5832,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C12">
         <v>0.25</v>
@@ -5797,7 +5840,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C13">
         <v>0.25</v>
@@ -5805,7 +5848,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C14">
         <v>0.25</v>
@@ -5813,7 +5856,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15">
         <v>0.25</v>
@@ -5821,7 +5864,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C16">
         <v>0.25</v>
@@ -5829,7 +5872,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17">
         <v>0.25</v>
@@ -5837,7 +5880,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18">
         <v>0.25</v>
@@ -5845,7 +5888,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C19">
         <v>0.25</v>
@@ -5853,7 +5896,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C20">
         <v>0.25</v>
@@ -5861,7 +5904,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C21">
         <v>0.25</v>
@@ -5869,7 +5912,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C22">
         <v>0.25</v>
@@ -5877,7 +5920,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C23">
         <v>0.25</v>
@@ -5885,7 +5928,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C24">
         <v>0.25</v>
@@ -5893,7 +5936,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C25">
         <v>0.25</v>
@@ -5901,7 +5944,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C26">
         <v>0.25</v>
@@ -5935,12 +5978,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -5951,10 +5994,10 @@
         <v>66</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -5993,12 +6036,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6009,10 +6052,10 @@
         <v>33</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -6051,12 +6094,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6064,13 +6107,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -6084,13 +6127,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -6122,12 +6165,12 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -6141,13 +6184,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>186</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>187</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -6161,10 +6204,10 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -6202,14 +6245,14 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -6223,19 +6266,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -6249,16 +6292,16 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -6269,16 +6312,16 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F4">
         <v>-0.1</v>
@@ -6300,7 +6343,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6317,21 +6360,21 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" t="s">
         <v>195</v>
       </c>
-      <c r="E1" t="s">
-        <v>196</v>
-      </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -6339,22 +6382,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -6365,19 +6408,19 @@
         <v>40</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -6388,16 +6431,16 @@
         <v>40</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -6408,19 +6451,19 @@
         <v>41</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -6431,16 +6474,16 @@
         <v>41</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -6448,19 +6491,19 @@
         <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -6468,19 +6511,19 @@
         <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -6527,7 +6570,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -6604,7 +6647,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -6644,7 +6687,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6701,10 +6744,10 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G3">
         <v>20</v>
@@ -6715,10 +6758,10 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G4">
         <v>20</v>
@@ -6729,10 +6772,10 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -6861,18 +6904,18 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -6901,7 +6944,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -6940,7 +6983,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>66</v>
@@ -6989,26 +7032,26 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -7022,10 +7065,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>152</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>153</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>33</v>
@@ -7034,19 +7077,19 @@
         <v>66</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>157</v>
-      </c>
       <c r="J2" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -7089,19 +7132,19 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -7115,22 +7158,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>152</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>153</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>65</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -7168,7 +7211,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -7177,13 +7220,13 @@
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -7197,7 +7240,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7213,114 +7256,114 @@
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="17"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -7341,7 +7384,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7356,11 +7399,11 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -7368,10 +7411,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7382,7 +7425,7 @@
         <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" s="5"/>
     </row>
@@ -7391,10 +7434,10 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -7405,7 +7448,7 @@
         <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -7413,10 +7456,10 @@
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -7455,26 +7498,26 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -7488,31 +7531,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>153</v>
-      </c>
       <c r="D2" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>66</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>157</v>
-      </c>
       <c r="J2" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -7537,7 +7580,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7554,7 +7597,7 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -7562,13 +7605,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7576,7 +7619,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>36</v>
@@ -7590,7 +7633,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>36</v>
@@ -7627,12 +7670,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -7640,13 +7683,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7654,7 +7697,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>36</v>
@@ -7668,7 +7711,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>37</v>
@@ -7682,10 +7725,10 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -7696,10 +7739,10 @@
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -7710,10 +7753,10 @@
         <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -7724,10 +7767,10 @@
         <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -7738,10 +7781,10 @@
         <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -7752,10 +7795,10 @@
         <v>35</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -7766,10 +7809,10 @@
         <v>35</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -7780,10 +7823,10 @@
         <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -7794,10 +7837,10 @@
         <v>35</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -7808,10 +7851,10 @@
         <v>35</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -7822,10 +7865,10 @@
         <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -7836,10 +7879,10 @@
         <v>35</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -7850,10 +7893,10 @@
         <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -7864,10 +7907,10 @@
         <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -7878,10 +7921,10 @@
         <v>35</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -7892,10 +7935,10 @@
         <v>35</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -7906,10 +7949,10 @@
         <v>35</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -7920,10 +7963,10 @@
         <v>35</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -7934,10 +7977,10 @@
         <v>35</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -7948,10 +7991,10 @@
         <v>35</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -7962,10 +8005,10 @@
         <v>35</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -7976,10 +8019,10 @@
         <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -7999,7 +8042,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD7B3D9-76DA-4A96-8BE2-2966A08AF799}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -8018,11 +8061,11 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -8030,10 +8073,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -8041,23 +8084,11 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C3">
         <f>24/8760</f>
         <v>2.7397260273972603E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C4">
-        <f>12/8760</f>
-        <v>1.3698630136986301E-3</v>
       </c>
     </row>
   </sheetData>
@@ -8075,7 +8106,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8087,26 +8118,26 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -8123,7 +8154,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8131,7 +8162,7 @@
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
@@ -8152,62 +8183,62 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E1" t="s">
         <v>216</v>
       </c>
-      <c r="D1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E1" t="s">
-        <v>218</v>
-      </c>
       <c r="F1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J1" t="s">
         <v>146</v>
       </c>
-      <c r="J1" t="s">
-        <v>147</v>
-      </c>
       <c r="K1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="P1" t="s">
         <v>24</v>
       </c>
       <c r="Q1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R1" t="s">
         <v>28</v>
       </c>
       <c r="S1" t="s">
+        <v>85</v>
+      </c>
+      <c r="T1" t="s">
         <v>86</v>
-      </c>
-      <c r="T1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8221,10 +8252,10 @@
         <v>68</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>12</v>
@@ -8233,13 +8264,13 @@
         <v>67</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>73</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>4</v>
@@ -8254,7 +8285,7 @@
         <v>8</v>
       </c>
       <c r="O2" s="24" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
@@ -8266,10 +8297,10 @@
         <v>13</v>
       </c>
       <c r="S2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="T2" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -8277,17 +8308,17 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>190</v>
+        <v>314</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I3">
         <v>10000</v>
@@ -8301,17 +8332,17 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>190</v>
+        <v>310</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I4">
         <v>10000</v>
@@ -8325,10 +8356,10 @@
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I5">
         <v>10000</v>
@@ -8342,10 +8373,10 @@
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I6">
         <v>10000</v>

</xml_diff>

<commit_message>
Changed unit_profile to unit_node_profile. Node_profile (state limits) and connection_profile now work on the model side too. Removed connection__node__node table.
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEF3D56-065D-4B80-BDCD-C8277D41C1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB754EFB-F020-4B7C-9590-ADD18E2EAF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" activeTab="1" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -30,29 +30,28 @@
     <sheet name="connection_c" sheetId="2" r:id="rId15"/>
     <sheet name="connection_p" sheetId="42" r:id="rId16"/>
     <sheet name="connection_t" sheetId="43" r:id="rId17"/>
-    <sheet name="connection_node_node" sheetId="25" r:id="rId18"/>
-    <sheet name="unit_c" sheetId="18" r:id="rId19"/>
-    <sheet name="unit_p" sheetId="21" r:id="rId20"/>
-    <sheet name="unit_t" sheetId="48" r:id="rId21"/>
-    <sheet name="unit_node_c" sheetId="38" r:id="rId22"/>
-    <sheet name="unit_node_t" sheetId="49" r:id="rId23"/>
-    <sheet name="profile_t" sheetId="10" r:id="rId24"/>
-    <sheet name="node_profile_c" sheetId="55" r:id="rId25"/>
-    <sheet name="connection_profile_c" sheetId="56" r:id="rId26"/>
-    <sheet name="unit_profile_c" sheetId="41" r:id="rId27"/>
-    <sheet name="constraint_sense_c" sheetId="44" r:id="rId28"/>
-    <sheet name="unit_node_constraint_c" sheetId="40" r:id="rId29"/>
-    <sheet name="group_c" sheetId="6" r:id="rId30"/>
-    <sheet name="group_p" sheetId="46" r:id="rId31"/>
-    <sheet name="group_connection" sheetId="26" r:id="rId32"/>
-    <sheet name="group_connection_node" sheetId="28" r:id="rId33"/>
-    <sheet name="group_node" sheetId="27" r:id="rId34"/>
-    <sheet name="group_unit" sheetId="29" r:id="rId35"/>
-    <sheet name="group_unit_node" sheetId="30" r:id="rId36"/>
-    <sheet name="reserve_connection_node_c" sheetId="31" r:id="rId37"/>
-    <sheet name="reserve_group_c" sheetId="32" r:id="rId38"/>
-    <sheet name="reserve_group_t" sheetId="50" r:id="rId39"/>
-    <sheet name="reserve_unit_node_c" sheetId="33" r:id="rId40"/>
+    <sheet name="unit_c" sheetId="18" r:id="rId18"/>
+    <sheet name="unit_p" sheetId="21" r:id="rId19"/>
+    <sheet name="unit_t" sheetId="48" r:id="rId20"/>
+    <sheet name="unit_node_c" sheetId="38" r:id="rId21"/>
+    <sheet name="unit_node_t" sheetId="49" r:id="rId22"/>
+    <sheet name="profile_t" sheetId="10" r:id="rId23"/>
+    <sheet name="node_profile_c" sheetId="55" r:id="rId24"/>
+    <sheet name="connection_profile_c" sheetId="56" r:id="rId25"/>
+    <sheet name="unit_node_profile_c" sheetId="41" r:id="rId26"/>
+    <sheet name="constraint_sense_c" sheetId="44" r:id="rId27"/>
+    <sheet name="unit_node_constraint_c" sheetId="40" r:id="rId28"/>
+    <sheet name="group_c" sheetId="6" r:id="rId29"/>
+    <sheet name="group_p" sheetId="46" r:id="rId30"/>
+    <sheet name="group_connection" sheetId="26" r:id="rId31"/>
+    <sheet name="group_connection_node" sheetId="28" r:id="rId32"/>
+    <sheet name="group_node" sheetId="27" r:id="rId33"/>
+    <sheet name="group_unit" sheetId="29" r:id="rId34"/>
+    <sheet name="group_unit_node" sheetId="30" r:id="rId35"/>
+    <sheet name="reserve_connection_node_c" sheetId="31" r:id="rId36"/>
+    <sheet name="reserve_group_c" sheetId="32" r:id="rId37"/>
+    <sheet name="reserve_group_t" sheetId="50" r:id="rId38"/>
+    <sheet name="reserve_unit_node_c" sheetId="33" r:id="rId39"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -201,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="327">
   <si>
     <t>commodity</t>
   </si>
@@ -854,9 +853,6 @@
     <t>A flag whether has a state variable (storage). If empty, then not true. Use 'yes' to indicate true.</t>
   </si>
   <si>
-    <t>Choice of conversion method (efficiency, operating_area).</t>
-  </si>
-  <si>
     <t>Choice between minimum up- and downtimes (&lt;empty&gt;, min_downtime, min_uptime, both).</t>
   </si>
   <si>
@@ -998,15 +994,9 @@
     <t>connection_t</t>
   </si>
   <si>
-    <t>connection_node_node</t>
-  </si>
-  <si>
     <t>profile_t</t>
   </si>
   <si>
-    <t>unit_profile_c</t>
-  </si>
-  <si>
     <t>constraint_sense_c</t>
   </si>
   <si>
@@ -1146,6 +1136,51 @@
   </si>
   <si>
     <t>scale_to_annual_flow</t>
+  </si>
+  <si>
+    <t>Choice of conversion method (efficiency, operating_area, profile).</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Conn1_thermal</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>Changed 'unit_profile' sheet to 'unit_node_profile'.</t>
+  </si>
+  <si>
+    <t>unit_node_profile_c</t>
+  </si>
+  <si>
+    <t>ConnBat</t>
+  </si>
+  <si>
+    <t>Battery_node</t>
+  </si>
+  <si>
+    <t>Battery_profile</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>Added 'Battery_node' and 'Conn_bat' and 'Battery_profile' and Connection_node_node set for the battery. Linked Battery_profile and Battery_node with an upper_limit.</t>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>Removed 'Connection_node_node' sheet. Information about left and right nodes is now contained in 'connection_c' sheet.</t>
+  </si>
+  <si>
+    <t>left_node</t>
+  </si>
+  <si>
+    <t>right_node</t>
   </si>
 </sst>
 </file>
@@ -1401,6 +1436,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1408,9 +1446,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2353,7 +2388,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -2759,11 +2794,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
-  <dimension ref="A2:E33"/>
+  <dimension ref="A2:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2771,302 +2804,293 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
         <v>251</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="E3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="E3" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
-        <v>253</v>
-      </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
       <c r="E4" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
-        <v>246</v>
-      </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
+      <c r="A5" s="43" t="s">
+        <v>245</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
       <c r="E5" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
         <v>254</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
-        <v>255</v>
-      </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="27"/>
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
       <c r="E8" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>256</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="C9" s="31" t="s">
         <v>257</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>259</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="C10" s="32"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
         <v>260</v>
       </c>
-      <c r="C10" s="32"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
-        <v>261</v>
-      </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="B12" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="C12" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>264</v>
-      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
-        <v>265</v>
-      </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
+      <c r="A13" s="31" t="s">
+        <v>280</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>281</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
-        <v>283</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>284</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="B14" s="32"/>
       <c r="C14" s="31" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
-        <v>282</v>
-      </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="31" t="s">
-        <v>281</v>
-      </c>
+      <c r="A15" s="44" t="s">
+        <v>265</v>
+      </c>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
-        <v>268</v>
-      </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
+      <c r="A16" s="44" t="s">
+        <v>266</v>
+      </c>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
-        <v>269</v>
-      </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="40" t="s">
-        <v>266</v>
-      </c>
+      <c r="A19" s="45" t="s">
+        <v>300</v>
+      </c>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
-        <v>303</v>
-      </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
+      <c r="A20" s="45" t="s">
+        <v>299</v>
+      </c>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
-        <v>302</v>
-      </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
+      <c r="A21" s="45" t="s">
+        <v>317</v>
+      </c>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="C23" s="34"/>
+      <c r="D23" s="28"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="41" t="s">
         <v>267</v>
       </c>
-      <c r="B22" s="44"/>
-      <c r="C22" s="44"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
-        <v>279</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>280</v>
-      </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="28"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="42" t="s">
+        <v>272</v>
+      </c>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
+        <v>273</v>
+      </c>
+      <c r="B31" s="36"/>
+      <c r="C31" s="35" t="s">
         <v>274</v>
       </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="45" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="42" t="s">
         <v>275</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
-        <v>276</v>
-      </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="35" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="45" t="s">
-        <v>278</v>
-      </c>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A33:C33"/>
+  <mergeCells count="18">
+    <mergeCell ref="A24:C24"/>
     <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A20:C20"/>
     <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A15:C15"/>
     <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A32:C32"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A31" location="reserve_unit_node_c!A1" display="reserve_connection_node_c" xr:uid="{3F855114-4A57-4E0A-A766-0317F980F4BF}"/>
-    <hyperlink ref="A29" location="group_unit_node!A1" display="group_unit_node" xr:uid="{B7C2FCA3-F9B2-4C44-95E7-EE78C953ADDA}"/>
-    <hyperlink ref="A28" location="group_unit!A1" display="group_unit" xr:uid="{B05CA82D-DD0B-41C5-A4A2-737EB6D8AF37}"/>
-    <hyperlink ref="A27" location="group_node!A1" display="group_node" xr:uid="{920BB948-3B7C-488B-B8B1-7504F3D3AD1A}"/>
-    <hyperlink ref="A26" location="group_connection_node!A1" display="group_connection_node" xr:uid="{811FD465-B06B-4481-9ED6-DE1222C0D3DE}"/>
-    <hyperlink ref="A32" location="reserve_group_c!A1" display="reserve_group_c" xr:uid="{2CFA818C-9B6A-474B-8E40-2E804C4A9677}"/>
-    <hyperlink ref="C32" location="reserve_group_t!A1" display="reserve_group_t" xr:uid="{401EE982-2E1A-4DC0-A8C5-8E9B177FDA74}"/>
-    <hyperlink ref="A33" location="reserve_unit_node_c!A1" display="reserve_unit_node_c" xr:uid="{78371C66-B81A-4E9B-96E1-6659A71B0BF4}"/>
-    <hyperlink ref="A25" location="group_connection!A1" display="group_connection" xr:uid="{A00C70C1-5203-41C9-BCBD-CC42FCD43017}"/>
-    <hyperlink ref="A24" location="group_c!A1" display="group_c" xr:uid="{8516B270-11A5-45FE-B8AE-F8BD21CE42EE}"/>
-    <hyperlink ref="B24" location="group_p!A1" display="group_p" xr:uid="{24A5AB85-580D-4C07-9C0C-EF096DF9B6A4}"/>
-    <hyperlink ref="A17" location="unit_node_constraint_c!A1" display="unit_node_constraint_c" xr:uid="{E752EE81-721A-467B-A89A-558EAD27CD18}"/>
-    <hyperlink ref="A16" location="constraint_sense_c!A1" display="constraint_sense_c" xr:uid="{E3638194-ABA1-4B52-B562-9CB1B5A7326A}"/>
-    <hyperlink ref="A15" location="unit_node_c!A1" display="unit_node_c" xr:uid="{588C2786-F4D1-490C-8299-996C761D1B0B}"/>
-    <hyperlink ref="C15" location="unit_node_t!A1" display="unit_node_t" xr:uid="{848C3082-4242-4C02-A2C8-1DDCCECDDCE4}"/>
-    <hyperlink ref="A14" location="unit_c!A1" display="unit_c" xr:uid="{0B24F06D-DF0D-43E9-A754-3D573B0328ED}"/>
-    <hyperlink ref="B14" location="unit_p!A1" display="unit_p" xr:uid="{6B0EC5F5-0D3E-41BB-B4D8-64F5821432A7}"/>
-    <hyperlink ref="C14" location="unit_t!A1" display="unit_t" xr:uid="{563A1A91-8913-4B2F-8BA5-4D350923C03F}"/>
-    <hyperlink ref="C19" location="profile_t!A1" display="profile_t" xr:uid="{78412094-AA9A-4901-935D-64F3C1AC7206}"/>
-    <hyperlink ref="A13" location="connection_node_node!A1" display="connection_node_node" xr:uid="{401C0132-E4E0-4396-A006-5B422AE5148C}"/>
+    <hyperlink ref="A30" location="reserve_unit_node_c!A1" display="reserve_connection_node_c" xr:uid="{3F855114-4A57-4E0A-A766-0317F980F4BF}"/>
+    <hyperlink ref="A28" location="group_unit_node!A1" display="group_unit_node" xr:uid="{B7C2FCA3-F9B2-4C44-95E7-EE78C953ADDA}"/>
+    <hyperlink ref="A27" location="group_unit!A1" display="group_unit" xr:uid="{B05CA82D-DD0B-41C5-A4A2-737EB6D8AF37}"/>
+    <hyperlink ref="A26" location="group_node!A1" display="group_node" xr:uid="{920BB948-3B7C-488B-B8B1-7504F3D3AD1A}"/>
+    <hyperlink ref="A25" location="group_connection_node!A1" display="group_connection_node" xr:uid="{811FD465-B06B-4481-9ED6-DE1222C0D3DE}"/>
+    <hyperlink ref="A31" location="reserve_group_c!A1" display="reserve_group_c" xr:uid="{2CFA818C-9B6A-474B-8E40-2E804C4A9677}"/>
+    <hyperlink ref="C31" location="reserve_group_t!A1" display="reserve_group_t" xr:uid="{401EE982-2E1A-4DC0-A8C5-8E9B177FDA74}"/>
+    <hyperlink ref="A32" location="reserve_unit_node_c!A1" display="reserve_unit_node_c" xr:uid="{78371C66-B81A-4E9B-96E1-6659A71B0BF4}"/>
+    <hyperlink ref="A24" location="group_connection!A1" display="group_connection" xr:uid="{A00C70C1-5203-41C9-BCBD-CC42FCD43017}"/>
+    <hyperlink ref="A23" location="group_c!A1" display="group_c" xr:uid="{8516B270-11A5-45FE-B8AE-F8BD21CE42EE}"/>
+    <hyperlink ref="B23" location="group_p!A1" display="group_p" xr:uid="{24A5AB85-580D-4C07-9C0C-EF096DF9B6A4}"/>
+    <hyperlink ref="A16" location="unit_node_constraint_c!A1" display="unit_node_constraint_c" xr:uid="{E752EE81-721A-467B-A89A-558EAD27CD18}"/>
+    <hyperlink ref="A15" location="constraint_sense_c!A1" display="constraint_sense_c" xr:uid="{E3638194-ABA1-4B52-B562-9CB1B5A7326A}"/>
+    <hyperlink ref="A14" location="unit_node_c!A1" display="unit_node_c" xr:uid="{588C2786-F4D1-490C-8299-996C761D1B0B}"/>
+    <hyperlink ref="C14" location="unit_node_t!A1" display="unit_node_t" xr:uid="{848C3082-4242-4C02-A2C8-1DDCCECDDCE4}"/>
+    <hyperlink ref="A13" location="unit_c!A1" display="unit_c" xr:uid="{0B24F06D-DF0D-43E9-A754-3D573B0328ED}"/>
+    <hyperlink ref="B13" location="unit_p!A1" display="unit_p" xr:uid="{6B0EC5F5-0D3E-41BB-B4D8-64F5821432A7}"/>
+    <hyperlink ref="C13" location="unit_t!A1" display="unit_t" xr:uid="{563A1A91-8913-4B2F-8BA5-4D350923C03F}"/>
+    <hyperlink ref="C18" location="profile_t!A1" display="profile_t" xr:uid="{78412094-AA9A-4901-935D-64F3C1AC7206}"/>
     <hyperlink ref="A12" location="connection_c!A1" display="connection_c" xr:uid="{03E6664B-5F07-4921-A88F-1CC8DA8E9FAE}"/>
     <hyperlink ref="B12" location="connection_p!A1" display="connection_p" xr:uid="{46902093-FDC0-4939-BBFD-2D41FFBE0F05}"/>
     <hyperlink ref="C12" location="connection_t!A1" display="connection_t" xr:uid="{5D63301C-ED60-425E-8FC0-334B75B4F98C}"/>
@@ -3083,11 +3107,12 @@
     <hyperlink ref="A4" location="solve_sequence!A1" display="solve_sequence" xr:uid="{3B08721C-A5BF-4AD9-9840-41F099D6F77C}"/>
     <hyperlink ref="A3" location="solve_period!A1" display="solve_period" xr:uid="{1A642A0E-886B-4C5F-9459-AF06B635D1C8}"/>
     <hyperlink ref="A2" location="version!A1" display="version" xr:uid="{5528FB5D-B49F-4A94-B79B-BD7CACBF6421}"/>
-    <hyperlink ref="A21" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{BFEE1E54-8BED-43DB-81D7-EF22B030644E}"/>
-    <hyperlink ref="A22" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{F130C8C0-C1F9-49C3-9475-FD4618C13C76}"/>
-    <hyperlink ref="A20" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{844403FD-DCCB-46C7-BE3C-C68DCAAB6B04}"/>
-    <hyperlink ref="A20:C20" location="node_profile_c!A1" display="node_profile_c" xr:uid="{826B47E5-87EB-412A-A0AE-C49CDB5CEB93}"/>
-    <hyperlink ref="A21:C21" location="connection_profile_c!A1" display="connection_profile_c" xr:uid="{DB781E38-3ACC-4F21-8D1E-B47D2A016C51}"/>
+    <hyperlink ref="A20" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{BFEE1E54-8BED-43DB-81D7-EF22B030644E}"/>
+    <hyperlink ref="A21" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{F130C8C0-C1F9-49C3-9475-FD4618C13C76}"/>
+    <hyperlink ref="A19" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{844403FD-DCCB-46C7-BE3C-C68DCAAB6B04}"/>
+    <hyperlink ref="A19:C19" location="node_profile_c!A1" display="node_profile_c" xr:uid="{826B47E5-87EB-412A-A0AE-C49CDB5CEB93}"/>
+    <hyperlink ref="A20:C20" location="connection_profile_c!A1" display="connection_profile_c" xr:uid="{DB781E38-3ACC-4F21-8D1E-B47D2A016C51}"/>
+    <hyperlink ref="A21:C21" location="unit_node_profile_c!A1" display="unit_profile_c" xr:uid="{B2BA97AF-8BE5-4D5F-8341-41044F5963AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3122,7 +3147,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -3145,7 +3170,7 @@
         <v>78</v>
       </c>
       <c r="J1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="K1" t="s">
         <v>24</v>
@@ -3186,7 +3211,7 @@
         <v>8</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>7</v>
@@ -3206,7 +3231,7 @@
         <v>177</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D3">
         <f>3000*8760/24*1.1</f>
@@ -3229,7 +3254,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3242,7 +3267,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -3285,7 +3310,7 @@
         <v>36</v>
       </c>
       <c r="C4">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>-100</v>
@@ -3296,7 +3321,7 @@
         <v>37</v>
       </c>
       <c r="C5">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>-100</v>
@@ -3308,7 +3333,7 @@
         <v>96</v>
       </c>
       <c r="C6">
-        <v>-30</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>-100</v>
@@ -3319,7 +3344,7 @@
         <v>97</v>
       </c>
       <c r="C7">
-        <v>-40</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>-100</v>
@@ -3330,7 +3355,7 @@
         <v>98</v>
       </c>
       <c r="C8">
-        <v>-50</v>
+        <v>-100</v>
       </c>
       <c r="D8">
         <v>-100</v>
@@ -3341,7 +3366,7 @@
         <v>99</v>
       </c>
       <c r="C9">
-        <v>-60</v>
+        <v>-100</v>
       </c>
       <c r="D9">
         <v>-100</v>
@@ -3352,7 +3377,7 @@
         <v>100</v>
       </c>
       <c r="C10">
-        <v>-70</v>
+        <v>-100</v>
       </c>
       <c r="D10">
         <v>-100</v>
@@ -3363,7 +3388,7 @@
         <v>101</v>
       </c>
       <c r="C11">
-        <v>-80</v>
+        <v>-100</v>
       </c>
       <c r="D11">
         <v>-100</v>
@@ -3374,7 +3399,7 @@
         <v>102</v>
       </c>
       <c r="C12">
-        <v>-90</v>
+        <v>-200</v>
       </c>
       <c r="D12">
         <v>-100</v>
@@ -3385,7 +3410,7 @@
         <v>103</v>
       </c>
       <c r="C13">
-        <v>-100</v>
+        <v>-200</v>
       </c>
       <c r="D13">
         <v>-100</v>
@@ -3396,7 +3421,7 @@
         <v>104</v>
       </c>
       <c r="C14">
-        <v>-110</v>
+        <v>-200</v>
       </c>
       <c r="D14">
         <v>-100</v>
@@ -3407,7 +3432,7 @@
         <v>105</v>
       </c>
       <c r="C15">
-        <v>-120</v>
+        <v>-200</v>
       </c>
       <c r="D15">
         <v>-100</v>
@@ -3418,7 +3443,7 @@
         <v>106</v>
       </c>
       <c r="C16">
-        <v>-130</v>
+        <v>-300</v>
       </c>
       <c r="D16">
         <v>-100</v>
@@ -3429,7 +3454,7 @@
         <v>107</v>
       </c>
       <c r="C17">
-        <v>-140</v>
+        <v>-300</v>
       </c>
       <c r="D17">
         <v>-100</v>
@@ -3440,7 +3465,7 @@
         <v>108</v>
       </c>
       <c r="C18">
-        <v>-150</v>
+        <v>-300</v>
       </c>
       <c r="D18">
         <v>-100</v>
@@ -3451,7 +3476,7 @@
         <v>109</v>
       </c>
       <c r="C19">
-        <v>-160</v>
+        <v>-300</v>
       </c>
       <c r="D19">
         <v>-100</v>
@@ -3462,7 +3487,7 @@
         <v>110</v>
       </c>
       <c r="C20">
-        <v>-170</v>
+        <v>-400</v>
       </c>
       <c r="D20">
         <v>-100</v>
@@ -3473,7 +3498,7 @@
         <v>111</v>
       </c>
       <c r="C21">
-        <v>-180</v>
+        <v>-400</v>
       </c>
       <c r="D21">
         <v>-100</v>
@@ -3484,7 +3509,7 @@
         <v>112</v>
       </c>
       <c r="C22">
-        <v>-190</v>
+        <v>-400</v>
       </c>
       <c r="D22">
         <v>-100</v>
@@ -3495,7 +3520,7 @@
         <v>113</v>
       </c>
       <c r="C23">
-        <v>-200</v>
+        <v>-400</v>
       </c>
       <c r="D23">
         <v>-100</v>
@@ -3506,7 +3531,7 @@
         <v>114</v>
       </c>
       <c r="C24">
-        <v>-210</v>
+        <v>-500</v>
       </c>
       <c r="D24">
         <v>-100</v>
@@ -3517,7 +3542,7 @@
         <v>115</v>
       </c>
       <c r="C25">
-        <v>-220</v>
+        <v>-500</v>
       </c>
       <c r="D25">
         <v>-100</v>
@@ -3528,7 +3553,7 @@
         <v>116</v>
       </c>
       <c r="C26">
-        <v>-230</v>
+        <v>-500</v>
       </c>
       <c r="D26">
         <v>-100</v>
@@ -3539,7 +3564,7 @@
         <v>117</v>
       </c>
       <c r="C27">
-        <v>-240</v>
+        <v>-500</v>
       </c>
       <c r="D27">
         <v>-100</v>
@@ -3575,7 +3600,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1"/>
       <c r="C1" t="s">
@@ -3653,7 +3678,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -3711,7 +3736,7 @@
         <v>191</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D5">
         <v>22</v>
@@ -3781,167 +3806,212 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D44D2B2-1DE7-400D-8C40-2CD59BEE6EC3}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M28" sqref="M28"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
-    <col min="12" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" customWidth="1"/>
-    <col min="17" max="17" width="10" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" customWidth="1"/>
+    <col min="19" max="19" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="3"/>
+      <c r="E1" t="s">
         <v>212</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>213</v>
       </c>
-      <c r="E1" t="s">
-        <v>221</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H1" t="s">
         <v>214</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>148</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>42</v>
       </c>
-      <c r="L1" t="s">
-        <v>297</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>294</v>
+      </c>
+      <c r="O1" t="s">
         <v>24</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>23</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="O2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3" t="s">
         <v>202</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>203</v>
       </c>
-      <c r="E3" t="s">
-        <v>220</v>
-      </c>
-      <c r="H3">
+      <c r="G3" t="s">
+        <v>219</v>
+      </c>
+      <c r="J3">
         <v>100</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>100</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>500</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>0.05</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="E4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F4" t="s">
+        <v>203</v>
+      </c>
+      <c r="G4" t="s">
+        <v>176</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="S4">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -3982,12 +4052,12 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E1" t="s">
         <v>26</v>
@@ -4002,7 +4072,7 @@
         <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="J1" t="s">
         <v>24</v>
@@ -4040,7 +4110,7 @@
         <v>8</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
@@ -4088,7 +4158,7 @@
         <v>38</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E5">
         <v>150</v>
@@ -4110,7 +4180,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4123,7 +4193,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -4356,59 +4426,6 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22779BFC-2A05-4741-ADBE-AFE66F77AC46}">
-  <dimension ref="A1:L2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="11" customWidth="1"/>
-    <col min="4" max="9" width="11.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6619729E-584E-41E3-B72E-7B2979330C88}">
   <dimension ref="A1:W5"/>
   <sheetViews>
@@ -4416,7 +4433,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4447,20 +4464,20 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>217</v>
+        <v>312</v>
       </c>
       <c r="D1" t="s">
         <v>213</v>
       </c>
       <c r="E1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G1" t="s">
         <v>22</v>
@@ -4475,7 +4492,7 @@
         <v>144</v>
       </c>
       <c r="K1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="L1" t="s">
         <v>24</v>
@@ -4502,10 +4519,10 @@
         <v>131</v>
       </c>
       <c r="T1" t="s">
+        <v>235</v>
+      </c>
+      <c r="U1" t="s">
         <v>236</v>
-      </c>
-      <c r="U1" t="s">
-        <v>237</v>
       </c>
       <c r="V1" t="s">
         <v>123</v>
@@ -4546,7 +4563,7 @@
         <v>8</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="L2" s="24" t="s">
         <v>7</v>
@@ -4599,7 +4616,7 @@
         <v>203</v>
       </c>
       <c r="F3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -4629,7 +4646,7 @@
         <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>313</v>
       </c>
       <c r="D4" t="s">
         <v>203</v>
@@ -4661,7 +4678,7 @@
         <v>176</v>
       </c>
       <c r="G5">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="Q5">
         <v>0.5</v>
@@ -4675,155 +4692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>227</v>
-      </c>
-      <c r="B3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B4" s="25">
-        <v>44594</v>
-      </c>
-      <c r="C4" t="s">
-        <v>231</v>
-      </c>
-      <c r="D4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B5" s="25">
-        <v>44595</v>
-      </c>
-      <c r="C5" t="s">
-        <v>231</v>
-      </c>
-      <c r="D5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B6" s="25">
-        <v>44600</v>
-      </c>
-      <c r="C6" t="s">
-        <v>231</v>
-      </c>
-      <c r="D6" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="B7" s="25">
-        <v>44602</v>
-      </c>
-      <c r="C7" t="s">
-        <v>231</v>
-      </c>
-      <c r="D7" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="B8" s="25">
-        <v>44602</v>
-      </c>
-      <c r="C8" t="s">
-        <v>231</v>
-      </c>
-      <c r="D8" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="B9" s="25">
-        <v>44602</v>
-      </c>
-      <c r="C9" t="s">
-        <v>231</v>
-      </c>
-      <c r="D9" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="B10" s="25">
-        <v>44602</v>
-      </c>
-      <c r="C10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D10" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B11" s="25">
-        <v>44603</v>
-      </c>
-      <c r="C11" t="s">
-        <v>231</v>
-      </c>
-      <c r="D11" t="s">
-        <v>313</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F519FEB-FCA9-4C11-88F7-D4EA23EF6482}">
   <dimension ref="A1:M5"/>
   <sheetViews>
@@ -4853,7 +4722,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4873,7 +4742,7 @@
         <v>144</v>
       </c>
       <c r="I1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="J1" t="s">
         <v>24</v>
@@ -4914,7 +4783,7 @@
         <v>8</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
@@ -4965,7 +4834,7 @@
         <v>180</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E5">
         <v>75</v>
@@ -4979,7 +4848,199 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="25">
+        <v>44594</v>
+      </c>
+      <c r="C4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" s="25">
+        <v>44595</v>
+      </c>
+      <c r="C5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" s="25">
+        <v>44600</v>
+      </c>
+      <c r="C6" t="s">
+        <v>230</v>
+      </c>
+      <c r="D6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B7" s="25">
+        <v>44602</v>
+      </c>
+      <c r="C7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B8" s="25">
+        <v>44602</v>
+      </c>
+      <c r="C8" t="s">
+        <v>230</v>
+      </c>
+      <c r="D8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B9" s="25">
+        <v>44602</v>
+      </c>
+      <c r="C9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B10" s="25">
+        <v>44602</v>
+      </c>
+      <c r="C10" t="s">
+        <v>230</v>
+      </c>
+      <c r="D10" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B11" s="25">
+        <v>44603</v>
+      </c>
+      <c r="C11" t="s">
+        <v>230</v>
+      </c>
+      <c r="D11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B12" s="25">
+        <v>44605</v>
+      </c>
+      <c r="C12" t="s">
+        <v>230</v>
+      </c>
+      <c r="D12" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B13" s="25">
+        <v>44605</v>
+      </c>
+      <c r="C13" t="s">
+        <v>230</v>
+      </c>
+      <c r="D13" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B14" s="25">
+        <v>44605</v>
+      </c>
+      <c r="C14" t="s">
+        <v>230</v>
+      </c>
+      <c r="D14" t="s">
+        <v>324</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A4A219-02B1-4261-8559-589A0949A31B}">
   <dimension ref="A1:K27"/>
   <sheetViews>
@@ -5000,7 +5061,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5232,7 +5293,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C13F0C3-2BD2-4859-9713-8823A445C2E8}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
@@ -5263,7 +5324,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5275,10 +5336,10 @@
         <v>172</v>
       </c>
       <c r="G1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I1" t="s">
         <v>136</v>
@@ -5316,7 +5377,7 @@
         <v>20</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>128</v>
@@ -5448,7 +5509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54CEF76-2D28-40D4-A5BB-1AAB8A75E52F}">
   <dimension ref="A1:K29"/>
   <sheetViews>
@@ -5469,7 +5530,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5719,15 +5780,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE19B28-F2BE-409F-B1A6-1F5F2146177E}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5736,7 +5797,7 @@
     <col min="2" max="2" width="12" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>174</v>
       </c>
@@ -5746,8 +5807,14 @@
       <c r="C1" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>34</v>
       </c>
@@ -5757,197 +5824,347 @@
       <c r="C2" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.8</v>
+      </c>
+      <c r="E3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C4">
+        <v>0.75</v>
+      </c>
+      <c r="D4">
+        <v>0.8</v>
+      </c>
+      <c r="E4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>96</v>
       </c>
       <c r="C5">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C6">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>98</v>
       </c>
       <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>99</v>
       </c>
       <c r="C8">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>100</v>
       </c>
       <c r="C9">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>101</v>
       </c>
       <c r="C10">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>102</v>
       </c>
       <c r="C11">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>103</v>
       </c>
       <c r="C12">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>104</v>
       </c>
       <c r="C13">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>105</v>
       </c>
       <c r="C14">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>106</v>
       </c>
       <c r="C15">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>107</v>
       </c>
       <c r="C16">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>108</v>
       </c>
       <c r="C17">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>109</v>
       </c>
       <c r="C18">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>110</v>
       </c>
       <c r="C19">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>111</v>
       </c>
       <c r="C20">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>112</v>
       </c>
       <c r="C21">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>113</v>
       </c>
       <c r="C22">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>114</v>
       </c>
       <c r="C23">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>115</v>
       </c>
       <c r="C24">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>116</v>
       </c>
       <c r="C25">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C26">
-        <v>0.25</v>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -5956,15 +6173,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F666A2D2-C97B-40BC-8DAB-2941397753E9}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5978,12 +6195,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6005,6 +6222,20 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="D3" t="s">
+        <v>209</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6014,15 +6245,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3E6DA50-D119-4E64-AFE0-DB17C1EE7F55}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6036,12 +6267,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6063,6 +6294,20 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="D3" t="s">
+        <v>209</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6072,67 +6317,75 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1EE4BC-08B3-4CC5-9A8F-D2957036E873}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="7" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="8" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D1" s="3"/>
+      <c r="E1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>209</v>
       </c>
     </row>
@@ -6144,7 +6397,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C017E3-B844-46CF-8B82-D76F5D9D7ACD}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -6165,7 +6418,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6221,7 +6474,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA1124C-4BD2-46D2-BD33-99ED754CAC73}">
   <dimension ref="A1:M4"/>
   <sheetViews>
@@ -6245,7 +6498,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6335,207 +6588,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F0779D-09F6-4BFC-A27B-5A43B3911876}">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="14" width="11.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>290</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E1" t="s">
-        <v>195</v>
-      </c>
-      <c r="F1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" t="s">
-        <v>197</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>189</v>
-      </c>
-      <c r="G3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" t="s">
-        <v>197</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>189</v>
-      </c>
-      <c r="G5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="D6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" t="s">
-        <v>196</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" t="s">
-        <v>196</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" location="navigate!A1" display="navigate" xr:uid="{C6E1C94C-815A-4152-B8CE-F4022E1F30E1}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -6570,7 +6623,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -6661,7 +6714,207 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F0779D-09F6-4BFC-A27B-5A43B3911876}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="14" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>287</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="navigate!A1" display="navigate" xr:uid="{C6E1C94C-815A-4152-B8CE-F4022E1F30E1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA54FD9A-FB2F-4111-AC75-F20843B34F53}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -6687,7 +6940,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6775,7 +7028,7 @@
         <v>183</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -6789,7 +7042,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B745B3BE-1539-44A7-9F68-00D8AEBADA46}">
   <dimension ref="A1:K1"/>
   <sheetViews>
@@ -6827,7 +7080,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C65105-DA47-40FD-BED9-039766CD67C2}">
   <dimension ref="A1:L1"/>
   <sheetViews>
@@ -6869,7 +7122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6F0B0-C8D9-4343-9EA4-859E87C9AF78}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -6923,7 +7176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5455887B-7914-47A3-A368-88187BB1082B}">
   <dimension ref="A1:K1"/>
   <sheetViews>
@@ -6961,7 +7214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8ED891B-8A85-405F-972C-9B1BFE92F9B9}">
   <dimension ref="A1:L1"/>
   <sheetViews>
@@ -7006,7 +7259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB87FF22-BB83-4D5E-B38D-455D581CF757}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -7032,14 +7285,14 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G1" t="s">
         <v>154</v>
@@ -7077,7 +7330,7 @@
         <v>66</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>153</v>
@@ -7106,7 +7359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{866244AD-1571-447F-BAEE-EFE2B5B3F812}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -7132,7 +7385,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7190,7 +7443,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E57CD72E-4345-442F-8DFC-A799FEED107D}">
   <dimension ref="A1:K29"/>
   <sheetViews>
@@ -7211,7 +7464,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -7373,6 +7626,107 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8C0D5E-7DB2-4BCF-8A8C-24C978AAECC4}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="13" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>287</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I1" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" t="s">
+        <v>159</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="navigate!A1" display="navigate" xr:uid="{B2A6F1D1-6C16-4B66-9828-5A584405A522}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -7399,11 +7753,11 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -7456,7 +7810,7 @@
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C6" t="s">
         <v>199</v>
@@ -7468,107 +7822,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8C0D5E-7DB2-4BCF-8A8C-24C978AAECC4}">
-  <dimension ref="A1:P2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="13" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="13" width="11.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>290</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G1" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1" t="s">
-        <v>166</v>
-      </c>
-      <c r="I1" t="s">
-        <v>157</v>
-      </c>
-      <c r="J1" t="s">
-        <v>159</v>
-      </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" location="navigate!A1" display="navigate" xr:uid="{B2A6F1D1-6C16-4B66-9828-5A584405A522}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -7605,13 +7858,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7670,12 +7923,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -7686,10 +7939,10 @@
         <v>118</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8061,7 +8314,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -8118,7 +8371,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>118</v>
@@ -8148,13 +8401,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8183,20 +8436,20 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
         <v>215</v>
       </c>
       <c r="D1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E1" t="s">
         <v>216</v>
       </c>
       <c r="F1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G1" t="s">
         <v>184</v>
@@ -8223,7 +8476,7 @@
         <v>78</v>
       </c>
       <c r="O1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="P1" t="s">
         <v>24</v>
@@ -8252,7 +8505,7 @@
         <v>68</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>69</v>
@@ -8285,7 +8538,7 @@
         <v>8</v>
       </c>
       <c r="O2" s="24" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
@@ -8314,7 +8567,7 @@
         <v>189</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" t="s">
@@ -8338,7 +8591,7 @@
         <v>189</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" t="s">
@@ -8383,6 +8636,32 @@
       </c>
       <c r="J6">
         <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E7" t="s">
+        <v>189</v>
+      </c>
+      <c r="F7" t="s">
+        <v>176</v>
+      </c>
+      <c r="I7">
+        <v>12000</v>
+      </c>
+      <c r="J7">
+        <v>12000</v>
+      </c>
+      <c r="K7">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Don't output reserve_method to reserve parameter csv
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD366C06-9047-4F82-B5C4-E04088C2F1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8AFB55-37C3-4B23-9DD1-925AB3F81820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="1000" firstSheet="10" activeTab="36" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="12795" yWindow="1065" windowWidth="16395" windowHeight="21000" tabRatio="1000" activeTab="8" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -2820,7 +2820,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3606,7 +3608,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3830,7 +3832,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4718,7 +4720,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6742,13 +6744,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F0779D-09F6-4BFC-A27B-5A43B3911876}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6931,12 +6933,20 @@
         <v>188</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="navigate!A1" display="navigate" xr:uid="{C6E1C94C-815A-4152-B8CE-F4022E1F30E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7397,11 +7407,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{866244AD-1571-447F-BAEE-EFE2B5B3F812}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7916,7 +7926,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8486,7 +8496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>

<commit_message>
Added inertia constraint to the model and data processing
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8AFB55-37C3-4B23-9DD1-925AB3F81820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A47841-46E1-4324-A074-C0470E74BEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12795" yWindow="1065" windowWidth="16395" windowHeight="21000" tabRatio="1000" activeTab="8" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="16" activeTab="28" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="334">
   <si>
     <t>commodity</t>
   </si>
@@ -943,9 +943,6 @@
     <t>block_duration</t>
   </si>
   <si>
-    <t>timesteps</t>
-  </si>
-  <si>
     <t>timestep_name</t>
   </si>
   <si>
@@ -1202,6 +1199,9 @@
   </si>
   <si>
     <t>primary</t>
+  </si>
+  <si>
+    <t>duration</t>
   </si>
 </sst>
 </file>
@@ -2040,7 +2040,7 @@
             <a:rPr lang="fi-FI" sz="1200" baseline="0">
               <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>- timesteps: duration of each time step (in hours)</a:t>
+            <a:t>- duration: duration of each time step (in hours)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2821,7 +2821,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2833,40 +2833,40 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
+        <v>325</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>326</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>328</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
       <c r="E3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="E4" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2876,24 +2876,24 @@
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="E5" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
@@ -2903,77 +2903,77 @@
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
       <c r="E8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>254</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="C9" s="31" t="s">
         <v>255</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>257</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>258</v>
       </c>
       <c r="C10" s="32"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="B12" s="31" t="s">
         <v>260</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="C12" s="31" t="s">
         <v>261</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>279</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="C13" s="31" t="s">
         <v>280</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B14" s="32"/>
       <c r="C14" s="31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B15" s="44"/>
       <c r="C15" s="44"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
@@ -2987,26 +2987,26 @@
       <c r="A18" s="39"/>
       <c r="B18" s="39"/>
       <c r="C18" s="40" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B19" s="45"/>
       <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
@@ -3018,45 +3018,45 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="B23" s="34" t="s">
         <v>275</v>
-      </c>
-      <c r="B23" s="34" t="s">
-        <v>276</v>
       </c>
       <c r="C23" s="34"/>
       <c r="D23" s="28"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B24" s="41"/>
       <c r="C24" s="41"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
@@ -3068,23 +3068,23 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="42"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B31" s="36"/>
       <c r="C31" s="35" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="42"/>
@@ -3167,7 +3167,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -3190,7 +3190,7 @@
         <v>78</v>
       </c>
       <c r="J1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K1" t="s">
         <v>24</v>
@@ -3231,7 +3231,7 @@
         <v>8</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>7</v>
@@ -3287,7 +3287,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -3620,7 +3620,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1"/>
       <c r="C1" t="s">
@@ -3698,7 +3698,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -3832,7 +3832,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3857,7 +3857,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -3890,7 +3890,7 @@
         <v>42</v>
       </c>
       <c r="N1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O1" t="s">
         <v>24</v>
@@ -3916,10 +3916,10 @@
         <v>33</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>324</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>325</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>19</v>
@@ -3949,7 +3949,7 @@
         <v>8</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O2" s="9" t="s">
         <v>7</v>
@@ -4010,13 +4010,13 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>176</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E4" t="s">
         <v>201</v>
@@ -4072,7 +4072,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4092,7 +4092,7 @@
         <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J1" t="s">
         <v>24</v>
@@ -4130,7 +4130,7 @@
         <v>8</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
@@ -4213,7 +4213,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -4453,7 +4453,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4484,11 +4484,11 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D1" t="s">
         <v>212</v>
@@ -4512,7 +4512,7 @@
         <v>144</v>
       </c>
       <c r="K1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L1" t="s">
         <v>24</v>
@@ -4583,7 +4583,7 @@
         <v>8</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L2" s="24" t="s">
         <v>7</v>
@@ -4666,7 +4666,7 @@
         <v>180</v>
       </c>
       <c r="C4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D4" t="s">
         <v>202</v>
@@ -4720,7 +4720,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4742,7 +4742,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4762,7 +4762,7 @@
         <v>144</v>
       </c>
       <c r="I1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J1" t="s">
         <v>24</v>
@@ -4803,7 +4803,7 @@
         <v>8</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
@@ -4954,12 +4954,12 @@
         <v>229</v>
       </c>
       <c r="D7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B8" s="25">
         <v>44602</v>
@@ -4968,12 +4968,12 @@
         <v>229</v>
       </c>
       <c r="D8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B9" s="25">
         <v>44602</v>
@@ -4982,12 +4982,12 @@
         <v>229</v>
       </c>
       <c r="D9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B10" s="25">
         <v>44602</v>
@@ -4996,12 +4996,12 @@
         <v>229</v>
       </c>
       <c r="D10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B11" s="25">
         <v>44603</v>
@@ -5010,12 +5010,12 @@
         <v>229</v>
       </c>
       <c r="D11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B12" s="25">
         <v>44605</v>
@@ -5024,12 +5024,12 @@
         <v>229</v>
       </c>
       <c r="D12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B13" s="25">
         <v>44605</v>
@@ -5038,12 +5038,12 @@
         <v>229</v>
       </c>
       <c r="D13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B14" s="25">
         <v>44605</v>
@@ -5052,7 +5052,7 @@
         <v>229</v>
       </c>
       <c r="D14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -5081,7 +5081,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5344,7 +5344,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5356,10 +5356,10 @@
         <v>171</v>
       </c>
       <c r="G1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I1" t="s">
         <v>136</v>
@@ -5397,7 +5397,7 @@
         <v>20</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>128</v>
@@ -5550,7 +5550,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5808,7 +5808,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5845,10 +5845,10 @@
         <v>174</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -6201,7 +6201,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6215,12 +6215,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6248,10 +6248,10 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>318</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>319</v>
       </c>
       <c r="D3" t="s">
         <v>208</v>
@@ -6287,12 +6287,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6323,7 +6323,7 @@
         <v>38</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D3" t="s">
         <v>208</v>
@@ -6360,13 +6360,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -6438,7 +6438,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6518,7 +6518,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6612,11 +6612,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6643,7 +6643,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -6731,7 +6731,16 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
+      </c>
+      <c r="E4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F4">
+        <v>200</v>
+      </c>
+      <c r="G4">
+        <v>5000</v>
       </c>
     </row>
   </sheetData>
@@ -6750,7 +6759,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6767,7 +6776,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6976,7 +6985,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7209,7 +7218,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>176</v>
@@ -7329,7 +7338,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7411,7 +7420,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7429,13 +7438,13 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F1" t="s">
         <v>163</v>
@@ -7484,16 +7493,16 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>330</v>
-      </c>
       <c r="E3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -7518,7 +7527,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7531,7 +7540,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -7704,7 +7713,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7723,7 +7732,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7794,10 +7803,10 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>179</v>
@@ -7846,7 +7855,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -7926,7 +7935,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8002,7 +8011,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8016,7 +8025,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -8032,10 +8041,10 @@
         <v>118</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>247</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8407,7 +8416,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -8496,11 +8505,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8529,14 +8538,14 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
         <v>214</v>
       </c>
       <c r="D1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E1" t="s">
         <v>215</v>
@@ -8569,7 +8578,7 @@
         <v>78</v>
       </c>
       <c r="O1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="P1" t="s">
         <v>24</v>
@@ -8598,7 +8607,7 @@
         <v>68</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>69</v>
@@ -8631,7 +8640,7 @@
         <v>8</v>
       </c>
       <c r="O2" s="24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
@@ -8660,7 +8669,7 @@
         <v>188</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" t="s">
@@ -8684,7 +8693,7 @@
         <v>188</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" t="s">
@@ -8736,7 +8745,7 @@
         <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C7" t="s">
         <v>188</v>

</xml_diff>

<commit_message>
Added is_active to choose active parts of the model.
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E1F970-BA5B-4652-8948-C7CD26ABEFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72154BA2-4C36-461E-B1D8-5F76038ADCCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="1000" activeTab="1" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="3" activeTab="20" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="342">
   <si>
     <t>commodity</t>
   </si>
@@ -1214,6 +1214,18 @@
   </si>
   <si>
     <t>Changed 'is_synchronous' to 'is_non_synchronous' in unit_node_c. Also 'has_DC' to 'is_DC' in connection_c. Added 'penalty_non_synchronous' to group_c.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> is_active</t>
+  </si>
+  <si>
+    <t>Whether the unit is present in the alternative.</t>
+  </si>
+  <si>
+    <t>Whether the node is present in the alternative.</t>
+  </si>
+  <si>
+    <t>Battery</t>
   </si>
 </sst>
 </file>
@@ -2214,7 +2226,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -2424,7 +2436,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -2832,7 +2844,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3836,13 +3850,13 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D44D2B2-1DE7-400D-8C40-2CD59BEE6EC3}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3852,20 +3866,21 @@
     <col min="3" max="3" width="12.140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" style="11" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="15" width="13" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" customWidth="1"/>
-    <col min="19" max="19" width="10" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="16" width="13" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" customWidth="1"/>
+    <col min="20" max="20" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>284</v>
       </c>
@@ -3873,52 +3888,55 @@
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F1" t="s">
         <v>210</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>211</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>218</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>212</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>147</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>291</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>23</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>22</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>31</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -3931,53 +3949,56 @@
       <c r="D2" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="24" t="s">
+        <v>338</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -3991,36 +4012,39 @@
         <v>176</v>
       </c>
       <c r="E3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F3" t="s">
         <v>200</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>201</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>217</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>187</v>
-      </c>
-      <c r="J3">
-        <v>100</v>
       </c>
       <c r="K3">
         <v>100</v>
       </c>
-      <c r="M3">
+      <c r="L3">
+        <v>100</v>
+      </c>
+      <c r="N3">
         <v>500</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0.05</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>341</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>314</v>
@@ -4032,18 +4056,21 @@
         <v>315</v>
       </c>
       <c r="E4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F4" t="s">
         <v>200</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>201</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>174</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>10</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>0.9</v>
       </c>
     </row>
@@ -4460,111 +4487,114 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6619729E-584E-41E3-B72E-7B2979330C88}">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" customWidth="1"/>
-    <col min="19" max="20" width="10.140625" customWidth="1"/>
-    <col min="21" max="21" width="8" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" customWidth="1"/>
-    <col min="23" max="23" width="8" customWidth="1"/>
-    <col min="25" max="25" width="8.140625" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="11" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" customWidth="1"/>
+    <col min="20" max="21" width="10.140625" customWidth="1"/>
+    <col min="22" max="22" width="8" customWidth="1"/>
+    <col min="23" max="23" width="10.85546875" customWidth="1"/>
+    <col min="24" max="24" width="8" customWidth="1"/>
+    <col min="26" max="26" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>284</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1" t="s">
         <v>308</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>211</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>215</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>218</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>30</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>143</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>289</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>22</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>140</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>199</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>124</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>126</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>130</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>233</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>234</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>122</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
@@ -4572,70 +4602,73 @@
         <v>142</v>
       </c>
       <c r="C2" s="24" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="E2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="F2" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="G2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="H2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="I2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="J2" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="K2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="L2" s="24" t="s">
         <v>288</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="M2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="N2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="O2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="24" t="s">
+      <c r="P2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="Q2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="24" t="s">
+      <c r="R2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="S2" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="S2" s="24" t="s">
+      <c r="T2" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="T2" s="24" t="s">
+      <c r="U2" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="U2" s="24" t="s">
+      <c r="V2" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="V2" s="24" t="s">
+      <c r="W2" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="24" t="s">
+      <c r="X2" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -4643,35 +4676,38 @@
         <v>178</v>
       </c>
       <c r="C3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>201</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>217</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>100</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>150</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>1000</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0.08</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>30</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>0.4</v>
       </c>
-      <c r="R3" s="5"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="S3" s="5"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -4679,22 +4715,25 @@
         <v>179</v>
       </c>
       <c r="C4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" t="s">
         <v>309</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>201</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>174</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>100</v>
       </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -4702,18 +4741,21 @@
         <v>190</v>
       </c>
       <c r="C5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>201</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>174</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>200</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>0.5</v>
       </c>
     </row>
@@ -4885,8 +4927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5344,18 +5386,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C13F0C3-2BD2-4859-9713-8823A445C2E8}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="20" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
@@ -7880,7 +7922,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8543,162 +8585,168 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="14" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="14" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" style="14" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" customWidth="1"/>
-    <col min="18" max="18" width="10.140625" customWidth="1"/>
-    <col min="19" max="19" width="18.140625" customWidth="1"/>
-    <col min="20" max="20" width="14.85546875" customWidth="1"/>
+    <col min="3" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" style="14" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="14" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" style="14" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" customWidth="1"/>
+    <col min="20" max="20" width="18.140625" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>284</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1" t="s">
         <v>213</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>304</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>214</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>218</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>182</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>198</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>144</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>145</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>75</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>80</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>83</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>77</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>289</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>76</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>27</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>84</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="24" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="24" t="s">
+      <c r="P2" s="24" t="s">
         <v>288</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -8709,20 +8757,23 @@
         <v>187</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>307</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" t="s">
         <v>174</v>
-      </c>
-      <c r="I3">
-        <v>10000</v>
       </c>
       <c r="J3">
         <v>10000</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -8733,77 +8784,92 @@
         <v>187</v>
       </c>
       <c r="D4" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" t="s">
         <v>174</v>
-      </c>
-      <c r="I4">
-        <v>10000</v>
       </c>
       <c r="J4">
         <v>10000</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F5" t="s">
+      <c r="C5" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="G5" t="s">
         <v>174</v>
-      </c>
-      <c r="I5">
-        <v>10000</v>
       </c>
       <c r="J5">
         <v>10000</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="F6" t="s">
+      <c r="C6" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="G6" t="s">
         <v>174</v>
-      </c>
-      <c r="I6">
-        <v>10000</v>
       </c>
       <c r="J6">
         <v>10000</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>341</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" t="s">
         <v>187</v>
       </c>
       <c r="F7" t="s">
+        <v>187</v>
+      </c>
+      <c r="G7" t="s">
         <v>174</v>
-      </c>
-      <c r="I7">
-        <v>12000</v>
       </c>
       <c r="J7">
         <v>12000</v>
       </c>
       <c r="K7">
+        <v>12000</v>
+      </c>
+      <c r="L7">
         <v>20</v>
+      </c>
+      <c r="T7">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing issues with timeline and is_active
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72154BA2-4C36-461E-B1D8-5F76038ADCCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96629EFE-E31D-438C-ACD4-1626A568BA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="3" activeTab="20" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="12900" yWindow="0" windowWidth="22305" windowHeight="21000" tabRatio="1000" firstSheet="5" activeTab="5" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -1195,9 +1195,6 @@
     <t>primary</t>
   </si>
   <si>
-    <t>duration</t>
-  </si>
-  <si>
     <t>is_non_synchronous</t>
   </si>
   <si>
@@ -1216,9 +1213,6 @@
     <t>Changed 'is_synchronous' to 'is_non_synchronous' in unit_node_c. Also 'has_DC' to 'is_DC' in connection_c. Added 'penalty_non_synchronous' to group_c.</t>
   </si>
   <si>
-    <t xml:space="preserve"> is_active</t>
-  </si>
-  <si>
     <t>Whether the unit is present in the alternative.</t>
   </si>
   <si>
@@ -1226,6 +1220,12 @@
   </si>
   <si>
     <t>Battery</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>timestep_duration</t>
   </si>
 </sst>
 </file>
@@ -3632,7 +3632,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3888,7 +3888,7 @@
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F1" t="s">
         <v>210</v>
@@ -3950,7 +3950,7 @@
         <v>322</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>18</v>
@@ -3962,7 +3962,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>16</v>
@@ -4044,7 +4044,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>314</v>
@@ -4493,7 +4493,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:C2"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4528,7 +4528,7 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D1" t="s">
         <v>308</v>
@@ -4602,7 +4602,7 @@
         <v>142</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>123</v>
@@ -5112,7 +5112,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B15" s="25">
         <v>44635</v>
@@ -5121,7 +5121,7 @@
         <v>228</v>
       </c>
       <c r="D15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -5386,7 +5386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C13F0C3-2BD2-4859-9713-8823A445C2E8}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -5466,7 +5466,7 @@
         <v>19</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>127</v>
@@ -6735,7 +6735,7 @@
         <v>61</v>
       </c>
       <c r="J1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K1" t="s">
         <v>45</v>
@@ -6776,7 +6776,7 @@
         <v>60</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>44</v>
@@ -8089,11 +8089,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C14DBC-6D65-48AD-9110-D1593FB205E8}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8101,7 +8101,7 @@
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="13" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8126,7 +8126,7 @@
         <v>246</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8485,7 +8485,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8624,7 +8624,7 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D1" t="s">
         <v>213</v>
@@ -8689,7 +8689,7 @@
         <v>65</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>67</v>
@@ -8842,7 +8842,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>315</v>

</xml_diff>

<commit_message>
Changes to user constraints (and hopefully a working version of the workflow).
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E436FB2-135E-4989-ACDB-AB1A013C3639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA7B315-7C3F-4B1B-87ED-B7B210C9AF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="270" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="8" activeTab="18" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="27840" yWindow="1740" windowWidth="16950" windowHeight="16200" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -142,6 +142,8 @@
           </rPr>
           <t xml:space="preserve">Possible parameters
 efficiency: [factor] Efficiency of a unit. Constant or time.
+efficiency_at_min_load: [e.g. 0.4 means 40%] Efficiency of the unit at minimum load. Applies only if the unit has an online variable. Constant or time.
+min_load: [0-1] Minimum load of the unit. Applies only if the unit has an online variable. Constant or time.
 variable_cost: [CUR/MWh] Variable operating cost. Fuel and CO2 cost can be given through separate means. Constant or time.
 </t>
         </r>
@@ -200,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="353">
   <si>
     <t>commodity</t>
   </si>
@@ -553,12 +555,6 @@
     <t>timeline_duration_in_years</t>
   </si>
   <si>
-    <t>constraint_constant</t>
-  </si>
-  <si>
-    <t>[MW or MWh] A constant offset for user defined constraints. Constant.</t>
-  </si>
-  <si>
     <t>conversion_method</t>
   </si>
   <si>
@@ -568,9 +564,6 @@
     <t>efficiency_at_min_load</t>
   </si>
   <si>
-    <t>[e.g. 0.4 means 40%] Efficiency of the unit at minimum load. Applies only if the unit has an online variable. Constant.</t>
-  </si>
-  <si>
     <t>inertia_constant</t>
   </si>
   <si>
@@ -580,9 +573,6 @@
     <t>min_load</t>
   </si>
   <si>
-    <t>[0-1] Minimum load of the unit. Applies only if the unit has an online variable. Constant.</t>
-  </si>
-  <si>
     <t>min_uptime</t>
   </si>
   <si>
@@ -1108,9 +1098,6 @@
     <t>scale_to_annual_flow</t>
   </si>
   <si>
-    <t>Choice of conversion method (efficiency, operating_area, profile).</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -1238,6 +1225,42 @@
   </si>
   <si>
     <t>[MW] Minimum retired storage capacity. Period.</t>
+  </si>
+  <si>
+    <t>Choice of conversion method (none, constant_efficiency, part_load_efficiency). With 'none' there should be a source or a sink with constraints (e.g., wind power with a upper_limit using a profile).</t>
+  </si>
+  <si>
+    <t>constant_efficiency</t>
+  </si>
+  <si>
+    <t>min_load_efficiency</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>Changed 'conversion_method' called 'efficiency' to 'constant_efficiency' and added 'min_load_efficiency' as an option and removed 'operating_area' as an option (it can be implemented in addition to a conversion_method).</t>
+  </si>
+  <si>
+    <t>[e.g. 0.4 means 40%] Efficiency of the unit at minimum load. Applies only if the unit has an online variable. Constant or time.</t>
+  </si>
+  <si>
+    <t>[0-1] Minimum load of the unit. Applies only if the unit has an online variable. Constant or time.</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>Added 'efficiency_at_min_load' and 'min_load' to unit_t sheet.</t>
+  </si>
+  <si>
+    <t>Whether the constraint is active.</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t>Added 'is_active' choice for the user constraints</t>
   </si>
 </sst>
 </file>
@@ -1416,7 +1439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1507,6 +1530,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2856,9 +2882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2869,67 +2893,67 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
       <c r="E3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="E4" s="5" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="E5" s="5" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="29" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
@@ -2939,77 +2963,77 @@
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
       <c r="E8" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C10" s="32"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B14" s="32"/>
       <c r="C14" s="31" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B15" s="44"/>
       <c r="C15" s="44"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
@@ -3023,26 +3047,26 @@
       <c r="A18" s="39"/>
       <c r="B18" s="39"/>
       <c r="C18" s="40" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B19" s="45"/>
       <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
@@ -3054,45 +3078,45 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C23" s="34"/>
       <c r="D23" s="28"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B24" s="41"/>
       <c r="C24" s="41"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
@@ -3104,23 +3128,23 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="42"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B31" s="36"/>
       <c r="C31" s="35" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="42"/>
@@ -3204,7 +3228,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -3218,19 +3242,19 @@
         <v>76</v>
       </c>
       <c r="G1" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="H1" t="s">
         <v>78</v>
       </c>
       <c r="I1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="J1" t="s">
         <v>74</v>
       </c>
       <c r="K1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="L1" t="s">
         <v>22</v>
@@ -3268,13 +3292,13 @@
         <v>13</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>6</v>
@@ -3291,10 +3315,10 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D3">
         <f>3000*8760/24*1.1</f>
@@ -3330,7 +3354,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -3345,7 +3369,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>66</v>
@@ -3362,10 +3386,10 @@
         <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3663,14 +3687,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1"/>
       <c r="C1" t="s">
         <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3684,7 +3708,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3692,7 +3716,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C3">
         <v>0.34</v>
@@ -3706,7 +3730,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C4">
         <v>0.2</v>
@@ -3729,7 +3753,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3741,12 +3765,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3760,7 +3784,7 @@
         <v>35</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3768,7 +3792,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>86</v>
@@ -3782,7 +3806,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>87</v>
@@ -3796,10 +3820,10 @@
         <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D5">
         <v>22</v>
@@ -3848,18 +3872,18 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -3904,28 +3928,28 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="F1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="G1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="H1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="I1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="J1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="K1" t="s">
         <v>20</v>
@@ -3934,19 +3958,19 @@
         <v>24</v>
       </c>
       <c r="M1" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="N1" t="s">
         <v>27</v>
       </c>
       <c r="O1" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="P1" t="s">
         <v>38</v>
       </c>
       <c r="Q1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="R1" t="s">
         <v>22</v>
@@ -3972,13 +3996,13 @@
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -3990,7 +4014,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>15</v>
@@ -4008,13 +4032,13 @@
         <v>14</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>6</v>
@@ -4040,25 +4064,25 @@
         <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="H3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="K3">
         <v>100</v>
@@ -4078,28 +4102,28 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="H4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="K4">
         <v>10</v>
@@ -4146,7 +4170,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4154,19 +4178,19 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="F1" t="s">
         <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="H1" t="s">
         <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="J1" t="s">
         <v>22</v>
@@ -4198,13 +4222,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -4252,7 +4276,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -4287,7 +4311,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -4299,7 +4323,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
@@ -4521,7 +4545,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6619729E-584E-41E3-B72E-7B2979330C88}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -4534,7 +4558,8 @@
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -4553,31 +4578,29 @@
     <col min="20" max="20" width="9.85546875" customWidth="1"/>
     <col min="21" max="21" width="12.140625" customWidth="1"/>
     <col min="22" max="23" width="10.140625" customWidth="1"/>
-    <col min="24" max="24" width="8" customWidth="1"/>
-    <col min="25" max="25" width="9.7109375" customWidth="1"/>
-    <col min="26" max="26" width="8" customWidth="1"/>
-    <col min="28" max="28" width="8.140625" customWidth="1"/>
+    <col min="24" max="25" width="8" customWidth="1"/>
+    <col min="27" max="27" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D1" t="s">
-        <v>302</v>
+        <v>341</v>
       </c>
       <c r="E1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" t="s">
         <v>206</v>
       </c>
-      <c r="F1" t="s">
-        <v>210</v>
-      </c>
       <c r="G1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="H1" t="s">
         <v>20</v>
@@ -4586,19 +4609,19 @@
         <v>24</v>
       </c>
       <c r="J1" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="K1" t="s">
         <v>27</v>
       </c>
       <c r="L1" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="M1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="N1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="O1" t="s">
         <v>22</v>
@@ -4610,51 +4633,48 @@
         <v>21</v>
       </c>
       <c r="R1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="S1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="T1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="U1" t="s">
-        <v>122</v>
+        <v>346</v>
       </c>
       <c r="V1" t="s">
-        <v>126</v>
+        <v>347</v>
       </c>
       <c r="W1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="X1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="Y1" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E2" s="24" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G2" s="24" t="s">
         <v>11</v>
@@ -4672,13 +4692,13 @@
         <v>14</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="M2" s="24" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="O2" s="24" t="s">
         <v>6</v>
@@ -4699,42 +4719,40 @@
         <v>3</v>
       </c>
       <c r="U2" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="V2" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="W2" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="V2" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="W2" s="24" t="s">
-        <v>124</v>
-      </c>
       <c r="X2" s="24" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="Y2" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z2" s="24" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C3" t="s">
-        <v>182</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>196</v>
-      </c>
-      <c r="G3" t="s">
-        <v>211</v>
+        <v>169</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>342</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47" t="s">
+        <v>207</v>
       </c>
       <c r="H3">
         <v>100</v>
@@ -4756,24 +4774,25 @@
       </c>
       <c r="U3" s="5"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" t="s">
-        <v>182</v>
-      </c>
-      <c r="D4" t="s">
-        <v>303</v>
-      </c>
-      <c r="E4" t="s">
-        <v>196</v>
-      </c>
-      <c r="G4" t="s">
-        <v>169</v>
+        <v>170</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>192</v>
+      </c>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47" t="s">
+        <v>165</v>
       </c>
       <c r="H4">
         <v>100</v>
@@ -4782,30 +4801,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>196</v>
-      </c>
-      <c r="G5" t="s">
-        <v>169</v>
+        <v>181</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>343</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>192</v>
+      </c>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47" t="s">
+        <v>165</v>
       </c>
       <c r="H5">
         <v>200</v>
       </c>
       <c r="T5">
         <v>0.5</v>
+      </c>
+      <c r="U5">
+        <v>0.45</v>
+      </c>
+      <c r="V5">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -4820,11 +4846,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F519FEB-FCA9-4C11-88F7-D4EA23EF6482}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4846,7 +4872,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4854,7 +4880,7 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="F1" t="s">
         <v>26</v>
@@ -4863,10 +4889,10 @@
         <v>26</v>
       </c>
       <c r="H1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="J1" t="s">
         <v>22</v>
@@ -4878,7 +4904,7 @@
         <v>21</v>
       </c>
       <c r="M1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4886,7 +4912,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>35</v>
@@ -4901,13 +4927,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -4927,7 +4953,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>86</v>
@@ -4941,7 +4967,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>87</v>
@@ -4955,10 +4981,10 @@
         <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D5">
         <v>75</v>
@@ -4974,11 +5000,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4988,189 +5012,231 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B4" s="25">
         <v>44594</v>
       </c>
       <c r="C4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B5" s="25">
         <v>44595</v>
       </c>
       <c r="C5" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B6" s="25">
         <v>44600</v>
       </c>
       <c r="C6" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B7" s="25">
         <v>44602</v>
       </c>
       <c r="C7" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D7" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B8" s="25">
         <v>44602</v>
       </c>
       <c r="C8" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D8" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B9" s="25">
         <v>44602</v>
       </c>
       <c r="C9" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D9" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B10" s="25">
         <v>44602</v>
       </c>
       <c r="C10" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D10" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B11" s="25">
         <v>44603</v>
       </c>
       <c r="C11" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D11" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B12" s="25">
         <v>44605</v>
       </c>
       <c r="C12" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D12" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B13" s="25">
         <v>44605</v>
       </c>
       <c r="C13" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D13" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B14" s="25">
         <v>44605</v>
       </c>
       <c r="C14" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D14" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B15" s="25">
         <v>44635</v>
       </c>
       <c r="C15" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D15" t="s">
-        <v>330</v>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="B16" s="25">
+        <v>44643</v>
+      </c>
+      <c r="C16" t="s">
+        <v>218</v>
+      </c>
+      <c r="D16" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B17" s="25">
+        <v>44643</v>
+      </c>
+      <c r="C17" t="s">
+        <v>218</v>
+      </c>
+      <c r="D17" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B18" s="25">
+        <v>44643</v>
+      </c>
+      <c r="C18" t="s">
+        <v>218</v>
+      </c>
+      <c r="D18" t="s">
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -5186,7 +5252,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5199,7 +5265,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5211,7 +5277,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>18</v>
@@ -5222,10 +5288,10 @@
         <v>30</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -5439,7 +5505,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5462,34 +5528,34 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="H1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="I1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" t="s">
         <v>131</v>
-      </c>
-      <c r="J1" t="s">
-        <v>142</v>
-      </c>
-      <c r="K1" t="s">
-        <v>133</v>
-      </c>
-      <c r="L1" t="s">
-        <v>135</v>
       </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -5500,37 +5566,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>62</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>130</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>134</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -5541,19 +5607,19 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -5564,13 +5630,13 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -5584,13 +5650,13 @@
         <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -5601,13 +5667,13 @@
         <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -5621,19 +5687,19 @@
         <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -5665,7 +5731,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5677,7 +5743,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>18</v>
@@ -5686,10 +5752,10 @@
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -5698,7 +5764,7 @@
         <v>62</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -5706,10 +5772,10 @@
         <v>30</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -5934,7 +6000,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5954,16 +6020,16 @@
         <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -6330,12 +6396,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6346,10 +6412,10 @@
         <v>62</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -6363,13 +6429,13 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -6402,12 +6468,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6418,10 +6484,10 @@
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -6438,10 +6504,10 @@
         <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -6475,13 +6541,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -6489,16 +6555,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>62</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -6512,16 +6578,16 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -6534,13 +6600,13 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C017E3-B844-46CF-8B82-D76F5D9D7ACD}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6548,56 +6614,65 @@
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="4" customWidth="1"/>
-    <col min="4" max="8" width="11.5703125" customWidth="1"/>
+    <col min="4" max="9" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F1" s="3"/>
+        <v>350</v>
+      </c>
+      <c r="E1" t="s">
+        <v>176</v>
+      </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F2" s="3"/>
+        <v>329</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>175</v>
+      </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="D3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3">
         <v>0</v>
       </c>
     </row>
@@ -6617,7 +6692,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6633,14 +6708,14 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -6654,19 +6729,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>62</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -6680,16 +6755,16 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D3" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>199</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>203</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -6700,16 +6775,16 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F4">
         <v>-0.1</v>
@@ -6727,11 +6802,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6759,7 +6834,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -6784,7 +6859,7 @@
         <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="K1" t="s">
         <v>42</v>
@@ -6825,7 +6900,7 @@
         <v>57</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>41</v>
@@ -6842,7 +6917,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -6853,10 +6928,10 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F4">
         <v>200</v>
@@ -6865,7 +6940,7 @@
         <v>5000</v>
       </c>
       <c r="H4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I4">
         <v>0.6</v>
@@ -6907,15 +6982,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F1" t="s">
         <v>84</v>
@@ -6935,16 +7010,16 @@
         <v>35</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -6958,16 +7033,16 @@
         <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -6981,13 +7056,13 @@
         <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -7001,16 +7076,16 @@
         <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -7021,16 +7096,16 @@
         <v>37</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -7038,19 +7113,19 @@
         <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -7058,19 +7133,19 @@
         <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -7116,7 +7191,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7173,7 +7248,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>86</v>
@@ -7187,7 +7262,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>87</v>
@@ -7201,10 +7276,10 @@
         <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -7303,8 +7378,8 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7333,26 +7408,26 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -7381,7 +7456,7 @@
         <v>61</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -7420,7 +7495,7 @@
         <v>61</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>62</v>
@@ -7469,26 +7544,26 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -7502,10 +7577,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>29</v>
@@ -7514,19 +7589,19 @@
         <v>62</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -7569,19 +7644,19 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="F1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -7595,22 +7670,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>61</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -7624,16 +7699,16 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E3" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -7671,7 +7746,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -7680,13 +7755,13 @@
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="11" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -7700,7 +7775,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7863,26 +7938,26 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -7896,31 +7971,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>62</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -7934,19 +8009,19 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I3">
         <v>0.5</v>
@@ -7986,11 +8061,11 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -8001,7 +8076,7 @@
         <v>85</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -8021,10 +8096,10 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -8043,10 +8118,10 @@
         <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -8091,13 +8166,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>90</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8105,7 +8180,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
@@ -8119,7 +8194,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>32</v>
@@ -8156,12 +8231,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -8172,10 +8247,10 @@
         <v>113</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8547,7 +8622,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -8604,7 +8679,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>113</v>
@@ -8612,7 +8687,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>114</v>
@@ -8620,7 +8695,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>114</v>
@@ -8672,35 +8747,35 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="D1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" t="s">
         <v>208</v>
       </c>
-      <c r="E1" t="s">
-        <v>298</v>
-      </c>
-      <c r="F1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G1" t="s">
-        <v>212</v>
-      </c>
       <c r="H1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="J1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="K1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="L1" t="s">
         <v>72</v>
@@ -8709,19 +8784,19 @@
         <v>77</v>
       </c>
       <c r="N1" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="O1" t="s">
         <v>79</v>
       </c>
       <c r="P1" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="Q1" t="s">
         <v>74</v>
       </c>
       <c r="R1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="S1" t="s">
         <v>22</v>
@@ -8747,13 +8822,13 @@
         <v>62</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>64</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>65</v>
@@ -8786,13 +8861,13 @@
         <v>14</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="R2" s="24" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="S2" s="9" t="s">
         <v>6</v>
@@ -8815,20 +8890,20 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J3">
         <v>10000</v>
@@ -8842,20 +8917,20 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J4">
         <v>10000</v>
@@ -8869,13 +8944,13 @@
         <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J5">
         <v>10000</v>
@@ -8889,13 +8964,13 @@
         <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J6">
         <v>10000</v>
@@ -8906,22 +8981,22 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J7">
         <v>12000</v>

</xml_diff>

<commit_message>
A bug in outputting results.
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B08AC6-14FA-4548-B8CE-3EEDD8421E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3455FC-D52A-4D8F-BD11-FCE4BAB48B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="0" windowWidth="22305" windowHeight="21000" tabRatio="1000" firstSheet="7" activeTab="18" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="1185" yWindow="90" windowWidth="22305" windowHeight="21000" tabRatio="1000" activeTab="2" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="358">
   <si>
     <t>commodity</t>
   </si>
@@ -1274,10 +1274,7 @@
     <t>only_invest</t>
   </si>
   <si>
-    <t>Alternative</t>
-  </si>
-  <si>
-    <t>Following alternative</t>
+    <t>alternatives in order</t>
   </si>
 </sst>
 </file>
@@ -2899,9 +2896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4896,11 +4891,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6619729E-584E-41E3-B72E-7B2979330C88}">
   <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7150,88 +7145,103 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6AC2C8-7B82-4BFA-94A3-ECFAF63F0D5D}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>352</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>357</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="14"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>353</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="14" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="14" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>354</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>326</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B8" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>355</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Scenarios can be imported from Excel input
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3455FC-D52A-4D8F-BD11-FCE4BAB48B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2754D57-2ADB-4CCA-9BD7-69C91197303F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="90" windowWidth="22305" windowHeight="21000" tabRatio="1000" activeTab="2" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" activeTab="2" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="367">
   <si>
     <t>commodity</t>
   </si>
@@ -1259,9 +1259,6 @@
     <t>linear</t>
   </si>
   <si>
-    <t>scenario_name</t>
-  </si>
-  <si>
     <t>Inertia</t>
   </si>
   <si>
@@ -1274,7 +1271,37 @@
     <t>only_invest</t>
   </si>
   <si>
-    <t>alternatives in order</t>
+    <t>alternative_1</t>
+  </si>
+  <si>
+    <t>base_alternative</t>
+  </si>
+  <si>
+    <t>alternative_2</t>
+  </si>
+  <si>
+    <t>alternative_3</t>
+  </si>
+  <si>
+    <t>alternative_4</t>
+  </si>
+  <si>
+    <t>alternative_5</t>
+  </si>
+  <si>
+    <t>alternative_6</t>
+  </si>
+  <si>
+    <t>alternative_7</t>
+  </si>
+  <si>
+    <t>alternative_8</t>
+  </si>
+  <si>
+    <t>Inv_bat</t>
+  </si>
+  <si>
+    <t>Scenario names</t>
   </si>
 </sst>
 </file>
@@ -4461,7 +4488,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>34</v>
@@ -4473,7 +4500,7 @@
         <v>166</v>
       </c>
       <c r="H5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -5170,13 +5197,13 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>168</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -7145,105 +7172,138 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6AC2C8-7B82-4BFA-94A3-ECFAF63F0D5D}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="9" customWidth="1"/>
+    <col min="2" max="21" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="D2" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>357</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="C3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="F4" t="s">
         <v>353</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="G4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="G5" t="s">
         <v>353</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>355</v>
-      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="B7" s="14"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="B9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="B11" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7403,7 +7463,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>314</v>
@@ -8174,7 +8234,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8556,7 +8616,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>36</v>
@@ -8567,7 +8627,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>181</v>
@@ -8578,7 +8638,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>37</v>
@@ -8589,7 +8649,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>224</v>

</xml_diff>

<commit_message>
Implemented cumulative flow limits
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F8BFDB-5068-4B11-864D-FC46F7D7FF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ACF9C4-5989-43BE-AD53-CEC1DBE90491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="1000" activeTab="29" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="377">
   <si>
     <t>commodity</t>
   </si>
@@ -782,15 +782,6 @@
     <t>parameter</t>
   </si>
   <si>
-    <t>source_sink</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>sink</t>
-  </si>
-  <si>
     <t>profile_method</t>
   </si>
   <si>
@@ -1304,22 +1295,43 @@
     <t>Scenario names</t>
   </si>
   <si>
-    <t>Limit_coal</t>
-  </si>
-  <si>
-    <t>Limit_flow</t>
-  </si>
-  <si>
-    <t>max_annual_flow</t>
-  </si>
-  <si>
-    <t>min_annual_flow</t>
-  </si>
-  <si>
-    <t>[MWh/a] Maximum cumulative annual flow for a group of connection_nodes and/or unit_nodes. Applied for each solve. Constant or period.</t>
-  </si>
-  <si>
-    <t>[MWh/a] Minimum cumulative annual flow for a group of connection_nodes and/or unit_nodes. Applied for each solve. Constant or period.</t>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>Changed scenario sheet outlay</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>Added 'max_cumulative_flow' and 'min_cumulative_flow' to group_c and group_p</t>
+  </si>
+  <si>
+    <t>input_output</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>max_cumulative_flow</t>
+  </si>
+  <si>
+    <t>min_cumulative_flow</t>
+  </si>
+  <si>
+    <t>[MW] Maximum average flow, which limits the cumulative flow for a group of connection_nodes and/or unit_nodes. The average value is multiplied by the model duration to get the cumulative limit (e.g. by 8760 if a single year is modelled). Applied for each solve. Constant or period.</t>
+  </si>
+  <si>
+    <t>[MW] Minimum average flow, which limits the cumulative flow for a group of connection_nodes and/or unit_nodes. The average value is multiplied by the model duration to get the cumulative limit (e.g. by 8760 if a single year is modelled). Applied for each solve. Constant or period.</t>
+  </si>
+  <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>Limit_fossil</t>
   </si>
 </sst>
 </file>
@@ -2939,9 +2951,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2952,305 +2964,313 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>236</v>
+        <v>375</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
-      <c r="E3" t="s">
-        <v>273</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
-      <c r="E4" s="5" t="s">
-        <v>274</v>
+      <c r="E4" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="E5" s="5" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>271</v>
-      </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="29" t="s">
-        <v>238</v>
-      </c>
+      <c r="A6" s="43" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
       <c r="E6" s="5" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
-        <v>239</v>
-      </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+      <c r="A7" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="E8" t="s">
-        <v>275</v>
-      </c>
+      <c r="A8" s="43" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>240</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>241</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>242</v>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="E9" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>244</v>
-      </c>
-      <c r="C10" s="32"/>
+        <v>238</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
-        <v>245</v>
-      </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
+      <c r="A11" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="C11" s="32"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>246</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>247</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>248</v>
-      </c>
+      <c r="A12" s="44" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
-        <v>265</v>
+        <v>243</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>266</v>
+        <v>244</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="C14" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="31" t="s">
-        <v>263</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="44" t="s">
-        <v>250</v>
-      </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
+      <c r="A15" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="31" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
+      <c r="A17" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40" t="s">
-        <v>249</v>
-      </c>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
-        <v>284</v>
-      </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="40" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
+      <c r="A22" s="45" t="s">
+        <v>297</v>
+      </c>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
-        <v>261</v>
-      </c>
-      <c r="B23" s="34" t="s">
-        <v>262</v>
-      </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="28"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="s">
-        <v>252</v>
-      </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
+      <c r="A24" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="C24" s="34"/>
+      <c r="D24" s="28"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
+      <c r="A29" s="41" t="s">
+        <v>253</v>
+      </c>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="42" t="s">
+        <v>254</v>
+      </c>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="B32" s="36"/>
+      <c r="C32" s="35" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="42" t="s">
         <v>257</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
-        <v>258</v>
-      </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="35" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="42" t="s">
-        <v>260</v>
-      </c>
-      <c r="B32" s="42"/>
-      <c r="C32" s="42"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A30" location="reserve_unit_node_c!A1" display="reserve_connection_node_c" xr:uid="{3F855114-4A57-4E0A-A766-0317F980F4BF}"/>
-    <hyperlink ref="A28" location="group_unit_node!A1" display="group_unit_node" xr:uid="{B7C2FCA3-F9B2-4C44-95E7-EE78C953ADDA}"/>
-    <hyperlink ref="A27" location="group_unit!A1" display="group_unit" xr:uid="{B05CA82D-DD0B-41C5-A4A2-737EB6D8AF37}"/>
-    <hyperlink ref="A26" location="group_node!A1" display="group_node" xr:uid="{920BB948-3B7C-488B-B8B1-7504F3D3AD1A}"/>
-    <hyperlink ref="A25" location="group_connection_node!A1" display="group_connection_node" xr:uid="{811FD465-B06B-4481-9ED6-DE1222C0D3DE}"/>
-    <hyperlink ref="A31" location="reserve_group_c!A1" display="reserve_group_c" xr:uid="{2CFA818C-9B6A-474B-8E40-2E804C4A9677}"/>
-    <hyperlink ref="C31" location="reserve_group_t!A1" display="reserve_group_t" xr:uid="{401EE982-2E1A-4DC0-A8C5-8E9B177FDA74}"/>
-    <hyperlink ref="A32" location="reserve_unit_node_c!A1" display="reserve_unit_node_c" xr:uid="{78371C66-B81A-4E9B-96E1-6659A71B0BF4}"/>
-    <hyperlink ref="A24" location="group_connection!A1" display="group_connection" xr:uid="{A00C70C1-5203-41C9-BCBD-CC42FCD43017}"/>
-    <hyperlink ref="A23" location="group_c!A1" display="group_c" xr:uid="{8516B270-11A5-45FE-B8AE-F8BD21CE42EE}"/>
-    <hyperlink ref="B23" location="group_p!A1" display="group_p" xr:uid="{24A5AB85-580D-4C07-9C0C-EF096DF9B6A4}"/>
-    <hyperlink ref="A16" location="unit_node_constraint_c!A1" display="unit_node_constraint_c" xr:uid="{E752EE81-721A-467B-A89A-558EAD27CD18}"/>
-    <hyperlink ref="A15" location="constraint_sense_c!A1" display="constraint_sense_c" xr:uid="{E3638194-ABA1-4B52-B562-9CB1B5A7326A}"/>
-    <hyperlink ref="A14" location="unit_node_c!A1" display="unit_node_c" xr:uid="{588C2786-F4D1-490C-8299-996C761D1B0B}"/>
-    <hyperlink ref="C14" location="unit_node_t!A1" display="unit_node_t" xr:uid="{848C3082-4242-4C02-A2C8-1DDCCECDDCE4}"/>
-    <hyperlink ref="A13" location="unit_c!A1" display="unit_c" xr:uid="{0B24F06D-DF0D-43E9-A754-3D573B0328ED}"/>
-    <hyperlink ref="B13" location="unit_p!A1" display="unit_p" xr:uid="{6B0EC5F5-0D3E-41BB-B4D8-64F5821432A7}"/>
-    <hyperlink ref="C13" location="unit_t!A1" display="unit_t" xr:uid="{563A1A91-8913-4B2F-8BA5-4D350923C03F}"/>
-    <hyperlink ref="C18" location="profile_t!A1" display="profile_t" xr:uid="{78412094-AA9A-4901-935D-64F3C1AC7206}"/>
-    <hyperlink ref="A12" location="connection_c!A1" display="connection_c" xr:uid="{03E6664B-5F07-4921-A88F-1CC8DA8E9FAE}"/>
-    <hyperlink ref="B12" location="connection_p!A1" display="connection_p" xr:uid="{46902093-FDC0-4939-BBFD-2D41FFBE0F05}"/>
-    <hyperlink ref="C12" location="connection_t!A1" display="connection_t" xr:uid="{5D63301C-ED60-425E-8FC0-334B75B4F98C}"/>
-    <hyperlink ref="A11" location="commodity_node!A1" display="commodity_node" xr:uid="{1A8DF925-BFFA-47C2-B595-2F06AACA43EF}"/>
-    <hyperlink ref="A10" location="commodity_c!A1" display="commodity_c" xr:uid="{37D28BB2-4F57-4EDF-A58D-D5D0B0DFCD29}"/>
-    <hyperlink ref="B10" location="commodity_p!A1" display="commodity_p" xr:uid="{B8974311-BDD6-456A-9C22-7DD64599915A}"/>
-    <hyperlink ref="A9" location="node_c!A1" display="node_c" xr:uid="{96541F46-A5D0-46A0-A7C5-61D6136DE6D8}"/>
-    <hyperlink ref="B9" location="node_p!A1" display="node_p" xr:uid="{AA8FF5EE-A7C6-4A42-B219-867295F74C98}"/>
-    <hyperlink ref="C9" location="node_t!A1" display="node_t" xr:uid="{10D2F31E-4A77-4C8D-A909-F30F7DA9A1B0}"/>
-    <hyperlink ref="A7" location="timeblockSet_timeline!A1" display="timeblockSet_timeline" xr:uid="{7E649E3B-8603-412B-85C7-55801419EDEB}"/>
-    <hyperlink ref="C6" location="timeline_t!A1" display="timeline_t" xr:uid="{0049663E-A2F9-49A0-A576-07D0A457655D}"/>
-    <hyperlink ref="A6" location="timeline_s!A1" display="timeline_s" xr:uid="{252B2493-68D2-4C5E-A6EA-89A71C7FBE09}"/>
+    <hyperlink ref="A31" location="reserve_unit_node_c!A1" display="reserve_connection_node_c" xr:uid="{3F855114-4A57-4E0A-A766-0317F980F4BF}"/>
+    <hyperlink ref="A29" location="group_unit_node!A1" display="group_unit_node" xr:uid="{B7C2FCA3-F9B2-4C44-95E7-EE78C953ADDA}"/>
+    <hyperlink ref="A28" location="group_unit!A1" display="group_unit" xr:uid="{B05CA82D-DD0B-41C5-A4A2-737EB6D8AF37}"/>
+    <hyperlink ref="A27" location="group_node!A1" display="group_node" xr:uid="{920BB948-3B7C-488B-B8B1-7504F3D3AD1A}"/>
+    <hyperlink ref="A26" location="group_connection_node!A1" display="group_connection_node" xr:uid="{811FD465-B06B-4481-9ED6-DE1222C0D3DE}"/>
+    <hyperlink ref="A32" location="reserve_group_c!A1" display="reserve_group_c" xr:uid="{2CFA818C-9B6A-474B-8E40-2E804C4A9677}"/>
+    <hyperlink ref="C32" location="reserve_group_t!A1" display="reserve_group_t" xr:uid="{401EE982-2E1A-4DC0-A8C5-8E9B177FDA74}"/>
+    <hyperlink ref="A33" location="reserve_unit_node_c!A1" display="reserve_unit_node_c" xr:uid="{78371C66-B81A-4E9B-96E1-6659A71B0BF4}"/>
+    <hyperlink ref="A25" location="group_connection!A1" display="group_connection" xr:uid="{A00C70C1-5203-41C9-BCBD-CC42FCD43017}"/>
+    <hyperlink ref="A24" location="group_c!A1" display="group_c" xr:uid="{8516B270-11A5-45FE-B8AE-F8BD21CE42EE}"/>
+    <hyperlink ref="B24" location="group_p!A1" display="group_p" xr:uid="{24A5AB85-580D-4C07-9C0C-EF096DF9B6A4}"/>
+    <hyperlink ref="A17" location="unit_node_constraint_c!A1" display="unit_node_constraint_c" xr:uid="{E752EE81-721A-467B-A89A-558EAD27CD18}"/>
+    <hyperlink ref="A16" location="constraint_sense_c!A1" display="constraint_sense_c" xr:uid="{E3638194-ABA1-4B52-B562-9CB1B5A7326A}"/>
+    <hyperlink ref="A15" location="unit_node_c!A1" display="unit_node_c" xr:uid="{588C2786-F4D1-490C-8299-996C761D1B0B}"/>
+    <hyperlink ref="C15" location="unit_node_t!A1" display="unit_node_t" xr:uid="{848C3082-4242-4C02-A2C8-1DDCCECDDCE4}"/>
+    <hyperlink ref="A14" location="unit_c!A1" display="unit_c" xr:uid="{0B24F06D-DF0D-43E9-A754-3D573B0328ED}"/>
+    <hyperlink ref="B14" location="unit_p!A1" display="unit_p" xr:uid="{6B0EC5F5-0D3E-41BB-B4D8-64F5821432A7}"/>
+    <hyperlink ref="C14" location="unit_t!A1" display="unit_t" xr:uid="{563A1A91-8913-4B2F-8BA5-4D350923C03F}"/>
+    <hyperlink ref="C19" location="profile_t!A1" display="profile_t" xr:uid="{78412094-AA9A-4901-935D-64F3C1AC7206}"/>
+    <hyperlink ref="A13" location="connection_c!A1" display="connection_c" xr:uid="{03E6664B-5F07-4921-A88F-1CC8DA8E9FAE}"/>
+    <hyperlink ref="B13" location="connection_p!A1" display="connection_p" xr:uid="{46902093-FDC0-4939-BBFD-2D41FFBE0F05}"/>
+    <hyperlink ref="C13" location="connection_t!A1" display="connection_t" xr:uid="{5D63301C-ED60-425E-8FC0-334B75B4F98C}"/>
+    <hyperlink ref="A12" location="commodity_node!A1" display="commodity_node" xr:uid="{1A8DF925-BFFA-47C2-B595-2F06AACA43EF}"/>
+    <hyperlink ref="A11" location="commodity_c!A1" display="commodity_c" xr:uid="{37D28BB2-4F57-4EDF-A58D-D5D0B0DFCD29}"/>
+    <hyperlink ref="B11" location="commodity_p!A1" display="commodity_p" xr:uid="{B8974311-BDD6-456A-9C22-7DD64599915A}"/>
+    <hyperlink ref="A10" location="node_c!A1" display="node_c" xr:uid="{96541F46-A5D0-46A0-A7C5-61D6136DE6D8}"/>
+    <hyperlink ref="B10" location="node_p!A1" display="node_p" xr:uid="{AA8FF5EE-A7C6-4A42-B219-867295F74C98}"/>
+    <hyperlink ref="C10" location="node_t!A1" display="node_t" xr:uid="{10D2F31E-4A77-4C8D-A909-F30F7DA9A1B0}"/>
+    <hyperlink ref="A8" location="timeblockSet_timeline!A1" display="timeblockSet_timeline" xr:uid="{7E649E3B-8603-412B-85C7-55801419EDEB}"/>
+    <hyperlink ref="C7" location="timeline_t!A1" display="timeline_t" xr:uid="{0049663E-A2F9-49A0-A576-07D0A457655D}"/>
+    <hyperlink ref="A7" location="timeline_s!A1" display="timeline_s" xr:uid="{252B2493-68D2-4C5E-A6EA-89A71C7FBE09}"/>
     <hyperlink ref="A2" location="version!A1" display="version" xr:uid="{5528FB5D-B49F-4A94-B79B-BD7CACBF6421}"/>
-    <hyperlink ref="A20" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{BFEE1E54-8BED-43DB-81D7-EF22B030644E}"/>
-    <hyperlink ref="A21" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{F130C8C0-C1F9-49C3-9475-FD4618C13C76}"/>
-    <hyperlink ref="A19" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{844403FD-DCCB-46C7-BE3C-C68DCAAB6B04}"/>
-    <hyperlink ref="A19:C19" location="node_profile_c!A1" display="node_profile_c" xr:uid="{826B47E5-87EB-412A-A0AE-C49CDB5CEB93}"/>
-    <hyperlink ref="A20:C20" location="connection_profile_c!A1" display="connection_profile_c" xr:uid="{DB781E38-3ACC-4F21-8D1E-B47D2A016C51}"/>
-    <hyperlink ref="A21:C21" location="unit_node_profile_c!A1" display="unit_profile_c" xr:uid="{B2BA97AF-8BE5-4D5F-8341-41044F5963AA}"/>
-    <hyperlink ref="A3" location="solve_period!A1" display="solve_period" xr:uid="{1A642A0E-886B-4C5F-9459-AF06B635D1C8}"/>
-    <hyperlink ref="A4" location="solve_sequence!A1" display="solve_sequence" xr:uid="{3B08721C-A5BF-4AD9-9840-41F099D6F77C}"/>
-    <hyperlink ref="A5" location="timeblockSet!A1" display="timeblockSet" xr:uid="{4C69C415-5F99-4696-8AE3-CE2F554DC3A9}"/>
+    <hyperlink ref="A21" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{BFEE1E54-8BED-43DB-81D7-EF22B030644E}"/>
+    <hyperlink ref="A22" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{F130C8C0-C1F9-49C3-9475-FD4618C13C76}"/>
+    <hyperlink ref="A20" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{844403FD-DCCB-46C7-BE3C-C68DCAAB6B04}"/>
+    <hyperlink ref="A20:C20" location="node_profile_c!A1" display="node_profile_c" xr:uid="{826B47E5-87EB-412A-A0AE-C49CDB5CEB93}"/>
+    <hyperlink ref="A21:C21" location="connection_profile_c!A1" display="connection_profile_c" xr:uid="{DB781E38-3ACC-4F21-8D1E-B47D2A016C51}"/>
+    <hyperlink ref="A22:C22" location="unit_node_profile_c!A1" display="unit_profile_c" xr:uid="{B2BA97AF-8BE5-4D5F-8341-41044F5963AA}"/>
+    <hyperlink ref="A4" location="solve_period!A1" display="solve_period" xr:uid="{1A642A0E-886B-4C5F-9459-AF06B635D1C8}"/>
+    <hyperlink ref="A5" location="solve_sequence!A1" display="solve_sequence" xr:uid="{3B08721C-A5BF-4AD9-9840-41F099D6F77C}"/>
+    <hyperlink ref="A6" location="timeblockSet!A1" display="timeblockSet" xr:uid="{4C69C415-5F99-4696-8AE3-CE2F554DC3A9}"/>
+    <hyperlink ref="A3" location="scenario!B3" display="scenario" xr:uid="{6595CB33-4050-4638-93A2-B2C50D1ED6D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -3297,23 +3317,23 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" t="s">
         <v>203</v>
-      </c>
-      <c r="E1" t="s">
-        <v>292</v>
-      </c>
-      <c r="F1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G1" t="s">
-        <v>206</v>
       </c>
       <c r="H1" t="s">
         <v>172</v>
@@ -3334,19 +3354,19 @@
         <v>77</v>
       </c>
       <c r="N1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="O1" t="s">
         <v>79</v>
       </c>
       <c r="P1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="Q1" t="s">
         <v>74</v>
       </c>
       <c r="R1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="S1" t="s">
         <v>22</v>
@@ -3372,13 +3392,13 @@
         <v>62</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>64</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>65</v>
@@ -3411,13 +3431,13 @@
         <v>14</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="R2" s="24" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S2" s="9" t="s">
         <v>6</v>
@@ -3449,7 +3469,7 @@
         <v>177</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" t="s">
@@ -3476,7 +3496,7 @@
         <v>177</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" t="s">
@@ -3531,10 +3551,10 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>177</v>
@@ -3600,7 +3620,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -3614,19 +3634,19 @@
         <v>76</v>
       </c>
       <c r="G1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="H1" t="s">
         <v>78</v>
       </c>
       <c r="I1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="J1" t="s">
         <v>74</v>
       </c>
       <c r="K1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="L1" t="s">
         <v>22</v>
@@ -3664,13 +3684,13 @@
         <v>13</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>6</v>
@@ -3690,7 +3710,7 @@
         <v>165</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D3">
         <f>3000*8760/24*1.1</f>
@@ -3726,7 +3746,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -4059,7 +4079,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1"/>
       <c r="C1" t="s">
@@ -4137,7 +4157,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -4195,7 +4215,7 @@
         <v>179</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D5">
         <v>22</v>
@@ -4300,25 +4320,25 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="J1" t="s">
         <v>189</v>
@@ -4330,19 +4350,19 @@
         <v>24</v>
       </c>
       <c r="M1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="N1" t="s">
         <v>27</v>
       </c>
       <c r="O1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="P1" t="s">
         <v>38</v>
       </c>
       <c r="Q1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="R1" t="s">
         <v>22</v>
@@ -4368,13 +4388,13 @@
         <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -4386,7 +4406,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>15</v>
@@ -4404,13 +4424,13 @@
         <v>14</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>6</v>
@@ -4474,16 +4494,16 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>165</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E4" t="s">
         <v>177</v>
@@ -4506,7 +4526,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>34</v>
@@ -4518,7 +4538,7 @@
         <v>166</v>
       </c>
       <c r="H5" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -4559,7 +4579,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4567,19 +4587,19 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F1" t="s">
         <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H1" t="s">
         <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="J1" t="s">
         <v>22</v>
@@ -4611,13 +4631,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -4665,7 +4685,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -4700,7 +4720,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -4940,7 +4960,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4972,23 +4992,23 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H1" t="s">
         <v>20</v>
@@ -4997,19 +5017,19 @@
         <v>24</v>
       </c>
       <c r="J1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="K1" t="s">
         <v>27</v>
       </c>
       <c r="L1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="M1" t="s">
         <v>134</v>
       </c>
       <c r="N1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O1" t="s">
         <v>22</v>
@@ -5027,16 +5047,16 @@
         <v>118</v>
       </c>
       <c r="T1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="U1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="V1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="W1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="X1" t="s">
         <v>132</v>
@@ -5050,7 +5070,7 @@
         <v>133</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>117</v>
@@ -5077,13 +5097,13 @@
         <v>14</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="M2" s="24" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="O2" s="24" t="s">
         <v>6</v>
@@ -5127,7 +5147,7 @@
         <v>177</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E3" s="47" t="s">
         <v>191</v>
@@ -5167,7 +5187,7 @@
         <v>177</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E4" s="47" t="s">
         <v>191</v>
@@ -5194,10 +5214,10 @@
         <v>177</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47" t="s">
@@ -5215,13 +5235,13 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>168</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -5234,9 +5254,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5246,231 +5268,259 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" t="s">
         <v>212</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>214</v>
-      </c>
-      <c r="C3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B4" s="25">
         <v>44594</v>
       </c>
       <c r="C4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B5" s="25">
         <v>44595</v>
       </c>
       <c r="C5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B6" s="25">
         <v>44600</v>
       </c>
       <c r="C6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B7" s="25">
         <v>44602</v>
       </c>
       <c r="C7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B8" s="25">
         <v>44602</v>
       </c>
       <c r="C8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B9" s="25">
         <v>44602</v>
       </c>
       <c r="C9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D9" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B10" s="25">
         <v>44602</v>
       </c>
       <c r="C10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D10" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B11" s="25">
         <v>44603</v>
       </c>
       <c r="C11" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B12" s="25">
         <v>44605</v>
       </c>
       <c r="C12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D12" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B13" s="25">
         <v>44605</v>
       </c>
       <c r="C13" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D13" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B14" s="25">
         <v>44605</v>
       </c>
       <c r="C14" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D14" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B15" s="25">
         <v>44635</v>
       </c>
       <c r="C15" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D15" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B16" s="25">
         <v>44643</v>
       </c>
       <c r="C16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D16" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B17" s="25">
         <v>44643</v>
       </c>
       <c r="C17" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D17" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B18" s="25">
         <v>44643</v>
       </c>
       <c r="C18" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D18" t="s">
-        <v>350</v>
+        <v>347</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="B19" s="25">
+        <v>44656</v>
+      </c>
+      <c r="C19" t="s">
+        <v>213</v>
+      </c>
+      <c r="D19" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="B20" s="25">
+        <v>44657</v>
+      </c>
+      <c r="C20" t="s">
+        <v>213</v>
+      </c>
+      <c r="D20" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -5508,7 +5558,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5516,7 +5566,7 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F1" t="s">
         <v>26</v>
@@ -5528,7 +5578,7 @@
         <v>134</v>
       </c>
       <c r="I1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J1" t="s">
         <v>22</v>
@@ -5563,13 +5613,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -5620,7 +5670,7 @@
         <v>168</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D5">
         <v>75</v>
@@ -5655,7 +5705,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5891,11 +5941,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C13F0C3-2BD2-4859-9713-8823A445C2E8}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5903,7 +5953,7 @@
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="20" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
     <col min="7" max="7" width="19.140625" customWidth="1"/>
@@ -5918,7 +5968,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5930,10 +5980,10 @@
         <v>160</v>
       </c>
       <c r="G1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="I1" t="s">
         <v>127</v>
@@ -5962,7 +6012,7 @@
         <v>62</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>193</v>
+        <v>368</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>156</v>
@@ -5971,7 +6021,7 @@
         <v>18</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>120</v>
@@ -6003,7 +6053,7 @@
         <v>167</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>194</v>
+        <v>369</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -6026,7 +6076,7 @@
         <v>165</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>195</v>
+        <v>370</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -6046,7 +6096,7 @@
         <v>178</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>194</v>
+        <v>369</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -6063,7 +6113,7 @@
         <v>166</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>195</v>
+        <v>370</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6083,7 +6133,7 @@
         <v>165</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>195</v>
+        <v>370</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -6114,14 +6164,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="17" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6162,10 +6212,10 @@
         <v>30</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>193</v>
+        <v>368</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>194</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -6416,10 +6466,10 @@
         <v>163</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -6778,20 +6828,20 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="7" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6805,7 +6855,7 @@
         <v>162</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -6819,13 +6869,13 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -6850,20 +6900,20 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="7" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6877,7 +6927,7 @@
         <v>162</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -6894,10 +6944,10 @@
         <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -6931,13 +6981,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -6954,7 +7004,7 @@
         <v>162</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -6977,7 +7027,7 @@
         <v>163</v>
       </c>
       <c r="E3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -7009,12 +7059,12 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E1" t="s">
         <v>175</v>
@@ -7037,7 +7087,7 @@
         <v>173</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>174</v>
@@ -7054,10 +7104,10 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D3" t="s">
         <v>177</v>
@@ -7082,7 +7132,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7090,7 +7140,7 @@
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="20" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" style="11" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="10" width="11.5703125" customWidth="1"/>
@@ -7098,7 +7148,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7125,7 +7175,7 @@
         <v>62</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>193</v>
+        <v>368</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>161</v>
@@ -7151,10 +7201,10 @@
         <v>167</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>194</v>
+        <v>369</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -7171,10 +7221,10 @@
         <v>165</v>
       </c>
       <c r="D4" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>195</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>198</v>
       </c>
       <c r="F4">
         <v>-0.1</v>
@@ -7196,7 +7246,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7207,10 +7257,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7219,27 +7269,27 @@
         <v>31</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>31</v>
@@ -7265,70 +7315,70 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F4" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G4" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="H4" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B5" s="14"/>
       <c r="G5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B11" s="14"/>
     </row>
@@ -7344,11 +7394,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7366,7 +7416,7 @@
     <col min="11" max="11" width="10.42578125" customWidth="1"/>
     <col min="12" max="12" width="16.7109375" customWidth="1"/>
     <col min="13" max="13" width="15.7109375" customWidth="1"/>
-    <col min="14" max="15" width="16.85546875" customWidth="1"/>
+    <col min="14" max="15" width="20.85546875" customWidth="1"/>
     <col min="16" max="16" width="17.5703125" customWidth="1"/>
     <col min="17" max="17" width="22.42578125" customWidth="1"/>
     <col min="18" max="18" width="16.42578125" customWidth="1"/>
@@ -7375,7 +7425,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -7400,7 +7450,7 @@
         <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="K1" t="s">
         <v>42</v>
@@ -7412,10 +7462,10 @@
         <v>56</v>
       </c>
       <c r="N1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="O1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -7447,7 +7497,7 @@
         <v>57</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>41</v>
@@ -7459,10 +7509,10 @@
         <v>55</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -7481,7 +7531,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F4">
         <v>200</v>
@@ -7501,10 +7551,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E5" t="s">
         <v>177</v>
@@ -7512,10 +7562,13 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>368</v>
+        <v>376</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>368</v>
+        <v>376</v>
+      </c>
+      <c r="N6">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -7534,7 +7587,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1:K1048576"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7547,12 +7600,12 @@
     <col min="6" max="6" width="22.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" customWidth="1"/>
     <col min="8" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="11" width="17.42578125" customWidth="1"/>
+    <col min="10" max="11" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7575,10 +7628,10 @@
         <v>54</v>
       </c>
       <c r="J1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="K1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -7610,10 +7663,10 @@
         <v>53</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -7652,7 +7705,7 @@
         <v>171</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -7752,7 +7805,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7797,7 +7850,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>165</v>
@@ -7814,7 +7867,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7848,7 +7901,7 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8ED891B-8A85-405F-972C-9B1BFE92F9B9}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7882,6 +7935,28 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>166</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7917,14 +7992,14 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G1" t="s">
         <v>143</v>
@@ -7962,7 +8037,7 @@
         <v>62</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>142</v>
@@ -8017,13 +8092,13 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="F1" t="s">
         <v>152</v>
@@ -8072,16 +8147,16 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="E3" t="s">
         <v>313</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="E3" t="s">
-        <v>316</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -8119,7 +8194,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -8292,7 +8367,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8309,7 +8384,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -8337,16 +8412,16 @@
         <v>35</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>176</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -8423,7 +8498,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D6" t="s">
         <v>185</v>
@@ -8460,7 +8535,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>87</v>
@@ -8519,14 +8594,14 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G1" t="s">
         <v>143</v>
@@ -8564,7 +8639,7 @@
         <v>62</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>142</v>
@@ -8590,10 +8665,10 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>168</v>
@@ -8642,11 +8717,11 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -8674,7 +8749,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>36</v>
@@ -8685,7 +8760,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>181</v>
@@ -8696,7 +8771,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>37</v>
@@ -8707,10 +8782,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C7" t="s">
         <v>187</v>
@@ -8758,13 +8833,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>90</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8823,12 +8898,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -8839,10 +8914,10 @@
         <v>113</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -9214,7 +9289,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -9271,7 +9346,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
Fixed a bug by changing, the objective function sign for the 1way_1variable conversion processes.
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ACF9C4-5989-43BE-AD53-CEC1DBE90491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC70F9F-6953-4FC4-9EAD-AF1F7F9EC9DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" activeTab="1" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="379">
   <si>
     <t>commodity</t>
   </si>
@@ -1332,6 +1332,12 @@
   </si>
   <si>
     <t>Limit_fossil</t>
+  </si>
+  <si>
+    <t>11.0</t>
+  </si>
+  <si>
+    <t>Changed source and sink to input and output</t>
   </si>
 </sst>
 </file>
@@ -2953,7 +2959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5254,10 +5260,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5521,6 +5527,20 @@
       </c>
       <c r="D20" t="s">
         <v>367</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="B21" s="25">
+        <v>44657</v>
+      </c>
+      <c r="C21" t="s">
+        <v>213</v>
+      </c>
+      <c r="D21" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'output_results', 'max_peak_flow', 'min_peak_flow'
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC70F9F-6953-4FC4-9EAD-AF1F7F9EC9DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF542768-91EB-491E-B20D-F3849075EB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" activeTab="1" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35595" windowHeight="21000" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="390">
   <si>
     <t>commodity</t>
   </si>
@@ -1338,6 +1338,39 @@
   </si>
   <si>
     <t>Changed source and sink to input and output</t>
+  </si>
+  <si>
+    <t>Elec</t>
+  </si>
+  <si>
+    <t>A flag to output aggregated results for the group members.</t>
+  </si>
+  <si>
+    <t>output_results</t>
+  </si>
+  <si>
+    <t>max_peak_flow</t>
+  </si>
+  <si>
+    <t>min_peak_flow</t>
+  </si>
+  <si>
+    <t>[MW] Minimum instantenous flow for the aggregated flow of all group members. Constant or period.</t>
+  </si>
+  <si>
+    <t>[MW] Maximum instantenous flow for the aggregated flow of all group members. Constant or period.</t>
+  </si>
+  <si>
+    <t>Added 'max_peak_flow' and 'min_peak_flow_'to group_c and group_p</t>
+  </si>
+  <si>
+    <t>11.1</t>
+  </si>
+  <si>
+    <t>11.2</t>
+  </si>
+  <si>
+    <t>Added 'output_results' to group_c</t>
   </si>
 </sst>
 </file>
@@ -2959,7 +2992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4151,7 +4184,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4966,7 +4999,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5260,11 +5293,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5541,6 +5572,34 @@
       </c>
       <c r="D21" t="s">
         <v>378</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="B22" s="25">
+        <v>44680</v>
+      </c>
+      <c r="C22" t="s">
+        <v>213</v>
+      </c>
+      <c r="D22" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="B23" s="25">
+        <v>44680</v>
+      </c>
+      <c r="C23" t="s">
+        <v>213</v>
+      </c>
+      <c r="D23" t="s">
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -5965,7 +6024,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6986,7 +7045,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7066,7 +7125,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7266,7 +7325,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7412,83 +7471,93 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
-    <col min="14" max="15" width="20.85546875" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" customWidth="1"/>
-    <col min="17" max="17" width="22.42578125" customWidth="1"/>
-    <col min="18" max="18" width="16.42578125" customWidth="1"/>
-    <col min="19" max="23" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="16" width="20.85546875" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" customWidth="1"/>
+    <col min="20" max="24" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>269</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>60</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>48</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>58</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>319</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>42</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>52</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>56</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>373</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>385</v>
+      </c>
+      <c r="R1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -7496,99 +7565,122 @@
         <v>61</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q2" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>200</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>5000</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>177</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.6</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>5500</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>349</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>376</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>40</v>
+      </c>
+      <c r="Q6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C7" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -7601,7 +7693,7 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA54FD9A-FB2F-4111-AC75-F20843B34F53}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
@@ -7619,11 +7711,13 @@
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="11" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="11" width="20.85546875" customWidth="1"/>
+    <col min="12" max="13" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>269</v>
       </c>
@@ -7653,8 +7747,14 @@
       <c r="K1" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>385</v>
+      </c>
+      <c r="M1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -7688,8 +7788,14 @@
       <c r="K2" s="9" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -7703,7 +7809,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -7717,7 +7823,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -7821,11 +7927,11 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6F0B0-C8D9-4343-9EA4-859E87C9AF78}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7874,6 +7980,22 @@
       </c>
       <c r="B4" s="4" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -8387,7 +8509,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8722,7 +8844,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8841,7 +8963,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
+      <c r="A1" s="37" t="s">
+        <v>269</v>
+      </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
@@ -8891,6 +9015,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="navigate!A1" display="navigate" xr:uid="{7B79F92D-CA1F-4A9E-928C-D02457244CEB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed to input and output (instead of source and sink) also in the Toolbox DB
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF542768-91EB-491E-B20D-F3849075EB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF1B50C-A6FA-4139-8EE2-BB59945FBDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35595" windowHeight="21000" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -1349,12 +1349,6 @@
     <t>output_results</t>
   </si>
   <si>
-    <t>max_peak_flow</t>
-  </si>
-  <si>
-    <t>min_peak_flow</t>
-  </si>
-  <si>
     <t>[MW] Minimum instantenous flow for the aggregated flow of all group members. Constant or period.</t>
   </si>
   <si>
@@ -1371,6 +1365,12 @@
   </si>
   <si>
     <t>Added 'output_results' to group_c</t>
+  </si>
+  <si>
+    <t>max_instant_flow</t>
+  </si>
+  <si>
+    <t>min_instant_flow</t>
   </si>
 </sst>
 </file>
@@ -5576,7 +5576,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B22" s="25">
         <v>44680</v>
@@ -5585,12 +5585,12 @@
         <v>213</v>
       </c>
       <c r="D22" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B23" s="25">
         <v>44680</v>
@@ -5599,7 +5599,7 @@
         <v>213</v>
       </c>
       <c r="D23" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -7477,7 +7477,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7497,8 +7497,7 @@
     <col min="13" max="13" width="16.7109375" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" customWidth="1"/>
     <col min="15" max="16" width="20.85546875" customWidth="1"/>
-    <col min="17" max="17" width="15.140625" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" customWidth="1"/>
+    <col min="17" max="18" width="16.7109375" customWidth="1"/>
     <col min="19" max="19" width="16.42578125" customWidth="1"/>
     <col min="20" max="24" width="11.5703125" customWidth="1"/>
   </cols>
@@ -7551,10 +7550,10 @@
         <v>374</v>
       </c>
       <c r="Q1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="R1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -7607,10 +7606,10 @@
         <v>372</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -7637,9 +7636,6 @@
       <c r="H4">
         <v>5000</v>
       </c>
-      <c r="I4" t="s">
-        <v>177</v>
-      </c>
       <c r="J4">
         <v>0.6</v>
       </c>
@@ -7655,6 +7651,9 @@
         <v>311</v>
       </c>
       <c r="F5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I5" t="s">
         <v>177</v>
       </c>
     </row>
@@ -7714,7 +7713,7 @@
     <col min="8" max="8" width="18.85546875" customWidth="1"/>
     <col min="9" max="9" width="18.140625" customWidth="1"/>
     <col min="10" max="11" width="20.85546875" customWidth="1"/>
-    <col min="12" max="13" width="15.140625" customWidth="1"/>
+    <col min="12" max="13" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -7748,10 +7747,10 @@
         <v>374</v>
       </c>
       <c r="L1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -7789,10 +7788,10 @@
         <v>372</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -7931,7 +7930,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8009,7 +8008,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8216,7 +8215,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8323,7 +8322,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8509,7 +8508,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8844,7 +8843,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed issues with multiple inputs or outputs (zero coefficient did not work due to MathProg defaults where zero was translated to 1).
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF1B50C-A6FA-4139-8EE2-BB59945FBDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73CD0BD-DAD7-4A16-87B3-CC29A5AFE973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="393">
   <si>
     <t>commodity</t>
   </si>
@@ -1371,6 +1371,15 @@
   </si>
   <si>
     <t>min_instant_flow</t>
+  </si>
+  <si>
+    <t>[factor] The reserve is increased by the sum of demands from the group members multiplied by this ratio. Constant.</t>
+  </si>
+  <si>
+    <t>12.0</t>
+  </si>
+  <si>
+    <t>In 'unit_node_p' it is required to insert a number for the 'coefficient' (typically 1). Previously the default was 1, but that run into problems in MathProg.</t>
   </si>
 </sst>
 </file>
@@ -5293,9 +5302,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5600,6 +5611,20 @@
       </c>
       <c r="D23" t="s">
         <v>387</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="B24" s="25">
+        <v>44690</v>
+      </c>
+      <c r="C24" t="s">
+        <v>213</v>
+      </c>
+      <c r="D24" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -8115,7 +8140,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8215,7 +8240,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8227,7 +8252,7 @@
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
     <col min="9" max="12" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8247,6 +8272,9 @@
       <c r="G1" t="s">
         <v>150</v>
       </c>
+      <c r="H1" t="s">
+        <v>390</v>
+      </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -8276,6 +8304,9 @@
       <c r="G2" s="9" t="s">
         <v>149</v>
       </c>
+      <c r="H2" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -8304,6 +8335,9 @@
       </c>
       <c r="G3">
         <v>20000</v>
+      </c>
+      <c r="H3">
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix some problems with reserves (still not perfect, but better)
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BB970F-1449-4632-95A2-95031E61BF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745F0C12-253A-46F0-BF24-78D2AD51DD6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="26" activeTab="39" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="401">
   <si>
     <t>commodity</t>
   </si>
@@ -1395,6 +1395,15 @@
   </si>
   <si>
     <t>Changed investment, salvage and fixed costs to €/MW to CUR/kW. (In the model investment was treated as €/kW but fixed cost was €/MW - now they are both CUR/kW). Also all other instances of € were changed to CUR in the descriptions.</t>
+  </si>
+  <si>
+    <t>Reserve</t>
+  </si>
+  <si>
+    <t>Reserve_wind</t>
+  </si>
+  <si>
+    <t>Reserve_transfer</t>
   </si>
 </sst>
 </file>
@@ -3016,7 +3025,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3661,7 +3672,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4354,7 +4365,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6076,7 +6087,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7371,13 +7382,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6AC2C8-7B82-4BFA-94A3-ECFAF63F0D5D}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7386,7 +7397,7 @@
     <col min="2" max="21" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>255</v>
       </c>
@@ -7394,7 +7405,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="6" t="s">
         <v>29</v>
@@ -7417,8 +7428,17 @@
       <c r="H2" s="6" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>336</v>
       </c>
@@ -7443,8 +7463,17 @@
       <c r="H3" s="14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>335</v>
       </c>
@@ -7467,8 +7496,17 @@
       <c r="H4" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>398</v>
+      </c>
+      <c r="J4" t="s">
+        <v>398</v>
+      </c>
+      <c r="K4" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>337</v>
       </c>
@@ -7476,38 +7514,44 @@
       <c r="G5" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>399</v>
+      </c>
+      <c r="K5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>338</v>
       </c>
       <c r="B6" s="14"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>339</v>
       </c>
       <c r="B7" s="14"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>340</v>
       </c>
       <c r="B8" s="14"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>341</v>
       </c>
       <c r="B9" s="14"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>342</v>
       </c>
       <c r="B10" s="14"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>343</v>
       </c>
@@ -8161,7 +8205,7 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB87FF22-BB83-4D5E-B38D-455D581CF757}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
@@ -8250,6 +8294,32 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F3" t="s">
+        <v>163</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8343,7 +8413,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>398</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>298</v>
@@ -8771,18 +8841,18 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8C0D5E-7DB2-4BCF-8A8C-24C978AAECC4}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="11" customWidth="1"/>
@@ -8864,7 +8934,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>398</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>298</v>
@@ -8885,6 +8955,110 @@
         <v>0.5</v>
       </c>
       <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I5">
+        <v>0.01</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" t="s">
+        <v>163</v>
+      </c>
+      <c r="I6">
+        <v>0.5</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7">
+        <v>0.01</v>
+      </c>
+      <c r="J7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed an issue when running scenarios with different sets of periods
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745F0C12-253A-46F0-BF24-78D2AD51DD6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E9BBF5-9329-4F81-BF2D-5207FC327F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="26" activeTab="39" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="1000" activeTab="10" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="402">
   <si>
     <t>commodity</t>
   </si>
@@ -1404,6 +1404,9 @@
   </si>
   <si>
     <t>Reserve_transfer</t>
+  </si>
+  <si>
+    <t>y2020_4s</t>
   </si>
 </sst>
 </file>
@@ -3026,7 +3029,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3668,11 +3671,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51F2ED7-E82A-4D3D-A4CE-E6A52C2211BA}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4219,7 +4222,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4632,7 +4635,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7794,7 +7797,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8741,13 +8744,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>333</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>401</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
         <v>171</v>
@@ -8755,22 +8758,19 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" t="s">
-        <v>163</v>
-      </c>
       <c r="G5" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>333</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>401</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>209</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
         <v>171</v>
@@ -8784,7 +8784,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>333</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>167</v>
@@ -8804,26 +8804,63 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>333</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>207</v>
+        <v>35</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="5"/>
+      <c r="A9" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E14" s="16"/>
@@ -8843,11 +8880,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8C0D5E-7DB2-4BCF-8A8C-24C978AAECC4}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9078,7 +9115,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added solver choice to input file and DB
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E9BBF5-9329-4F81-BF2D-5207FC327F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7232B4-E792-4559-B14B-0FE8DD7CA96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="1000" activeTab="10" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-28920" yWindow="5145" windowWidth="29040" windowHeight="16440" tabRatio="1000" activeTab="1" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="406">
   <si>
     <t>commodity</t>
   </si>
@@ -1406,7 +1406,19 @@
     <t>Reserve_transfer</t>
   </si>
   <si>
-    <t>y2020_4s</t>
+    <t>solver</t>
+  </si>
+  <si>
+    <t>Choice of solver (highs, glpsol)</t>
+  </si>
+  <si>
+    <t>highs</t>
+  </si>
+  <si>
+    <t>13.1</t>
+  </si>
+  <si>
+    <t>Added solver option</t>
   </si>
 </sst>
 </file>
@@ -3028,9 +3040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3671,7 +3681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51F2ED7-E82A-4D3D-A4CE-E6A52C2211BA}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -5331,9 +5341,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5666,6 +5678,20 @@
       </c>
       <c r="D25" t="s">
         <v>397</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B26" s="25">
+        <v>44701</v>
+      </c>
+      <c r="C26" t="s">
+        <v>199</v>
+      </c>
+      <c r="D26" t="s">
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -8747,7 +8773,7 @@
         <v>333</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>401</v>
+        <v>34</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>79</v>
@@ -8767,7 +8793,7 @@
         <v>333</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>401</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>80</v>
@@ -9136,6 +9162,9 @@
       <c r="C1" t="s">
         <v>194</v>
       </c>
+      <c r="D1" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -9146,6 +9175,9 @@
       </c>
       <c r="C2" s="9" t="s">
         <v>172</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9158,6 +9190,9 @@
       <c r="C3" t="s">
         <v>81</v>
       </c>
+      <c r="D3" t="s">
+        <v>403</v>
+      </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9170,6 +9205,9 @@
       <c r="C4" t="s">
         <v>81</v>
       </c>
+      <c r="D4" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -9181,6 +9219,9 @@
       <c r="C5" t="s">
         <v>173</v>
       </c>
+      <c r="D5" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -9192,6 +9233,9 @@
       <c r="C6" t="s">
         <v>81</v>
       </c>
+      <c r="D6" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -9202,6 +9246,9 @@
       </c>
       <c r="C7" t="s">
         <v>173</v>
+      </c>
+      <c r="D7" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can choose solver between HiGHS (default) and glpsol
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7232B4-E792-4559-B14B-0FE8DD7CA96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF06AE8C-1E16-4AF6-B6F2-94FEF4BB9880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5145" windowWidth="29040" windowHeight="16440" tabRatio="1000" activeTab="1" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" activeTab="4" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="411">
   <si>
     <t>commodity</t>
   </si>
@@ -785,9 +785,6 @@
     <t>Map of timestep durations. Index: timestep name, value: duration of time step [in hours].</t>
   </si>
   <si>
-    <t>A choice of solve mode (invest, dispatch_single, dispatch_rolling)</t>
-  </si>
-  <si>
     <t>Version number</t>
   </si>
   <si>
@@ -1419,6 +1416,24 @@
   </si>
   <si>
     <t>Added solver option</t>
+  </si>
+  <si>
+    <t>Choice of solve mode (invest, dispatch_single, dispatch_rolling)</t>
+  </si>
+  <si>
+    <t>13.2</t>
+  </si>
+  <si>
+    <t>Added solver example</t>
+  </si>
+  <si>
+    <t>Solver</t>
+  </si>
+  <si>
+    <t>Solver_glpsol</t>
+  </si>
+  <si>
+    <t>glpsol</t>
   </si>
 </sst>
 </file>
@@ -3040,7 +3055,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3051,74 +3068,74 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>291</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>293</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="E4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="E5" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="E6" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="43"/>
@@ -3128,77 +3145,77 @@
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
       <c r="E9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="C10" s="31" t="s">
         <v>224</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>226</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>227</v>
       </c>
       <c r="C11" s="32"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>229</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="C13" s="31" t="s">
         <v>230</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
+        <v>247</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>248</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="C14" s="31" t="s">
         <v>249</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -3212,26 +3229,26 @@
       <c r="A19" s="39"/>
       <c r="B19" s="39"/>
       <c r="C19" s="40" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
@@ -3243,45 +3260,45 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="B24" s="34" t="s">
         <v>244</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>245</v>
       </c>
       <c r="C24" s="34"/>
       <c r="D24" s="28"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="41"/>
@@ -3293,23 +3310,23 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B32" s="36"/>
       <c r="C32" s="35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="42"/>
@@ -3372,7 +3389,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3404,17 +3421,17 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D1" t="s">
         <v>186</v>
       </c>
       <c r="E1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F1" t="s">
         <v>187</v>
@@ -3429,10 +3446,10 @@
         <v>174</v>
       </c>
       <c r="J1" t="s">
+        <v>374</v>
+      </c>
+      <c r="K1" t="s">
         <v>375</v>
-      </c>
-      <c r="K1" t="s">
-        <v>376</v>
       </c>
       <c r="L1" t="s">
         <v>68</v>
@@ -3441,25 +3458,25 @@
         <v>71</v>
       </c>
       <c r="N1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="O1" t="s">
         <v>72</v>
       </c>
       <c r="P1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q1" t="s">
+        <v>376</v>
+      </c>
+      <c r="R1" t="s">
         <v>377</v>
-      </c>
-      <c r="R1" t="s">
-        <v>378</v>
       </c>
       <c r="S1" t="s">
         <v>21</v>
       </c>
       <c r="T1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="U1" t="s">
         <v>24</v>
@@ -3479,13 +3496,13 @@
         <v>58</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>60</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>61</v>
@@ -3518,13 +3535,13 @@
         <v>14</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="R2" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="S2" s="9" t="s">
         <v>6</v>
@@ -3556,7 +3573,7 @@
         <v>163</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" t="s">
@@ -3583,7 +3600,7 @@
         <v>163</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" t="s">
@@ -3638,10 +3655,10 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>163</v>
@@ -3707,7 +3724,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -3721,19 +3738,19 @@
         <v>70</v>
       </c>
       <c r="G1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H1" t="s">
+        <v>379</v>
+      </c>
+      <c r="I1" t="s">
         <v>380</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>376</v>
+      </c>
+      <c r="K1" t="s">
         <v>381</v>
-      </c>
-      <c r="J1" t="s">
-        <v>377</v>
-      </c>
-      <c r="K1" t="s">
-        <v>382</v>
       </c>
       <c r="L1" t="s">
         <v>21</v>
@@ -3742,7 +3759,7 @@
         <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3771,13 +3788,13 @@
         <v>13</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>6</v>
@@ -3797,7 +3814,7 @@
         <v>151</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D3">
         <f>3000*8760/24*1.1</f>
@@ -3833,7 +3850,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -4166,14 +4183,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1"/>
       <c r="C1" t="s">
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4244,12 +4261,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4302,7 +4319,7 @@
         <v>165</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D5">
         <v>22</v>
@@ -4407,13 +4424,13 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F1" t="s">
         <v>183</v>
@@ -4437,19 +4454,19 @@
         <v>23</v>
       </c>
       <c r="M1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="N1" t="s">
         <v>26</v>
       </c>
       <c r="O1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P1" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q1" t="s">
         <v>385</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>386</v>
       </c>
       <c r="R1" t="s">
         <v>21</v>
@@ -4458,10 +4475,10 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
+        <v>386</v>
+      </c>
+      <c r="U1" t="s">
         <v>387</v>
-      </c>
-      <c r="U1" t="s">
-        <v>388</v>
       </c>
       <c r="V1" t="s">
         <v>19</v>
@@ -4475,13 +4492,13 @@
         <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>290</v>
-      </c>
       <c r="E2" s="24" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -4493,7 +4510,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>15</v>
@@ -4511,13 +4528,13 @@
         <v>14</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>6</v>
@@ -4581,16 +4598,16 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>151</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E4" t="s">
         <v>163</v>
@@ -4613,7 +4630,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>32</v>
@@ -4625,7 +4642,7 @@
         <v>152</v>
       </c>
       <c r="H5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -4666,7 +4683,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4674,19 +4691,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H1" t="s">
+        <v>384</v>
+      </c>
+      <c r="I1" t="s">
         <v>385</v>
-      </c>
-      <c r="I1" t="s">
-        <v>386</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -4695,7 +4712,7 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -4718,13 +4735,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -4772,7 +4789,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -4807,7 +4824,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5079,14 +5096,14 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E1" t="s">
         <v>184</v>
@@ -5104,19 +5121,19 @@
         <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K1" t="s">
         <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M1" t="s">
+        <v>388</v>
+      </c>
+      <c r="N1" t="s">
         <v>389</v>
-      </c>
-      <c r="N1" t="s">
-        <v>390</v>
       </c>
       <c r="O1" t="s">
         <v>21</v>
@@ -5125,7 +5142,7 @@
         <v>24</v>
       </c>
       <c r="Q1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="R1" t="s">
         <v>175</v>
@@ -5134,16 +5151,16 @@
         <v>111</v>
       </c>
       <c r="T1" t="s">
+        <v>322</v>
+      </c>
+      <c r="U1" t="s">
         <v>323</v>
       </c>
-      <c r="U1" t="s">
-        <v>324</v>
-      </c>
       <c r="V1" t="s">
+        <v>203</v>
+      </c>
+      <c r="W1" t="s">
         <v>204</v>
-      </c>
-      <c r="W1" t="s">
-        <v>205</v>
       </c>
       <c r="X1" t="s">
         <v>125</v>
@@ -5157,7 +5174,7 @@
         <v>126</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>110</v>
@@ -5184,13 +5201,13 @@
         <v>14</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M2" s="24" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O2" s="24" t="s">
         <v>6</v>
@@ -5234,7 +5251,7 @@
         <v>163</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E3" s="47" t="s">
         <v>177</v>
@@ -5274,7 +5291,7 @@
         <v>163</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E4" s="47" t="s">
         <v>177</v>
@@ -5301,10 +5318,10 @@
         <v>163</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47" t="s">
@@ -5322,13 +5339,13 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>154</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -5341,9 +5358,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -5355,343 +5372,357 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" t="s">
         <v>197</v>
       </c>
-      <c r="C3" t="s">
-        <v>198</v>
-      </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B4" s="25">
         <v>44594</v>
       </c>
       <c r="C4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B5" s="25">
         <v>44595</v>
       </c>
       <c r="C5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6" s="25">
         <v>44600</v>
       </c>
       <c r="C6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B7" s="25">
         <v>44602</v>
       </c>
       <c r="C7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B8" s="25">
         <v>44602</v>
       </c>
       <c r="C8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B9" s="25">
         <v>44602</v>
       </c>
       <c r="C9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B10" s="25">
         <v>44602</v>
       </c>
       <c r="C10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B11" s="25">
         <v>44603</v>
       </c>
       <c r="C11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B12" s="25">
         <v>44605</v>
       </c>
       <c r="C12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B13" s="25">
         <v>44605</v>
       </c>
       <c r="C13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B14" s="25">
         <v>44605</v>
       </c>
       <c r="C14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B15" s="25">
         <v>44635</v>
       </c>
       <c r="C15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B16" s="25">
         <v>44643</v>
       </c>
       <c r="C16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D16" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B17" s="25">
         <v>44643</v>
       </c>
       <c r="C17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B18" s="25">
         <v>44643</v>
       </c>
       <c r="C18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B19" s="25">
         <v>44656</v>
       </c>
       <c r="C19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B20" s="25">
         <v>44657</v>
       </c>
       <c r="C20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D20" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B21" s="25">
         <v>44657</v>
       </c>
       <c r="C21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D21" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B22" s="25">
         <v>44680</v>
       </c>
       <c r="C22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D22" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B23" s="25">
         <v>44680</v>
       </c>
       <c r="C23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B24" s="25">
         <v>44690</v>
       </c>
       <c r="C24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D24" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B25" s="25">
         <v>44695</v>
       </c>
       <c r="C25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D25" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B26" s="25">
         <v>44701</v>
       </c>
       <c r="C26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D26" t="s">
-        <v>405</v>
+        <v>404</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="B27" s="25">
+        <v>44701</v>
+      </c>
+      <c r="C27" t="s">
+        <v>198</v>
+      </c>
+      <c r="D27" t="s">
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -5729,7 +5760,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5737,19 +5768,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H1" t="s">
+        <v>388</v>
+      </c>
+      <c r="I1" t="s">
         <v>389</v>
-      </c>
-      <c r="I1" t="s">
-        <v>390</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -5758,7 +5789,7 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="M1" t="s">
         <v>175</v>
@@ -5784,13 +5815,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -5841,7 +5872,7 @@
         <v>154</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D5">
         <v>75</v>
@@ -5876,7 +5907,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6139,7 +6170,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6148,19 +6179,19 @@
         <v>145</v>
       </c>
       <c r="F1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I1" t="s">
         <v>120</v>
       </c>
       <c r="J1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K1" t="s">
         <v>122</v>
@@ -6183,7 +6214,7 @@
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>143</v>
@@ -6192,7 +6223,7 @@
         <v>18</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>113</v>
@@ -6224,7 +6255,7 @@
         <v>153</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -6247,7 +6278,7 @@
         <v>151</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -6267,7 +6298,7 @@
         <v>164</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -6284,7 +6315,7 @@
         <v>152</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6304,7 +6335,7 @@
         <v>151</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -6342,7 +6373,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6383,10 +6414,10 @@
         <v>28</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>349</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>350</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -6637,10 +6668,10 @@
         <v>149</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -7007,12 +7038,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7040,10 +7071,10 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>283</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>284</v>
       </c>
       <c r="D3" t="s">
         <v>180</v>
@@ -7079,12 +7110,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7115,7 +7146,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
         <v>180</v>
@@ -7152,13 +7183,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -7230,12 +7261,12 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E1" t="s">
         <v>161</v>
@@ -7258,7 +7289,7 @@
         <v>159</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>160</v>
@@ -7319,7 +7350,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7346,7 +7377,7 @@
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>147</v>
@@ -7372,7 +7403,7 @@
         <v>153</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>181</v>
@@ -7392,7 +7423,7 @@
         <v>151</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>181</v>
@@ -7411,13 +7442,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6AC2C8-7B82-4BFA-94A3-ECFAF63F0D5D}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7426,50 +7457,53 @@
     <col min="2" max="21" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>333</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>332</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="6" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>29</v>
@@ -7501,88 +7535,94 @@
       <c r="K3" s="14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="F4" t="s">
         <v>331</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>306</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>333</v>
-      </c>
-      <c r="F4" t="s">
-        <v>332</v>
-      </c>
       <c r="G4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K4" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+      <c r="L4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B5" s="14"/>
       <c r="G5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="J5" t="s">
+        <v>398</v>
+      </c>
+      <c r="K5" t="s">
         <v>399</v>
       </c>
-      <c r="K5" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>338</v>
       </c>
-      <c r="B6" s="14"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="B7" s="14"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="B7" s="14"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="B8" s="14"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="B9" s="14"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="B9" s="14"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>342</v>
-      </c>
-      <c r="B10" s="14"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>343</v>
       </c>
       <c r="B11" s="14"/>
     </row>
@@ -7629,11 +7669,11 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D1" t="s">
         <v>41</v>
@@ -7648,7 +7688,7 @@
         <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I1" t="s">
         <v>45</v>
@@ -7657,7 +7697,7 @@
         <v>55</v>
       </c>
       <c r="K1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="L1" t="s">
         <v>39</v>
@@ -7669,16 +7709,16 @@
         <v>53</v>
       </c>
       <c r="O1" t="s">
+        <v>354</v>
+      </c>
+      <c r="P1" t="s">
         <v>355</v>
       </c>
-      <c r="P1" t="s">
-        <v>356</v>
-      </c>
       <c r="Q1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="R1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -7689,7 +7729,7 @@
         <v>57</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>40</v>
@@ -7713,7 +7753,7 @@
         <v>54</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>38</v>
@@ -7725,16 +7765,16 @@
         <v>52</v>
       </c>
       <c r="O2" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="P2" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="P2" s="9" t="s">
-        <v>354</v>
-      </c>
       <c r="Q2" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="R2" s="9" t="s">
         <v>370</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -7753,7 +7793,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G4">
         <v>200</v>
@@ -7770,10 +7810,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F5" t="s">
         <v>163</v>
@@ -7784,10 +7824,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="O6">
         <v>40</v>
@@ -7801,7 +7841,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C7" t="s">
         <v>163</v>
@@ -7843,7 +7883,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7866,16 +7906,16 @@
         <v>51</v>
       </c>
       <c r="J1" t="s">
+        <v>354</v>
+      </c>
+      <c r="K1" t="s">
         <v>355</v>
       </c>
-      <c r="K1" t="s">
-        <v>356</v>
-      </c>
       <c r="L1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -7907,16 +7947,16 @@
         <v>50</v>
       </c>
       <c r="J2" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>354</v>
-      </c>
       <c r="L2" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>370</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -7955,7 +7995,7 @@
         <v>157</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -8100,7 +8140,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>151</v>
@@ -8108,7 +8148,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>151</v>
@@ -8116,7 +8156,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>152</v>
@@ -8204,7 +8244,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>154</v>
@@ -8215,7 +8255,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>166</v>
@@ -8258,7 +8298,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -8326,13 +8366,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>32</v>
@@ -8384,22 +8424,22 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F1" t="s">
         <v>139</v>
       </c>
       <c r="G1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -8442,19 +8482,19 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>295</v>
-      </c>
       <c r="E3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -8495,7 +8535,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -8685,7 +8725,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -8713,16 +8753,16 @@
         <v>33</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>162</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>211</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -8770,7 +8810,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>34</v>
@@ -8790,7 +8830,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
@@ -8810,7 +8850,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>167</v>
@@ -8830,7 +8870,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>35</v>
@@ -8850,13 +8890,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D9" t="s">
         <v>171</v>
@@ -8870,10 +8910,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>80</v>
@@ -8929,7 +8969,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -8997,13 +9037,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>154</v>
@@ -9023,13 +9063,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>155</v>
@@ -9049,13 +9089,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>154</v>
@@ -9075,13 +9115,13 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>166</v>
@@ -9101,13 +9141,13 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>154</v>
@@ -9135,9 +9175,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9640D032-37A5-47CC-8407-C4F7168BB93B}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -9156,14 +9196,14 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>194</v>
+        <v>405</v>
       </c>
       <c r="D1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -9177,7 +9217,7 @@
         <v>172</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9191,13 +9231,13 @@
         <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>34</v>
@@ -9206,12 +9246,12 @@
         <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>167</v>
@@ -9220,12 +9260,12 @@
         <v>173</v>
       </c>
       <c r="D5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>35</v>
@@ -9234,21 +9274,65 @@
         <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C7" t="s">
         <v>173</v>
       </c>
       <c r="D7" t="s">
-        <v>403</v>
+        <v>402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D11" t="s">
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -9282,7 +9366,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -9295,13 +9379,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>83</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -9363,7 +9447,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -9379,10 +9463,10 @@
         <v>106</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -9754,7 +9838,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -9811,7 +9895,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>106</v>

</xml_diff>

<commit_message>
Fixing an issue with multiple input/output units. They became online units by accident.
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF06AE8C-1E16-4AF6-B6F2-94FEF4BB9880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94DB579-8994-4AC3-A4B5-A94203A5C874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" activeTab="4" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="420">
   <si>
     <t>commodity</t>
   </si>
@@ -1028,9 +1028,6 @@
     <t>Changed 'has_inflow' in node to 'inflow_method'. This also changes what parameters are allowed in there.</t>
   </si>
   <si>
-    <t>scale_to_annual_flow</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -1434,6 +1431,36 @@
   </si>
   <si>
     <t>glpsol</t>
+  </si>
+  <si>
+    <t>scale_in_proportion</t>
+  </si>
+  <si>
+    <t>Gas_export</t>
+  </si>
+  <si>
+    <t>Gas_export_pump</t>
+  </si>
+  <si>
+    <t>gas_export</t>
+  </si>
+  <si>
+    <t>equal</t>
+  </si>
+  <si>
+    <t>lower_limit</t>
+  </si>
+  <si>
+    <t>13.3</t>
+  </si>
+  <si>
+    <t>Added an example with gas export and gas pump</t>
+  </si>
+  <si>
+    <t>Gas_export_node</t>
+  </si>
+  <si>
+    <t>Gas_export_profile</t>
   </si>
 </sst>
 </file>
@@ -1874,10 +1901,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="7486280" cy="650756"/>
     <xdr:sp macro="" textlink="">
@@ -1893,7 +1920,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3609975" y="571500"/>
+          <a:off x="4467225" y="638175"/>
           <a:ext cx="7486280" cy="650756"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3055,9 +3082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3068,13 +3093,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>291</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>290</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>292</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3086,7 +3111,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
@@ -3248,7 +3273,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
@@ -3383,13 +3408,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3425,7 +3450,7 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D1" t="s">
         <v>186</v>
@@ -3446,10 +3471,10 @@
         <v>174</v>
       </c>
       <c r="J1" t="s">
+        <v>373</v>
+      </c>
+      <c r="K1" t="s">
         <v>374</v>
-      </c>
-      <c r="K1" t="s">
-        <v>375</v>
       </c>
       <c r="L1" t="s">
         <v>68</v>
@@ -3458,25 +3483,25 @@
         <v>71</v>
       </c>
       <c r="N1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O1" t="s">
         <v>72</v>
       </c>
       <c r="P1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q1" t="s">
+        <v>375</v>
+      </c>
+      <c r="R1" t="s">
         <v>376</v>
-      </c>
-      <c r="R1" t="s">
-        <v>377</v>
       </c>
       <c r="S1" t="s">
         <v>21</v>
       </c>
       <c r="T1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="U1" t="s">
         <v>24</v>
@@ -3496,7 +3521,7 @@
         <v>58</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>60</v>
@@ -3535,7 +3560,7 @@
         <v>14</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>7</v>
@@ -3573,7 +3598,7 @@
         <v>163</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>275</v>
+        <v>410</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" t="s">
@@ -3655,10 +3680,10 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>163</v>
@@ -3683,6 +3708,29 @@
       </c>
       <c r="V7">
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" t="s">
+        <v>150</v>
+      </c>
+      <c r="J8">
+        <v>12000</v>
+      </c>
+      <c r="K8">
+        <v>12000</v>
+      </c>
+      <c r="L8">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -3738,19 +3786,19 @@
         <v>70</v>
       </c>
       <c r="G1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H1" t="s">
+        <v>378</v>
+      </c>
+      <c r="I1" t="s">
         <v>379</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>375</v>
+      </c>
+      <c r="K1" t="s">
         <v>380</v>
-      </c>
-      <c r="J1" t="s">
-        <v>376</v>
-      </c>
-      <c r="K1" t="s">
-        <v>381</v>
       </c>
       <c r="L1" t="s">
         <v>21</v>
@@ -3759,7 +3807,7 @@
         <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3788,7 +3836,7 @@
         <v>13</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
@@ -4190,7 +4238,7 @@
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4249,7 +4297,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4266,7 +4314,7 @@
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4395,7 +4443,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4430,7 +4478,7 @@
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F1" t="s">
         <v>183</v>
@@ -4454,19 +4502,19 @@
         <v>23</v>
       </c>
       <c r="M1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N1" t="s">
         <v>26</v>
       </c>
       <c r="O1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="P1" t="s">
+        <v>383</v>
+      </c>
+      <c r="Q1" t="s">
         <v>384</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>385</v>
       </c>
       <c r="R1" t="s">
         <v>21</v>
@@ -4475,10 +4523,10 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
+        <v>385</v>
+      </c>
+      <c r="U1" t="s">
         <v>386</v>
-      </c>
-      <c r="U1" t="s">
-        <v>387</v>
       </c>
       <c r="V1" t="s">
         <v>19</v>
@@ -4492,13 +4540,13 @@
         <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>289</v>
-      </c>
       <c r="E2" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -4510,7 +4558,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>15</v>
@@ -4528,7 +4576,7 @@
         <v>14</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
@@ -4598,16 +4646,16 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>151</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E4" t="s">
         <v>163</v>
@@ -4630,7 +4678,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>32</v>
@@ -4642,7 +4690,7 @@
         <v>152</v>
       </c>
       <c r="H5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -4691,19 +4739,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H1" t="s">
+        <v>383</v>
+      </c>
+      <c r="I1" t="s">
         <v>384</v>
-      </c>
-      <c r="I1" t="s">
-        <v>385</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -4712,7 +4760,7 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -4735,7 +4783,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
@@ -5058,13 +5106,13 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6619729E-584E-41E3-B72E-7B2979330C88}">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5100,10 +5148,10 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E1" t="s">
         <v>184</v>
@@ -5121,19 +5169,19 @@
         <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K1" t="s">
         <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M1" t="s">
+        <v>387</v>
+      </c>
+      <c r="N1" t="s">
         <v>388</v>
-      </c>
-      <c r="N1" t="s">
-        <v>389</v>
       </c>
       <c r="O1" t="s">
         <v>21</v>
@@ -5142,7 +5190,7 @@
         <v>24</v>
       </c>
       <c r="Q1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="R1" t="s">
         <v>175</v>
@@ -5151,10 +5199,10 @@
         <v>111</v>
       </c>
       <c r="T1" t="s">
+        <v>321</v>
+      </c>
+      <c r="U1" t="s">
         <v>322</v>
-      </c>
-      <c r="U1" t="s">
-        <v>323</v>
       </c>
       <c r="V1" t="s">
         <v>203</v>
@@ -5174,7 +5222,7 @@
         <v>126</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>110</v>
@@ -5201,7 +5249,7 @@
         <v>14</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M2" s="24" t="s">
         <v>7</v>
@@ -5251,7 +5299,7 @@
         <v>163</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E3" s="47" t="s">
         <v>177</v>
@@ -5291,7 +5339,7 @@
         <v>163</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E4" s="47" t="s">
         <v>177</v>
@@ -5318,10 +5366,10 @@
         <v>163</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47" t="s">
@@ -5339,13 +5387,39 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>154</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>333</v>
+        <v>332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>317</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="G7" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5358,10 +5432,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5503,7 +5577,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B12" s="25">
         <v>44605</v>
@@ -5512,12 +5586,12 @@
         <v>198</v>
       </c>
       <c r="D12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B13" s="25">
         <v>44605</v>
@@ -5526,12 +5600,12 @@
         <v>198</v>
       </c>
       <c r="D13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B14" s="25">
         <v>44605</v>
@@ -5540,12 +5614,12 @@
         <v>198</v>
       </c>
       <c r="D14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B15" s="25">
         <v>44635</v>
@@ -5554,12 +5628,12 @@
         <v>198</v>
       </c>
       <c r="D15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B16" s="25">
         <v>44643</v>
@@ -5568,12 +5642,12 @@
         <v>198</v>
       </c>
       <c r="D16" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B17" s="25">
         <v>44643</v>
@@ -5582,12 +5656,12 @@
         <v>198</v>
       </c>
       <c r="D17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B18" s="25">
         <v>44643</v>
@@ -5596,12 +5670,12 @@
         <v>198</v>
       </c>
       <c r="D18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B19" s="25">
         <v>44656</v>
@@ -5610,12 +5684,12 @@
         <v>198</v>
       </c>
       <c r="D19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B20" s="25">
         <v>44657</v>
@@ -5624,12 +5698,12 @@
         <v>198</v>
       </c>
       <c r="D20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B21" s="25">
         <v>44657</v>
@@ -5638,12 +5712,12 @@
         <v>198</v>
       </c>
       <c r="D21" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B22" s="25">
         <v>44680</v>
@@ -5652,12 +5726,12 @@
         <v>198</v>
       </c>
       <c r="D22" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B23" s="25">
         <v>44680</v>
@@ -5666,12 +5740,12 @@
         <v>198</v>
       </c>
       <c r="D23" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B24" s="25">
         <v>44690</v>
@@ -5680,12 +5754,12 @@
         <v>198</v>
       </c>
       <c r="D24" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B25" s="25">
         <v>44695</v>
@@ -5694,12 +5768,12 @@
         <v>198</v>
       </c>
       <c r="D25" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B26" s="25">
         <v>44701</v>
@@ -5708,12 +5782,12 @@
         <v>198</v>
       </c>
       <c r="D26" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B27" s="25">
         <v>44701</v>
@@ -5722,11 +5796,26 @@
         <v>198</v>
       </c>
       <c r="D27" t="s">
-        <v>407</v>
+        <v>406</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="B28" s="25">
+        <v>44712</v>
+      </c>
+      <c r="C28" t="s">
+        <v>198</v>
+      </c>
+      <c r="D28" t="s">
+        <v>417</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5738,7 +5827,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5768,19 +5857,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H1" t="s">
+        <v>387</v>
+      </c>
+      <c r="I1" t="s">
         <v>388</v>
-      </c>
-      <c r="I1" t="s">
-        <v>389</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -5789,7 +5878,7 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="M1" t="s">
         <v>175</v>
@@ -5815,7 +5904,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
@@ -6141,13 +6230,13 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C13F0C3-2BD2-4859-9713-8823A445C2E8}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6179,7 +6268,7 @@
         <v>145</v>
       </c>
       <c r="F1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G1" t="s">
         <v>261</v>
@@ -6191,7 +6280,7 @@
         <v>120</v>
       </c>
       <c r="J1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K1" t="s">
         <v>122</v>
@@ -6214,7 +6303,7 @@
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>143</v>
@@ -6223,7 +6312,7 @@
         <v>18</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>113</v>
@@ -6255,7 +6344,7 @@
         <v>153</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -6278,7 +6367,7 @@
         <v>151</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -6298,7 +6387,7 @@
         <v>164</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -6315,7 +6404,7 @@
         <v>152</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6335,13 +6424,64 @@
         <v>151</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6360,7 +6500,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6414,10 +6554,10 @@
         <v>28</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>348</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>349</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -6625,13 +6765,13 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE19B28-F2BE-409F-B1A6-1F5F2146177E}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6640,7 +6780,7 @@
     <col min="2" max="2" width="12" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>148</v>
       </c>
@@ -6656,8 +6796,11 @@
       <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>28</v>
       </c>
@@ -6668,13 +6811,16 @@
         <v>149</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -6687,8 +6833,11 @@
       <c r="E3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -6701,8 +6850,11 @@
       <c r="E4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>84</v>
       </c>
@@ -6715,8 +6867,11 @@
       <c r="E5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>85</v>
       </c>
@@ -6729,8 +6884,11 @@
       <c r="E6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>86</v>
       </c>
@@ -6743,8 +6901,11 @@
       <c r="E7">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>87</v>
       </c>
@@ -6757,8 +6918,11 @@
       <c r="E8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>88</v>
       </c>
@@ -6771,8 +6935,11 @@
       <c r="E9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>89</v>
       </c>
@@ -6785,8 +6952,11 @@
       <c r="E10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>90</v>
       </c>
@@ -6799,8 +6969,11 @@
       <c r="E11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>91</v>
       </c>
@@ -6813,8 +6986,11 @@
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>92</v>
       </c>
@@ -6827,8 +7003,11 @@
       <c r="E13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>93</v>
       </c>
@@ -6841,8 +7020,11 @@
       <c r="E14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>94</v>
       </c>
@@ -6855,8 +7037,11 @@
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>95</v>
       </c>
@@ -6869,8 +7054,11 @@
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>96</v>
       </c>
@@ -6883,8 +7071,11 @@
       <c r="E17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>97</v>
       </c>
@@ -6897,8 +7088,11 @@
       <c r="E18">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>98</v>
       </c>
@@ -6911,8 +7105,11 @@
       <c r="E19">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>99</v>
       </c>
@@ -6925,8 +7122,11 @@
       <c r="E20">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>100</v>
       </c>
@@ -6939,8 +7139,11 @@
       <c r="E21">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>101</v>
       </c>
@@ -6953,8 +7156,11 @@
       <c r="E22">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>102</v>
       </c>
@@ -6967,8 +7173,11 @@
       <c r="E23">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>103</v>
       </c>
@@ -6981,8 +7190,11 @@
       <c r="E24">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>104</v>
       </c>
@@ -6995,8 +7207,11 @@
       <c r="E25">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>105</v>
       </c>
@@ -7008,6 +7223,9 @@
       </c>
       <c r="E26">
         <v>0.5</v>
+      </c>
+      <c r="F26">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -7024,7 +7242,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7071,10 +7289,10 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>282</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>283</v>
       </c>
       <c r="D3" t="s">
         <v>180</v>
@@ -7146,7 +7364,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D3" t="s">
         <v>180</v>
@@ -7162,13 +7380,13 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1EE4BC-08B3-4CC5-9A8F-D2957036E873}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7232,6 +7450,23 @@
         <v>180</v>
       </c>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>418</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="E4" t="s">
+        <v>415</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="navigate!A1" display="navigate" xr:uid="{7BA55ECF-6A2F-4A56-B656-1811BDE72C64}"/>
@@ -7242,13 +7477,13 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C017E3-B844-46CF-8B82-D76F5D9D7ACD}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7266,7 +7501,7 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E1" t="s">
         <v>161</v>
@@ -7289,7 +7524,7 @@
         <v>159</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>160</v>
@@ -7315,6 +7550,23 @@
         <v>163</v>
       </c>
       <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="D4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4">
         <v>0</v>
       </c>
     </row>
@@ -7328,7 +7580,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA1124C-4BD2-46D2-BD33-99ED754CAC73}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
@@ -7377,7 +7629,7 @@
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>147</v>
@@ -7403,7 +7655,7 @@
         <v>153</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>181</v>
@@ -7423,13 +7675,53 @@
         <v>151</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>181</v>
       </c>
       <c r="F4">
         <v>-0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="F5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -7442,7 +7734,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6AC2C8-7B82-4BFA-94A3-ECFAF63F0D5D}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -7457,53 +7749,56 @@
     <col min="2" max="21" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>254</v>
       </c>
       <c r="B1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>331</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>399</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>29</v>
@@ -7538,91 +7833,97 @@
       <c r="L3" s="14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="F4" t="s">
         <v>330</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>305</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>332</v>
-      </c>
-      <c r="F4" t="s">
-        <v>331</v>
-      </c>
       <c r="G4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="L4" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+      <c r="M4" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B5" s="14"/>
       <c r="G5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="J5" t="s">
+        <v>397</v>
+      </c>
+      <c r="K5" t="s">
         <v>398</v>
       </c>
-      <c r="K5" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B6" s="14"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="B7" s="14"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>338</v>
       </c>
-      <c r="B7" s="14"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="B8" s="14"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="B9" s="14"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="B9" s="14"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>341</v>
-      </c>
-      <c r="B10" s="14"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>342</v>
       </c>
       <c r="B11" s="14"/>
     </row>
@@ -7673,7 +7974,7 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D1" t="s">
         <v>41</v>
@@ -7688,7 +7989,7 @@
         <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I1" t="s">
         <v>45</v>
@@ -7697,7 +7998,7 @@
         <v>55</v>
       </c>
       <c r="K1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="L1" t="s">
         <v>39</v>
@@ -7709,16 +8010,16 @@
         <v>53</v>
       </c>
       <c r="O1" t="s">
+        <v>353</v>
+      </c>
+      <c r="P1" t="s">
         <v>354</v>
       </c>
-      <c r="P1" t="s">
-        <v>355</v>
-      </c>
       <c r="Q1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -7729,7 +8030,7 @@
         <v>57</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>40</v>
@@ -7753,7 +8054,7 @@
         <v>54</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>38</v>
@@ -7765,16 +8066,16 @@
         <v>52</v>
       </c>
       <c r="O2" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="P2" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="P2" s="9" t="s">
-        <v>353</v>
-      </c>
       <c r="Q2" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="R2" s="9" t="s">
         <v>369</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -7793,7 +8094,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G4">
         <v>200</v>
@@ -7810,10 +8111,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F5" t="s">
         <v>163</v>
@@ -7824,10 +8125,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="O6">
         <v>40</v>
@@ -7841,7 +8142,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C7" t="s">
         <v>163</v>
@@ -7906,16 +8207,16 @@
         <v>51</v>
       </c>
       <c r="J1" t="s">
+        <v>353</v>
+      </c>
+      <c r="K1" t="s">
         <v>354</v>
       </c>
-      <c r="K1" t="s">
-        <v>355</v>
-      </c>
       <c r="L1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -7947,16 +8248,16 @@
         <v>50</v>
       </c>
       <c r="J2" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>353</v>
-      </c>
       <c r="L2" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>369</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -8140,7 +8441,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>151</v>
@@ -8148,7 +8449,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>151</v>
@@ -8156,7 +8457,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>152</v>
@@ -8244,7 +8545,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>154</v>
@@ -8255,7 +8556,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>166</v>
@@ -8366,13 +8667,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>32</v>
@@ -8430,16 +8731,16 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F1" t="s">
         <v>139</v>
       </c>
       <c r="G1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -8482,19 +8783,19 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>294</v>
-      </c>
       <c r="E3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -8708,7 +9009,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8810,7 +9111,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>34</v>
@@ -8830,7 +9131,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
@@ -8850,7 +9151,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>167</v>
@@ -8870,7 +9171,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>35</v>
@@ -8890,7 +9191,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>35</v>
@@ -8910,7 +9211,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>206</v>
@@ -9037,13 +9338,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>154</v>
@@ -9063,13 +9364,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>155</v>
@@ -9089,13 +9390,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>154</v>
@@ -9115,13 +9416,13 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>166</v>
@@ -9141,13 +9442,13 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>154</v>
@@ -9177,11 +9478,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9640D032-37A5-47CC-8407-C4F7168BB93B}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9200,10 +9501,10 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -9217,7 +9518,7 @@
         <v>172</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9231,13 +9532,13 @@
         <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>34</v>
@@ -9246,12 +9547,12 @@
         <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>167</v>
@@ -9260,12 +9561,12 @@
         <v>173</v>
       </c>
       <c r="D5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>35</v>
@@ -9274,12 +9575,12 @@
         <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>206</v>
@@ -9288,51 +9589,51 @@
         <v>173</v>
       </c>
       <c r="D7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>206</v>
       </c>
       <c r="D11" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -9466,7 +9767,7 @@
         <v>216</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding an option to use 'scale_in_proportion': will calculate a scaling factor from the division of 'annual_flow' and the sum of inflow time series (after it has been absoluted and annualized).
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94DB579-8994-4AC3-A4B5-A94203A5C874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FDBC58-89FF-423F-8538-93E74763F0E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="420">
   <si>
     <t>commodity</t>
   </si>
@@ -1016,12 +1016,6 @@
     <t>inflow_method</t>
   </si>
   <si>
-    <t>use_original</t>
-  </si>
-  <si>
-    <t>Choice how to treat inflow time series. Empty defaults to 'use_original', which does not scale the time series. 'no_inflow' ignores the inflow time series. 'scale_to_annual_flow' will scale the time series to match the 'annual_flow' when the sum of inflow is multiplied by 8760/'hours_in_solve'.</t>
-  </si>
-  <si>
     <t>5.0</t>
   </si>
   <si>
@@ -1461,6 +1455,12 @@
   </si>
   <si>
     <t>Gas_export_profile</t>
+  </si>
+  <si>
+    <t>scale_to_annual_flow</t>
+  </si>
+  <si>
+    <t>Choice how to treat inflow time series. Empty defaults to 'use_original', which does not scale the time series. 'no_inflow' ignores the inflow time series. 'scale_to_annual_flow' will scale the time series to match the 'annual_flow' so that the sum of inflow is multiplied by 8760/'hours_in_solve'. 'scale_in_proprotion' calculates a scaling factor by dividing 'annual_flow' with the sum of time series inflow (after it has been annualized using 'timeline_duration_in_years').</t>
   </si>
 </sst>
 </file>
@@ -3093,13 +3093,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
+        <v>287</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>289</v>
       </c>
-      <c r="B1" s="46" t="s">
-        <v>291</v>
-      </c>
       <c r="C1" s="46" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3111,7 +3111,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
@@ -3273,7 +3273,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
@@ -3414,7 +3414,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3450,13 +3450,13 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D1" t="s">
         <v>186</v>
       </c>
       <c r="E1" t="s">
-        <v>272</v>
+        <v>419</v>
       </c>
       <c r="F1" t="s">
         <v>187</v>
@@ -3471,10 +3471,10 @@
         <v>174</v>
       </c>
       <c r="J1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="K1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="L1" t="s">
         <v>68</v>
@@ -3483,25 +3483,25 @@
         <v>71</v>
       </c>
       <c r="N1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="O1" t="s">
         <v>72</v>
       </c>
       <c r="P1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Q1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="R1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="S1" t="s">
         <v>21</v>
       </c>
       <c r="T1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="U1" t="s">
         <v>24</v>
@@ -3521,7 +3521,7 @@
         <v>58</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>60</v>
@@ -3560,7 +3560,7 @@
         <v>14</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>7</v>
@@ -3598,7 +3598,7 @@
         <v>163</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>410</v>
+        <v>418</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" t="s">
@@ -3625,12 +3625,16 @@
         <v>163</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>271</v>
+        <v>408</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" t="s">
         <v>150</v>
       </c>
+      <c r="H4">
+        <f>100*8760</f>
+        <v>876000</v>
+      </c>
       <c r="J4">
         <v>10000</v>
       </c>
@@ -3680,10 +3684,10 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>163</v>
@@ -3712,10 +3716,10 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>163</v>
@@ -3744,13 +3748,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51F2ED7-E82A-4D3D-A4CE-E6A52C2211BA}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3786,19 +3790,19 @@
         <v>70</v>
       </c>
       <c r="G1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H1" t="s">
+        <v>376</v>
+      </c>
+      <c r="I1" t="s">
+        <v>377</v>
+      </c>
+      <c r="J1" t="s">
+        <v>373</v>
+      </c>
+      <c r="K1" t="s">
         <v>378</v>
-      </c>
-      <c r="I1" t="s">
-        <v>379</v>
-      </c>
-      <c r="J1" t="s">
-        <v>375</v>
-      </c>
-      <c r="K1" t="s">
-        <v>380</v>
       </c>
       <c r="L1" t="s">
         <v>21</v>
@@ -3807,7 +3811,7 @@
         <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3836,7 +3840,7 @@
         <v>13</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
@@ -3862,11 +3866,41 @@
         <v>151</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3">
+        <f>250*8760*0.9</f>
+        <v>1971000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4">
+        <f>250*8760*1</f>
+        <v>2190000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="D3">
-        <f>3000*8760/24*1.1</f>
-        <v>1204500</v>
+      <c r="D5">
+        <f>250*8760*1.1</f>
+        <v>2409000</v>
       </c>
     </row>
   </sheetData>
@@ -4238,7 +4272,7 @@
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4314,7 +4348,7 @@
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4478,7 +4512,7 @@
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F1" t="s">
         <v>183</v>
@@ -4502,19 +4536,19 @@
         <v>23</v>
       </c>
       <c r="M1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="N1" t="s">
         <v>26</v>
       </c>
       <c r="O1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="P1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="Q1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="R1" t="s">
         <v>21</v>
@@ -4523,10 +4557,10 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="U1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="V1" t="s">
         <v>19</v>
@@ -4540,13 +4574,13 @@
         <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -4558,7 +4592,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>15</v>
@@ -4576,7 +4610,7 @@
         <v>14</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
@@ -4646,16 +4680,16 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>151</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E4" t="s">
         <v>163</v>
@@ -4678,7 +4712,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>32</v>
@@ -4690,7 +4724,7 @@
         <v>152</v>
       </c>
       <c r="H5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -4739,19 +4773,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -4760,7 +4794,7 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -4783,7 +4817,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
@@ -5112,7 +5146,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5148,10 +5182,10 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E1" t="s">
         <v>184</v>
@@ -5169,19 +5203,19 @@
         <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="K1" t="s">
         <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="M1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="N1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="O1" t="s">
         <v>21</v>
@@ -5190,7 +5224,7 @@
         <v>24</v>
       </c>
       <c r="Q1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="R1" t="s">
         <v>175</v>
@@ -5199,10 +5233,10 @@
         <v>111</v>
       </c>
       <c r="T1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="U1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="V1" t="s">
         <v>203</v>
@@ -5222,7 +5256,7 @@
         <v>126</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>110</v>
@@ -5249,7 +5283,7 @@
         <v>14</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="M2" s="24" t="s">
         <v>7</v>
@@ -5299,7 +5333,7 @@
         <v>163</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E3" s="47" t="s">
         <v>177</v>
@@ -5339,7 +5373,7 @@
         <v>163</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E4" s="47" t="s">
         <v>177</v>
@@ -5366,10 +5400,10 @@
         <v>163</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47" t="s">
@@ -5387,27 +5421,27 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>154</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C7" s="47" t="s">
         <v>163</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E7" s="47" t="s">
         <v>177</v>
@@ -5563,7 +5597,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B11" s="25">
         <v>44603</v>
@@ -5572,12 +5606,12 @@
         <v>198</v>
       </c>
       <c r="D11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B12" s="25">
         <v>44605</v>
@@ -5586,12 +5620,12 @@
         <v>198</v>
       </c>
       <c r="D12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B13" s="25">
         <v>44605</v>
@@ -5600,12 +5634,12 @@
         <v>198</v>
       </c>
       <c r="D13" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B14" s="25">
         <v>44605</v>
@@ -5614,12 +5648,12 @@
         <v>198</v>
       </c>
       <c r="D14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B15" s="25">
         <v>44635</v>
@@ -5628,12 +5662,12 @@
         <v>198</v>
       </c>
       <c r="D15" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B16" s="25">
         <v>44643</v>
@@ -5642,12 +5676,12 @@
         <v>198</v>
       </c>
       <c r="D16" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B17" s="25">
         <v>44643</v>
@@ -5656,12 +5690,12 @@
         <v>198</v>
       </c>
       <c r="D17" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B18" s="25">
         <v>44643</v>
@@ -5670,12 +5704,12 @@
         <v>198</v>
       </c>
       <c r="D18" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B19" s="25">
         <v>44656</v>
@@ -5684,12 +5718,12 @@
         <v>198</v>
       </c>
       <c r="D19" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B20" s="25">
         <v>44657</v>
@@ -5698,12 +5732,12 @@
         <v>198</v>
       </c>
       <c r="D20" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B21" s="25">
         <v>44657</v>
@@ -5712,12 +5746,12 @@
         <v>198</v>
       </c>
       <c r="D21" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B22" s="25">
         <v>44680</v>
@@ -5726,12 +5760,12 @@
         <v>198</v>
       </c>
       <c r="D22" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B23" s="25">
         <v>44680</v>
@@ -5740,12 +5774,12 @@
         <v>198</v>
       </c>
       <c r="D23" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B24" s="25">
         <v>44690</v>
@@ -5754,12 +5788,12 @@
         <v>198</v>
       </c>
       <c r="D24" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B25" s="25">
         <v>44695</v>
@@ -5768,12 +5802,12 @@
         <v>198</v>
       </c>
       <c r="D25" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B26" s="25">
         <v>44701</v>
@@ -5782,12 +5816,12 @@
         <v>198</v>
       </c>
       <c r="D26" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B27" s="25">
         <v>44701</v>
@@ -5796,12 +5830,12 @@
         <v>198</v>
       </c>
       <c r="D27" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B28" s="25">
         <v>44712</v>
@@ -5810,7 +5844,7 @@
         <v>198</v>
       </c>
       <c r="D28" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -5857,19 +5891,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -5878,7 +5912,7 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M1" t="s">
         <v>175</v>
@@ -5904,7 +5938,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
@@ -6268,7 +6302,7 @@
         <v>145</v>
       </c>
       <c r="F1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G1" t="s">
         <v>261</v>
@@ -6280,7 +6314,7 @@
         <v>120</v>
       </c>
       <c r="J1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="K1" t="s">
         <v>122</v>
@@ -6303,7 +6337,7 @@
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>143</v>
@@ -6312,7 +6346,7 @@
         <v>18</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>113</v>
@@ -6344,7 +6378,7 @@
         <v>153</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -6367,7 +6401,7 @@
         <v>151</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -6387,7 +6421,7 @@
         <v>164</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -6404,7 +6438,7 @@
         <v>152</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6424,7 +6458,7 @@
         <v>151</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -6435,16 +6469,16 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>164</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -6452,16 +6486,16 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>151</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -6469,16 +6503,16 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -6554,10 +6588,10 @@
         <v>28</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -6797,7 +6831,7 @@
         <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6811,13 +6845,13 @@
         <v>149</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7289,10 +7323,10 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D3" t="s">
         <v>180</v>
@@ -7364,7 +7398,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D3" t="s">
         <v>180</v>
@@ -7455,16 +7489,16 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -7501,7 +7535,7 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E1" t="s">
         <v>161</v>
@@ -7524,7 +7558,7 @@
         <v>159</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>160</v>
@@ -7555,13 +7589,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>413</v>
-      </c>
       <c r="C4" s="4" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D4" t="s">
         <v>163</v>
@@ -7629,7 +7663,7 @@
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>147</v>
@@ -7655,7 +7689,7 @@
         <v>153</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>181</v>
@@ -7675,7 +7709,7 @@
         <v>151</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>181</v>
@@ -7686,19 +7720,19 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>164</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -7706,19 +7740,19 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>151</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -7754,7 +7788,7 @@
         <v>254</v>
       </c>
       <c r="B1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7763,42 +7797,42 @@
         <v>29</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>331</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>398</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>29</v>
@@ -7839,91 +7873,91 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>304</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>331</v>
-      </c>
       <c r="F4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="I4" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J4" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="K4" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="L4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="M4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B5" s="14"/>
       <c r="G5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="J5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B11" s="14"/>
     </row>
@@ -7974,7 +8008,7 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D1" t="s">
         <v>41</v>
@@ -7989,7 +8023,7 @@
         <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I1" t="s">
         <v>45</v>
@@ -7998,7 +8032,7 @@
         <v>55</v>
       </c>
       <c r="K1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L1" t="s">
         <v>39</v>
@@ -8010,16 +8044,16 @@
         <v>53</v>
       </c>
       <c r="O1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="P1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="Q1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="R1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -8030,7 +8064,7 @@
         <v>57</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>40</v>
@@ -8054,7 +8088,7 @@
         <v>54</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>38</v>
@@ -8066,16 +8100,16 @@
         <v>52</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -8094,7 +8128,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G4">
         <v>200</v>
@@ -8111,10 +8145,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F5" t="s">
         <v>163</v>
@@ -8125,10 +8159,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="O6">
         <v>40</v>
@@ -8142,7 +8176,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C7" t="s">
         <v>163</v>
@@ -8207,16 +8241,16 @@
         <v>51</v>
       </c>
       <c r="J1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="K1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="L1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -8248,16 +8282,16 @@
         <v>50</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -8441,7 +8475,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>151</v>
@@ -8449,7 +8483,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>151</v>
@@ -8457,7 +8491,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>152</v>
@@ -8545,7 +8579,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>154</v>
@@ -8556,7 +8590,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>166</v>
@@ -8667,13 +8701,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>32</v>
@@ -8731,16 +8765,16 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F1" t="s">
         <v>139</v>
       </c>
       <c r="G1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="H1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -8783,19 +8817,19 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D3" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" t="s">
         <v>293</v>
-      </c>
-      <c r="E3" t="s">
-        <v>295</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -9111,7 +9145,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>34</v>
@@ -9131,7 +9165,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
@@ -9151,7 +9185,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>167</v>
@@ -9171,7 +9205,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>35</v>
@@ -9191,7 +9225,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>35</v>
@@ -9211,7 +9245,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>206</v>
@@ -9338,13 +9372,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>154</v>
@@ -9364,13 +9398,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>155</v>
@@ -9390,13 +9424,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>154</v>
@@ -9416,13 +9450,13 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>166</v>
@@ -9442,13 +9476,13 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>154</v>
@@ -9501,10 +9535,10 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -9518,7 +9552,7 @@
         <v>172</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9532,13 +9566,13 @@
         <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>34</v>
@@ -9547,12 +9581,12 @@
         <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>167</v>
@@ -9561,12 +9595,12 @@
         <v>173</v>
       </c>
       <c r="D5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>35</v>
@@ -9575,12 +9609,12 @@
         <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>206</v>
@@ -9589,51 +9623,51 @@
         <v>173</v>
       </c>
       <c r="D7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>167</v>
       </c>
       <c r="D9" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>206</v>
       </c>
       <c r="D11" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -9767,7 +9801,7 @@
         <v>216</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding capacity margin constraint (and limiting node state to the storage capacity - which was missing)
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FDBC58-89FF-423F-8538-93E74763F0E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39E88DD-0044-4F03-95B6-4823CDED110E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="1000" activeTab="1" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="426">
   <si>
     <t>commodity</t>
   </si>
@@ -578,9 +578,6 @@
     <t>[per unit  / minute] Maximum ramp up speed. Constant.</t>
   </si>
   <si>
-    <t>[MW] Size of single unit - used for investments and some technical limits. If not provided, the sum of outputs from the unit is assumed. Constant.</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
@@ -1373,9 +1370,6 @@
     <t>[CUR/MWs] Penalty for violating the inertia constraint. Constant.</t>
   </si>
   <si>
-    <t>[CUR/MWh] Penalty for violating the non synchronous constraint. Constant.</t>
-  </si>
-  <si>
     <t>[CUR/MW] Penalty for violating a reserve constraint. Constant.</t>
   </si>
   <si>
@@ -1461,6 +1455,30 @@
   </si>
   <si>
     <t>Choice how to treat inflow time series. Empty defaults to 'use_original', which does not scale the time series. 'no_inflow' ignores the inflow time series. 'scale_to_annual_flow' will scale the time series to match the 'annual_flow' so that the sum of inflow is multiplied by 8760/'hours_in_solve'. 'scale_in_proprotion' calculates a scaling factor by dividing 'annual_flow' with the sum of time series inflow (after it has been annualized using 'timeline_duration_in_years').</t>
+  </si>
+  <si>
+    <t>max_relative_capacity</t>
+  </si>
+  <si>
+    <t>[MW] Size of single unit - used for investments and some technical limits. If not provided, existing capacity is assumed. Constant.</t>
+  </si>
+  <si>
+    <t>[factor, typically 0-1] Maximum input/output in relation to the capacity of the unit. Ignored if not provided (existing capacity will limit each output and [existing capacity/efficiency] will limit each input). Constant.</t>
+  </si>
+  <si>
+    <t>penalty_capacity_margin</t>
+  </si>
+  <si>
+    <t>[CUR/MWh] Penalty for violating the non synchronous constraint. Constant or period.</t>
+  </si>
+  <si>
+    <t>[CUR/MW] Penalty for violating the capacity margin constraint. Constant or period.</t>
+  </si>
+  <si>
+    <t>13.4</t>
+  </si>
+  <si>
+    <t>Added penalty for violating capacity margin</t>
   </si>
 </sst>
 </file>
@@ -3082,7 +3100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3093,74 +3111,74 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
+        <v>286</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>287</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>289</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="E4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="E5" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="E6" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="43"/>
@@ -3170,77 +3188,77 @@
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
       <c r="E9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="C10" s="31" t="s">
         <v>223</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>225</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>226</v>
       </c>
       <c r="C11" s="32"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="C13" s="31" t="s">
         <v>229</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
+        <v>246</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>247</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="C14" s="31" t="s">
         <v>248</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -3254,26 +3272,26 @@
       <c r="A19" s="39"/>
       <c r="B19" s="39"/>
       <c r="C19" s="40" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
@@ -3285,45 +3303,45 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="B24" s="34" t="s">
         <v>243</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>244</v>
       </c>
       <c r="C24" s="34"/>
       <c r="D24" s="28"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="41"/>
@@ -3335,23 +3353,23 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B32" s="36"/>
       <c r="C32" s="35" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="42"/>
@@ -3446,35 +3464,35 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" t="s">
+        <v>417</v>
+      </c>
+      <c r="F1" t="s">
         <v>186</v>
       </c>
-      <c r="E1" t="s">
-        <v>419</v>
-      </c>
-      <c r="F1" t="s">
-        <v>187</v>
-      </c>
       <c r="G1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J1" t="s">
+        <v>370</v>
+      </c>
+      <c r="K1" t="s">
         <v>371</v>
-      </c>
-      <c r="K1" t="s">
-        <v>372</v>
       </c>
       <c r="L1" t="s">
         <v>68</v>
@@ -3483,25 +3501,25 @@
         <v>71</v>
       </c>
       <c r="N1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="O1" t="s">
         <v>72</v>
       </c>
       <c r="P1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q1" t="s">
+        <v>372</v>
+      </c>
+      <c r="R1" t="s">
         <v>373</v>
-      </c>
-      <c r="R1" t="s">
-        <v>374</v>
       </c>
       <c r="S1" t="s">
         <v>21</v>
       </c>
       <c r="T1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="U1" t="s">
         <v>24</v>
@@ -3521,13 +3539,13 @@
         <v>58</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>60</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>61</v>
@@ -3560,13 +3578,13 @@
         <v>14</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="R2" s="24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="S2" s="9" t="s">
         <v>6</v>
@@ -3589,20 +3607,20 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J3">
         <v>10000</v>
@@ -3616,20 +3634,20 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H4">
         <f>100*8760</f>
@@ -3647,13 +3665,13 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J5">
         <v>10000</v>
@@ -3667,13 +3685,13 @@
         <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J6">
         <v>10000</v>
@@ -3684,22 +3702,22 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J7">
         <v>12000</v>
@@ -3716,16 +3734,16 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J8">
         <v>12000</v>
@@ -3776,7 +3794,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -3790,19 +3808,19 @@
         <v>70</v>
       </c>
       <c r="G1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H1" t="s">
+        <v>375</v>
+      </c>
+      <c r="I1" t="s">
         <v>376</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>372</v>
+      </c>
+      <c r="K1" t="s">
         <v>377</v>
-      </c>
-      <c r="J1" t="s">
-        <v>373</v>
-      </c>
-      <c r="K1" t="s">
-        <v>378</v>
       </c>
       <c r="L1" t="s">
         <v>21</v>
@@ -3811,7 +3829,7 @@
         <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3840,13 +3858,13 @@
         <v>13</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>6</v>
@@ -3863,7 +3881,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>79</v>
@@ -3878,7 +3896,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>80</v>
@@ -3893,10 +3911,10 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D5">
         <f>250*8760*1.1</f>
@@ -3932,7 +3950,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -3947,7 +3965,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>62</v>
@@ -3964,10 +3982,10 @@
         <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -4265,14 +4283,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1"/>
       <c r="C1" t="s">
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4286,7 +4304,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4294,7 +4312,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C3">
         <v>0.34</v>
@@ -4308,7 +4326,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C4">
         <v>0.2</v>
@@ -4343,12 +4361,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4362,7 +4380,7 @@
         <v>33</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4370,7 +4388,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>79</v>
@@ -4384,7 +4402,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>80</v>
@@ -4398,10 +4416,10 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D5">
         <v>22</v>
@@ -4450,18 +4468,18 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -4506,28 +4524,28 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G1" t="s">
         <v>183</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1" t="s">
         <v>184</v>
       </c>
-      <c r="H1" t="s">
-        <v>189</v>
-      </c>
-      <c r="I1" t="s">
-        <v>185</v>
-      </c>
       <c r="J1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K1" t="s">
         <v>20</v>
@@ -4536,19 +4554,19 @@
         <v>23</v>
       </c>
       <c r="M1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="N1" t="s">
         <v>26</v>
       </c>
       <c r="O1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P1" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q1" t="s">
         <v>381</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>382</v>
       </c>
       <c r="R1" t="s">
         <v>21</v>
@@ -4557,10 +4575,10 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
+        <v>382</v>
+      </c>
+      <c r="U1" t="s">
         <v>383</v>
-      </c>
-      <c r="U1" t="s">
-        <v>384</v>
       </c>
       <c r="V1" t="s">
         <v>19</v>
@@ -4574,13 +4592,13 @@
         <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>286</v>
-      </c>
       <c r="E2" s="24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -4592,7 +4610,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>15</v>
@@ -4610,13 +4628,13 @@
         <v>14</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>6</v>
@@ -4642,25 +4660,25 @@
         <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>152</v>
-      </c>
       <c r="E3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" t="s">
         <v>176</v>
       </c>
-      <c r="G3" t="s">
-        <v>177</v>
-      </c>
       <c r="H3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K3">
         <v>100</v>
@@ -4680,28 +4698,28 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>279</v>
-      </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" t="s">
         <v>176</v>
       </c>
-      <c r="G4" t="s">
-        <v>177</v>
-      </c>
       <c r="H4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K4">
         <v>10</v>
@@ -4712,19 +4730,19 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>152</v>
-      </c>
       <c r="H5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -4765,7 +4783,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4773,19 +4791,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H1" t="s">
+        <v>380</v>
+      </c>
+      <c r="I1" t="s">
         <v>381</v>
-      </c>
-      <c r="I1" t="s">
-        <v>382</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -4794,7 +4812,7 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -4817,13 +4835,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -4871,7 +4889,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -4906,7 +4924,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -4918,7 +4936,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
@@ -5178,23 +5196,23 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G1" t="s">
         <v>188</v>
-      </c>
-      <c r="G1" t="s">
-        <v>189</v>
       </c>
       <c r="H1" t="s">
         <v>20</v>
@@ -5203,19 +5221,19 @@
         <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K1" t="s">
         <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M1" t="s">
+        <v>384</v>
+      </c>
+      <c r="N1" t="s">
         <v>385</v>
-      </c>
-      <c r="N1" t="s">
-        <v>386</v>
       </c>
       <c r="O1" t="s">
         <v>21</v>
@@ -5224,28 +5242,28 @@
         <v>24</v>
       </c>
       <c r="Q1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="R1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="S1" t="s">
         <v>111</v>
       </c>
       <c r="T1" t="s">
+        <v>318</v>
+      </c>
+      <c r="U1" t="s">
         <v>319</v>
       </c>
-      <c r="U1" t="s">
-        <v>320</v>
-      </c>
       <c r="V1" t="s">
+        <v>202</v>
+      </c>
+      <c r="W1" t="s">
         <v>203</v>
       </c>
-      <c r="W1" t="s">
-        <v>204</v>
-      </c>
       <c r="X1" t="s">
-        <v>125</v>
+        <v>419</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5253,10 +5271,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>110</v>
@@ -5283,13 +5301,13 @@
         <v>14</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M2" s="24" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="O2" s="24" t="s">
         <v>6</v>
@@ -5327,20 +5345,20 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F3" s="47"/>
       <c r="G3" s="47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H3">
         <v>100</v>
@@ -5367,20 +5385,20 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H4">
         <v>100</v>
@@ -5394,20 +5412,20 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H5">
         <v>200</v>
@@ -5421,33 +5439,33 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G7" s="47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H7">
         <v>10</v>
@@ -5466,11 +5484,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5480,371 +5496,385 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" t="s">
         <v>196</v>
       </c>
-      <c r="C3" t="s">
-        <v>197</v>
-      </c>
       <c r="D3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B4" s="25">
         <v>44594</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B5" s="25">
         <v>44595</v>
       </c>
       <c r="C5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B6" s="25">
         <v>44600</v>
       </c>
       <c r="C6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B7" s="25">
         <v>44602</v>
       </c>
       <c r="C7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B8" s="25">
         <v>44602</v>
       </c>
       <c r="C8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B9" s="25">
         <v>44602</v>
       </c>
       <c r="C9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B10" s="25">
         <v>44602</v>
       </c>
       <c r="C10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B11" s="25">
         <v>44603</v>
       </c>
       <c r="C11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B12" s="25">
         <v>44605</v>
       </c>
       <c r="C12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B13" s="25">
         <v>44605</v>
       </c>
       <c r="C13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B14" s="25">
         <v>44605</v>
       </c>
       <c r="C14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B15" s="25">
         <v>44635</v>
       </c>
       <c r="C15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B16" s="25">
         <v>44643</v>
       </c>
       <c r="C16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B17" s="25">
         <v>44643</v>
       </c>
       <c r="C17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B18" s="25">
         <v>44643</v>
       </c>
       <c r="C18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D18" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B19" s="25">
         <v>44656</v>
       </c>
       <c r="C19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B20" s="25">
         <v>44657</v>
       </c>
       <c r="C20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B21" s="25">
         <v>44657</v>
       </c>
       <c r="C21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B22" s="25">
         <v>44680</v>
       </c>
       <c r="C22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D22" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B23" s="25">
         <v>44680</v>
       </c>
       <c r="C23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D23" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B24" s="25">
         <v>44690</v>
       </c>
       <c r="C24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D24" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B25" s="25">
         <v>44695</v>
       </c>
       <c r="C25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D25" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B26" s="25">
         <v>44701</v>
       </c>
       <c r="C26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D26" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B27" s="25">
         <v>44701</v>
       </c>
       <c r="C27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D27" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B28" s="25">
         <v>44712</v>
       </c>
       <c r="C28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D28" t="s">
-        <v>415</v>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="B29" s="25">
+        <v>44727</v>
+      </c>
+      <c r="C29" t="s">
+        <v>197</v>
+      </c>
+      <c r="D29" t="s">
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -5861,7 +5891,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5883,7 +5913,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5891,19 +5921,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H1" t="s">
+        <v>384</v>
+      </c>
+      <c r="I1" t="s">
         <v>385</v>
-      </c>
-      <c r="I1" t="s">
-        <v>386</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -5912,10 +5942,10 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5923,7 +5953,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>33</v>
@@ -5938,13 +5968,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -5964,7 +5994,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>79</v>
@@ -5978,7 +6008,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>80</v>
@@ -5992,10 +6022,10 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D5">
         <v>75</v>
@@ -6030,7 +6060,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6042,7 +6072,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
@@ -6053,10 +6083,10 @@
         <v>28</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -6264,7 +6294,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C13F0C3-2BD2-4859-9713-8823A445C2E8}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
@@ -6287,34 +6317,35 @@
     <col min="10" max="10" width="10.42578125" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" customWidth="1"/>
+    <col min="14" max="14" width="7.85546875" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I1" t="s">
         <v>120</v>
       </c>
       <c r="J1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K1" t="s">
         <v>122</v>
@@ -6322,31 +6353,34 @@
       <c r="L1" t="s">
         <v>124</v>
       </c>
-      <c r="O1" s="3"/>
+      <c r="M1" t="s">
+        <v>420</v>
+      </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" s="3"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>113</v>
@@ -6363,22 +6397,25 @@
       <c r="L2" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="O2" s="3"/>
+      <c r="M2" s="9" t="s">
+        <v>418</v>
+      </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -6390,18 +6427,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -6410,35 +6447,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6447,72 +6484,72 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>164</v>
-      </c>
       <c r="D8" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -6547,7 +6584,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6559,7 +6596,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>18</v>
@@ -6568,10 +6605,10 @@
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -6580,7 +6617,7 @@
         <v>58</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -6588,10 +6625,10 @@
         <v>28</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>345</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>346</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -6816,7 +6853,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6831,7 +6868,7 @@
         <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6839,19 +6876,19 @@
         <v>28</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7290,12 +7327,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7306,10 +7343,10 @@
         <v>58</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -7323,13 +7360,13 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>280</v>
-      </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -7362,12 +7399,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7378,10 +7415,10 @@
         <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -7398,10 +7435,10 @@
         <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -7435,13 +7472,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -7449,16 +7486,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>58</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -7472,16 +7509,16 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -7489,16 +7526,16 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E4" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -7530,15 +7567,15 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -7552,16 +7589,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>160</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -7575,13 +7612,13 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>182</v>
-      </c>
       <c r="D3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -7589,16 +7626,16 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>411</v>
-      </c>
       <c r="C4" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -7636,14 +7673,14 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -7657,19 +7694,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -7683,16 +7720,16 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -7703,16 +7740,16 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F4">
         <v>-0.1</v>
@@ -7720,19 +7757,19 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>409</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>347</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>411</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -7740,19 +7777,19 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>409</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>347</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>411</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -7785,10 +7822,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7797,42 +7834,42 @@
         <v>29</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>328</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>396</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>29</v>
@@ -7873,91 +7910,91 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="F4" t="s">
         <v>327</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="F4" t="s">
-        <v>328</v>
-      </c>
       <c r="G4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="K4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="M4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B5" s="14"/>
       <c r="G5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="K5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B11" s="14"/>
     </row>
@@ -7971,13 +8008,13 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7987,28 +8024,29 @@
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="22" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
-    <col min="15" max="16" width="20.85546875" customWidth="1"/>
-    <col min="17" max="18" width="16.7109375" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" customWidth="1"/>
-    <col min="20" max="24" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="17" width="20.85546875" customWidth="1"/>
+    <col min="18" max="19" width="16.7109375" customWidth="1"/>
+    <col min="20" max="20" width="16.42578125" customWidth="1"/>
+    <col min="21" max="25" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D1" t="s">
         <v>41</v>
@@ -8017,46 +8055,49 @@
         <v>37</v>
       </c>
       <c r="F1" t="s">
+        <v>423</v>
+      </c>
+      <c r="G1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>47</v>
       </c>
-      <c r="H1" t="s">
-        <v>389</v>
-      </c>
       <c r="I1" t="s">
+        <v>388</v>
+      </c>
+      <c r="J1" t="s">
         <v>45</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>55</v>
       </c>
-      <c r="K1" t="s">
-        <v>390</v>
-      </c>
       <c r="L1" t="s">
+        <v>422</v>
+      </c>
+      <c r="M1" t="s">
         <v>39</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>49</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>53</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>350</v>
+      </c>
+      <c r="Q1" t="s">
         <v>351</v>
-      </c>
-      <c r="P1" t="s">
-        <v>352</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>361</v>
       </c>
       <c r="R1" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -8064,7 +8105,7 @@
         <v>57</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>40</v>
@@ -8073,113 +8114,116 @@
         <v>36</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>298</v>
-      </c>
       <c r="L2" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q2" s="9" t="s">
         <v>349</v>
       </c>
-      <c r="P2" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="S2" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="R2" s="9" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="G4">
+        <v>290</v>
+      </c>
+      <c r="H4">
         <v>200</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>5000</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.6</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>5500</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="F5" t="s">
-        <v>163</v>
-      </c>
-      <c r="I5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="G5" t="s">
+        <v>162</v>
+      </c>
+      <c r="J5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="O6">
+        <v>353</v>
+      </c>
+      <c r="P6">
         <v>40</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -8218,7 +8262,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -8241,16 +8285,16 @@
         <v>51</v>
       </c>
       <c r="J1" t="s">
+        <v>350</v>
+      </c>
+      <c r="K1" t="s">
         <v>351</v>
       </c>
-      <c r="K1" t="s">
-        <v>352</v>
-      </c>
       <c r="L1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="M1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -8282,16 +8326,16 @@
         <v>50</v>
       </c>
       <c r="J2" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>349</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>350</v>
-      </c>
       <c r="L2" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>366</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -8299,7 +8343,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>79</v>
@@ -8313,7 +8357,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>80</v>
@@ -8327,10 +8371,10 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -8459,42 +8503,42 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -8523,7 +8567,7 @@
         <v>57</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -8562,7 +8606,7 @@
         <v>57</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>58</v>
@@ -8579,24 +8623,24 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -8633,26 +8677,26 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -8666,10 +8710,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>129</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>27</v>
@@ -8678,19 +8722,19 @@
         <v>58</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>133</v>
-      </c>
       <c r="J2" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -8701,22 +8745,22 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>32</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -8759,22 +8803,22 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -8788,25 +8832,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>129</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>57</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -8817,19 +8861,19 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>291</v>
-      </c>
       <c r="E3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -8870,7 +8914,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -8879,13 +8923,13 @@
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -8899,7 +8943,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -9060,15 +9104,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" t="s">
         <v>168</v>
-      </c>
-      <c r="E1" t="s">
-        <v>169</v>
       </c>
       <c r="F1" t="s">
         <v>77</v>
@@ -9088,16 +9132,16 @@
         <v>33</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>210</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -9111,16 +9155,16 @@
         <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -9134,18 +9178,18 @@
         <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>34</v>
@@ -9154,18 +9198,18 @@
         <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
@@ -9174,38 +9218,38 @@
         <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>35</v>
@@ -9214,53 +9258,53 @@
         <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E9">
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -9304,26 +9348,26 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -9337,31 +9381,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>129</v>
-      </c>
       <c r="D2" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>58</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>133</v>
-      </c>
       <c r="J2" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -9372,22 +9416,22 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I3">
         <v>0.5</v>
@@ -9398,22 +9442,22 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -9424,22 +9468,22 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I5">
         <v>0.01</v>
@@ -9450,22 +9494,22 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I6">
         <v>0.5</v>
@@ -9476,22 +9520,22 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I7">
         <v>0.01</v>
@@ -9531,14 +9575,14 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -9549,10 +9593,10 @@
         <v>78</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9566,13 +9610,13 @@
         <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>34</v>
@@ -9581,26 +9625,26 @@
         <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>35</v>
@@ -9609,65 +9653,65 @@
         <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D9" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D11" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -9701,7 +9745,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -9714,13 +9758,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>83</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -9728,7 +9772,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -9742,7 +9786,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>30</v>
@@ -9782,12 +9826,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -9798,10 +9842,10 @@
         <v>106</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -10173,7 +10217,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -10230,7 +10274,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>106</v>
@@ -10238,7 +10282,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>107</v>
@@ -10246,7 +10290,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>107</v>

</xml_diff>

<commit_message>
Fixing a bug with profile units having unlimited reserves. Improving and adding results.
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39E88DD-0044-4F03-95B6-4823CDED110E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693AC068-1150-46AC-8F53-DB225EF8AA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="1000" activeTab="1" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="427">
   <si>
     <t>commodity</t>
   </si>
@@ -770,9 +770,6 @@
     <t>Choice of investment method (only_invest, only_retire, invest_and_retire, not_allowed).</t>
   </si>
   <si>
-    <t>can_provide</t>
-  </si>
-  <si>
     <t>Can the unit provide this reserve. Empty indicates not allowed. Use 'yes' to indicate true.</t>
   </si>
   <si>
@@ -1479,6 +1476,12 @@
   </si>
   <si>
     <t>Added penalty for violating capacity margin</t>
+  </si>
+  <si>
+    <t>14.0</t>
+  </si>
+  <si>
+    <t>Changed 'can_provide' to 'is_active' for reserve_connection_node_c and reserve_unit_node_c</t>
   </si>
 </sst>
 </file>
@@ -3100,7 +3103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3111,74 +3114,74 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
+        <v>285</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>286</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>288</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="E4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="E5" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="E6" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="43"/>
@@ -3188,77 +3191,77 @@
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
       <c r="E9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="C10" s="31" t="s">
         <v>222</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>224</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>225</v>
       </c>
       <c r="C11" s="32"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>227</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="C13" s="31" t="s">
         <v>228</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="C14" s="31" t="s">
         <v>247</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -3272,26 +3275,26 @@
       <c r="A19" s="39"/>
       <c r="B19" s="39"/>
       <c r="C19" s="40" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
@@ -3303,45 +3306,45 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="B24" s="34" t="s">
         <v>242</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>243</v>
       </c>
       <c r="C24" s="34"/>
       <c r="D24" s="28"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="41"/>
@@ -3353,23 +3356,23 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B32" s="36"/>
       <c r="C32" s="35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="42"/>
@@ -3464,17 +3467,17 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D1" t="s">
         <v>185</v>
       </c>
       <c r="E1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F1" t="s">
         <v>186</v>
@@ -3489,10 +3492,10 @@
         <v>173</v>
       </c>
       <c r="J1" t="s">
+        <v>369</v>
+      </c>
+      <c r="K1" t="s">
         <v>370</v>
-      </c>
-      <c r="K1" t="s">
-        <v>371</v>
       </c>
       <c r="L1" t="s">
         <v>68</v>
@@ -3501,25 +3504,25 @@
         <v>71</v>
       </c>
       <c r="N1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O1" t="s">
         <v>72</v>
       </c>
       <c r="P1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Q1" t="s">
+        <v>371</v>
+      </c>
+      <c r="R1" t="s">
         <v>372</v>
-      </c>
-      <c r="R1" t="s">
-        <v>373</v>
       </c>
       <c r="S1" t="s">
         <v>21</v>
       </c>
       <c r="T1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="U1" t="s">
         <v>24</v>
@@ -3539,13 +3542,13 @@
         <v>58</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>60</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>61</v>
@@ -3578,13 +3581,13 @@
         <v>14</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="R2" s="24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="S2" s="9" t="s">
         <v>6</v>
@@ -3616,7 +3619,7 @@
         <v>162</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" t="s">
@@ -3643,7 +3646,7 @@
         <v>162</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" t="s">
@@ -3702,10 +3705,10 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>162</v>
@@ -3734,10 +3737,10 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>162</v>
@@ -3794,7 +3797,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -3808,19 +3811,19 @@
         <v>70</v>
       </c>
       <c r="G1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I1" t="s">
         <v>375</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>371</v>
+      </c>
+      <c r="K1" t="s">
         <v>376</v>
-      </c>
-      <c r="J1" t="s">
-        <v>372</v>
-      </c>
-      <c r="K1" t="s">
-        <v>377</v>
       </c>
       <c r="L1" t="s">
         <v>21</v>
@@ -3829,7 +3832,7 @@
         <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3858,13 +3861,13 @@
         <v>13</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>6</v>
@@ -3914,7 +3917,7 @@
         <v>150</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D5">
         <f>250*8760*1.1</f>
@@ -3950,7 +3953,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -4283,14 +4286,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1"/>
       <c r="C1" t="s">
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4361,12 +4364,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4419,7 +4422,7 @@
         <v>164</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D5">
         <v>22</v>
@@ -4524,13 +4527,13 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F1" t="s">
         <v>182</v>
@@ -4554,19 +4557,19 @@
         <v>23</v>
       </c>
       <c r="M1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N1" t="s">
         <v>26</v>
       </c>
       <c r="O1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P1" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q1" t="s">
         <v>380</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>381</v>
       </c>
       <c r="R1" t="s">
         <v>21</v>
@@ -4575,10 +4578,10 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
+        <v>381</v>
+      </c>
+      <c r="U1" t="s">
         <v>382</v>
-      </c>
-      <c r="U1" t="s">
-        <v>383</v>
       </c>
       <c r="V1" t="s">
         <v>19</v>
@@ -4592,13 +4595,13 @@
         <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>285</v>
-      </c>
       <c r="E2" s="24" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -4610,7 +4613,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>15</v>
@@ -4628,13 +4631,13 @@
         <v>14</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>6</v>
@@ -4698,16 +4701,16 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>150</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E4" t="s">
         <v>162</v>
@@ -4730,7 +4733,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>32</v>
@@ -4742,7 +4745,7 @@
         <v>151</v>
       </c>
       <c r="H5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -4783,7 +4786,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4791,19 +4794,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H1" t="s">
+        <v>379</v>
+      </c>
+      <c r="I1" t="s">
         <v>380</v>
-      </c>
-      <c r="I1" t="s">
-        <v>381</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -4812,7 +4815,7 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -4835,13 +4838,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -4889,7 +4892,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -4924,7 +4927,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5196,14 +5199,14 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E1" t="s">
         <v>183</v>
@@ -5221,19 +5224,19 @@
         <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K1" t="s">
         <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M1" t="s">
+        <v>383</v>
+      </c>
+      <c r="N1" t="s">
         <v>384</v>
-      </c>
-      <c r="N1" t="s">
-        <v>385</v>
       </c>
       <c r="O1" t="s">
         <v>21</v>
@@ -5242,7 +5245,7 @@
         <v>24</v>
       </c>
       <c r="Q1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="R1" t="s">
         <v>174</v>
@@ -5251,19 +5254,19 @@
         <v>111</v>
       </c>
       <c r="T1" t="s">
+        <v>317</v>
+      </c>
+      <c r="U1" t="s">
         <v>318</v>
       </c>
-      <c r="U1" t="s">
-        <v>319</v>
-      </c>
       <c r="V1" t="s">
+        <v>201</v>
+      </c>
+      <c r="W1" t="s">
         <v>202</v>
       </c>
-      <c r="W1" t="s">
-        <v>203</v>
-      </c>
       <c r="X1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5274,7 +5277,7 @@
         <v>125</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>110</v>
@@ -5301,13 +5304,13 @@
         <v>14</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M2" s="24" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O2" s="24" t="s">
         <v>6</v>
@@ -5351,7 +5354,7 @@
         <v>162</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E3" s="47" t="s">
         <v>176</v>
@@ -5391,7 +5394,7 @@
         <v>162</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E4" s="47" t="s">
         <v>176</v>
@@ -5418,10 +5421,10 @@
         <v>162</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47" t="s">
@@ -5439,27 +5442,27 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>153</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="C7" s="47" t="s">
         <v>162</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E7" s="47" t="s">
         <v>176</v>
@@ -5484,9 +5487,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5496,385 +5501,399 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" t="s">
         <v>195</v>
       </c>
-      <c r="C3" t="s">
-        <v>196</v>
-      </c>
       <c r="D3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B4" s="25">
         <v>44594</v>
       </c>
       <c r="C4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B5" s="25">
         <v>44595</v>
       </c>
       <c r="C5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B6" s="25">
         <v>44600</v>
       </c>
       <c r="C6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" s="25">
         <v>44602</v>
       </c>
       <c r="C7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B8" s="25">
         <v>44602</v>
       </c>
       <c r="C8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B9" s="25">
         <v>44602</v>
       </c>
       <c r="C9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B10" s="25">
         <v>44602</v>
       </c>
       <c r="C10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B11" s="25">
         <v>44603</v>
       </c>
       <c r="C11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B12" s="25">
         <v>44605</v>
       </c>
       <c r="C12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B13" s="25">
         <v>44605</v>
       </c>
       <c r="C13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B14" s="25">
         <v>44605</v>
       </c>
       <c r="C14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B15" s="25">
         <v>44635</v>
       </c>
       <c r="C15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B16" s="25">
         <v>44643</v>
       </c>
       <c r="C16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B17" s="25">
         <v>44643</v>
       </c>
       <c r="C17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B18" s="25">
         <v>44643</v>
       </c>
       <c r="C18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B19" s="25">
         <v>44656</v>
       </c>
       <c r="C19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B20" s="25">
         <v>44657</v>
       </c>
       <c r="C20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B21" s="25">
         <v>44657</v>
       </c>
       <c r="C21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B22" s="25">
         <v>44680</v>
       </c>
       <c r="C22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D22" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B23" s="25">
         <v>44680</v>
       </c>
       <c r="C23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D23" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B24" s="25">
         <v>44690</v>
       </c>
       <c r="C24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D24" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B25" s="25">
         <v>44695</v>
       </c>
       <c r="C25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D25" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B26" s="25">
         <v>44701</v>
       </c>
       <c r="C26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D26" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B27" s="25">
         <v>44701</v>
       </c>
       <c r="C27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D27" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B28" s="25">
         <v>44712</v>
       </c>
       <c r="C28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D28" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B29" s="25">
         <v>44727</v>
       </c>
       <c r="C29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D29" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>425</v>
+      </c>
+      <c r="B30" s="25">
+        <v>44734</v>
+      </c>
+      <c r="C30" t="s">
+        <v>196</v>
+      </c>
+      <c r="D30" t="s">
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -5913,7 +5932,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5921,19 +5940,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H1" t="s">
+        <v>383</v>
+      </c>
+      <c r="I1" t="s">
         <v>384</v>
-      </c>
-      <c r="I1" t="s">
-        <v>385</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -5942,7 +5961,7 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="M1" t="s">
         <v>174</v>
@@ -5968,13 +5987,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -6025,7 +6044,7 @@
         <v>153</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D5">
         <v>75</v>
@@ -6060,7 +6079,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6324,7 +6343,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6333,19 +6352,19 @@
         <v>144</v>
       </c>
       <c r="F1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I1" t="s">
         <v>120</v>
       </c>
       <c r="J1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K1" t="s">
         <v>122</v>
@@ -6354,7 +6373,7 @@
         <v>124</v>
       </c>
       <c r="M1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -6371,7 +6390,7 @@
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>142</v>
@@ -6380,7 +6399,7 @@
         <v>18</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>113</v>
@@ -6398,7 +6417,7 @@
         <v>123</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -6415,7 +6434,7 @@
         <v>152</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -6438,7 +6457,7 @@
         <v>150</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -6458,7 +6477,7 @@
         <v>163</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -6475,7 +6494,7 @@
         <v>151</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6495,7 +6514,7 @@
         <v>150</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -6506,16 +6525,16 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>163</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -6523,16 +6542,16 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>150</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -6540,16 +6559,16 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>408</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -6584,7 +6603,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6625,10 +6644,10 @@
         <v>28</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>345</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -6868,7 +6887,7 @@
         <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6882,13 +6901,13 @@
         <v>148</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7327,12 +7346,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7360,10 +7379,10 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>279</v>
       </c>
       <c r="D3" t="s">
         <v>179</v>
@@ -7399,12 +7418,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7435,7 +7454,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D3" t="s">
         <v>179</v>
@@ -7472,13 +7491,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -7526,16 +7545,16 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C4" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>415</v>
-      </c>
       <c r="E4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -7567,12 +7586,12 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E1" t="s">
         <v>160</v>
@@ -7595,7 +7614,7 @@
         <v>158</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>159</v>
@@ -7626,13 +7645,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>409</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>410</v>
       </c>
       <c r="D4" t="s">
         <v>162</v>
@@ -7657,7 +7676,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7673,7 +7692,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7700,7 +7719,7 @@
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>146</v>
@@ -7726,7 +7745,7 @@
         <v>152</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>180</v>
@@ -7746,7 +7765,7 @@
         <v>150</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>180</v>
@@ -7757,19 +7776,19 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>163</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -7777,19 +7796,19 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>150</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -7822,10 +7841,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7834,42 +7853,42 @@
         <v>29</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>327</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>394</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>29</v>
@@ -7910,91 +7929,91 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="F4" t="s">
         <v>326</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>301</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="F4" t="s">
-        <v>327</v>
-      </c>
       <c r="G4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="M4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B5" s="14"/>
       <c r="G5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J5" t="s">
+        <v>392</v>
+      </c>
+      <c r="K5" t="s">
         <v>393</v>
-      </c>
-      <c r="K5" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B11" s="14"/>
     </row>
@@ -8042,11 +8061,11 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D1" t="s">
         <v>41</v>
@@ -8055,7 +8074,7 @@
         <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G1" t="s">
         <v>43</v>
@@ -8064,7 +8083,7 @@
         <v>47</v>
       </c>
       <c r="I1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J1" t="s">
         <v>45</v>
@@ -8073,7 +8092,7 @@
         <v>55</v>
       </c>
       <c r="L1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="M1" t="s">
         <v>39</v>
@@ -8085,16 +8104,16 @@
         <v>53</v>
       </c>
       <c r="P1" t="s">
+        <v>349</v>
+      </c>
+      <c r="Q1" t="s">
         <v>350</v>
       </c>
-      <c r="Q1" t="s">
-        <v>351</v>
-      </c>
       <c r="R1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="S1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -8105,7 +8124,7 @@
         <v>57</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>40</v>
@@ -8114,7 +8133,7 @@
         <v>36</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>42</v>
@@ -8132,7 +8151,7 @@
         <v>54</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>38</v>
@@ -8144,16 +8163,16 @@
         <v>52</v>
       </c>
       <c r="P2" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="Q2" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="Q2" s="9" t="s">
-        <v>349</v>
-      </c>
       <c r="R2" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="S2" s="9" t="s">
         <v>365</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -8172,7 +8191,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H4">
         <v>200</v>
@@ -8189,10 +8208,10 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G5" t="s">
         <v>162</v>
@@ -8203,10 +8222,10 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P6">
         <v>40</v>
@@ -8220,7 +8239,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C7" t="s">
         <v>162</v>
@@ -8262,7 +8281,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -8285,16 +8304,16 @@
         <v>51</v>
       </c>
       <c r="J1" t="s">
+        <v>349</v>
+      </c>
+      <c r="K1" t="s">
         <v>350</v>
       </c>
-      <c r="K1" t="s">
-        <v>351</v>
-      </c>
       <c r="L1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="M1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -8326,16 +8345,16 @@
         <v>50</v>
       </c>
       <c r="J2" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>349</v>
-      </c>
       <c r="L2" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>365</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -8374,7 +8393,7 @@
         <v>156</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -8519,7 +8538,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>150</v>
@@ -8527,7 +8546,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>150</v>
@@ -8535,7 +8554,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>151</v>
@@ -8623,7 +8642,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>153</v>
@@ -8634,7 +8653,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>165</v>
@@ -8677,14 +8696,14 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G1" t="s">
         <v>130</v>
@@ -8722,7 +8741,7 @@
         <v>58</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>189</v>
+        <v>301</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>129</v>
@@ -8745,13 +8764,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>32</v>
@@ -8803,22 +8822,22 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F1" t="s">
         <v>138</v>
       </c>
       <c r="G1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -8861,19 +8880,19 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>290</v>
-      </c>
       <c r="E3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -8914,7 +8933,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -9104,7 +9123,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -9132,16 +9151,16 @@
         <v>33</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>161</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>209</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -9189,7 +9208,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>34</v>
@@ -9209,7 +9228,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
@@ -9229,7 +9248,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>166</v>
@@ -9249,7 +9268,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>35</v>
@@ -9269,13 +9288,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D9" t="s">
         <v>170</v>
@@ -9289,10 +9308,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>80</v>
@@ -9329,7 +9348,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9348,14 +9367,14 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G1" t="s">
         <v>130</v>
@@ -9393,7 +9412,7 @@
         <v>58</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>189</v>
+        <v>301</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>129</v>
@@ -9416,13 +9435,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>153</v>
@@ -9442,13 +9461,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>154</v>
@@ -9468,13 +9487,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>153</v>
@@ -9494,13 +9513,13 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>165</v>
@@ -9520,13 +9539,13 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>153</v>
@@ -9575,14 +9594,14 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -9596,7 +9615,7 @@
         <v>171</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9610,13 +9629,13 @@
         <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>34</v>
@@ -9625,12 +9644,12 @@
         <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>166</v>
@@ -9639,12 +9658,12 @@
         <v>172</v>
       </c>
       <c r="D5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>35</v>
@@ -9653,65 +9672,65 @@
         <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C7" t="s">
         <v>172</v>
       </c>
       <c r="D7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>166</v>
       </c>
       <c r="D9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11" t="s">
         <v>404</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D11" t="s">
-        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -9745,7 +9764,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -9758,13 +9777,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>83</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -9826,12 +9845,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -9842,10 +9861,10 @@
         <v>106</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -10217,7 +10236,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -10274,7 +10293,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>106</v>

</xml_diff>

<commit_message>
profile constraints made more simple
</commit_message>
<xml_diff>
--- a/FlexTool3_import_template.xlsx
+++ b/FlexTool3_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693AC068-1150-46AC-8F53-DB225EF8AA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79382EC-4474-4591-B3DE-D98B31AB9CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="1000" firstSheet="6" activeTab="28" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -632,9 +632,6 @@
     <t>coefficient</t>
   </si>
   <si>
-    <t>constraint_coefficient</t>
-  </si>
-  <si>
     <t>[factor] Coefficient to scale the output from a unit to a particular node (also affected by unit efficiency). Constant.</t>
   </si>
   <si>
@@ -1482,6 +1479,9 @@
   </si>
   <si>
     <t>Changed 'can_provide' to 'is_active' for reserve_connection_node_c and reserve_unit_node_c</t>
+  </si>
+  <si>
+    <t>constraint_flow_coefficient</t>
   </si>
 </sst>
 </file>
@@ -3103,7 +3103,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3114,74 +3116,74 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>285</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>287</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="E4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="E5" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="E6" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="43"/>
@@ -3191,77 +3193,77 @@
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
       <c r="E9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="C10" s="31" t="s">
         <v>221</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>223</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>224</v>
       </c>
       <c r="C11" s="32"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>226</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="C13" s="31" t="s">
         <v>227</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="C14" s="31" t="s">
         <v>246</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -3275,26 +3277,26 @@
       <c r="A19" s="39"/>
       <c r="B19" s="39"/>
       <c r="C19" s="40" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
@@ -3306,45 +3308,45 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="B24" s="34" t="s">
         <v>241</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>242</v>
       </c>
       <c r="C24" s="34"/>
       <c r="D24" s="28"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="41"/>
@@ -3356,23 +3358,23 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B32" s="36"/>
       <c r="C32" s="35" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="42"/>
@@ -3467,35 +3469,35 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" t="s">
+        <v>415</v>
+      </c>
+      <c r="F1" t="s">
         <v>185</v>
       </c>
-      <c r="E1" t="s">
-        <v>416</v>
-      </c>
-      <c r="F1" t="s">
-        <v>186</v>
-      </c>
       <c r="G1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J1" t="s">
+        <v>368</v>
+      </c>
+      <c r="K1" t="s">
         <v>369</v>
-      </c>
-      <c r="K1" t="s">
-        <v>370</v>
       </c>
       <c r="L1" t="s">
         <v>68</v>
@@ -3504,25 +3506,25 @@
         <v>71</v>
       </c>
       <c r="N1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="O1" t="s">
         <v>72</v>
       </c>
       <c r="P1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Q1" t="s">
+        <v>370</v>
+      </c>
+      <c r="R1" t="s">
         <v>371</v>
-      </c>
-      <c r="R1" t="s">
-        <v>372</v>
       </c>
       <c r="S1" t="s">
         <v>21</v>
       </c>
       <c r="T1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="U1" t="s">
         <v>24</v>
@@ -3542,13 +3544,13 @@
         <v>58</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>60</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>61</v>
@@ -3581,13 +3583,13 @@
         <v>14</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="R2" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="S2" s="9" t="s">
         <v>6</v>
@@ -3610,20 +3612,20 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J3">
         <v>10000</v>
@@ -3637,20 +3639,20 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H4">
         <f>100*8760</f>
@@ -3668,13 +3670,13 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J5">
         <v>10000</v>
@@ -3688,13 +3690,13 @@
         <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J6">
         <v>10000</v>
@@ -3705,22 +3707,22 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J7">
         <v>12000</v>
@@ -3737,16 +3739,16 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J8">
         <v>12000</v>
@@ -3797,7 +3799,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -3811,19 +3813,19 @@
         <v>70</v>
       </c>
       <c r="G1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I1" t="s">
         <v>374</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>370</v>
+      </c>
+      <c r="K1" t="s">
         <v>375</v>
-      </c>
-      <c r="J1" t="s">
-        <v>371</v>
-      </c>
-      <c r="K1" t="s">
-        <v>376</v>
       </c>
       <c r="L1" t="s">
         <v>21</v>
@@ -3832,7 +3834,7 @@
         <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3861,13 +3863,13 @@
         <v>13</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>6</v>
@@ -3884,7 +3886,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>79</v>
@@ -3899,7 +3901,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>80</v>
@@ -3914,10 +3916,10 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D5">
         <f>250*8760*1.1</f>
@@ -3953,7 +3955,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -3968,7 +3970,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>62</v>
@@ -3985,10 +3987,10 @@
         <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -4286,14 +4288,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1"/>
       <c r="C1" t="s">
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4315,7 +4317,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C3">
         <v>0.34</v>
@@ -4329,7 +4331,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4">
         <v>0.2</v>
@@ -4364,12 +4366,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4391,7 +4393,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>79</v>
@@ -4405,7 +4407,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>80</v>
@@ -4419,10 +4421,10 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D5">
         <v>22</v>
@@ -4471,18 +4473,18 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -4527,28 +4529,28 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" t="s">
         <v>182</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I1" t="s">
         <v>183</v>
       </c>
-      <c r="H1" t="s">
-        <v>188</v>
-      </c>
-      <c r="I1" t="s">
-        <v>184</v>
-      </c>
       <c r="J1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K1" t="s">
         <v>20</v>
@@ -4557,19 +4559,19 @@
         <v>23</v>
       </c>
       <c r="M1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="N1" t="s">
         <v>26</v>
       </c>
       <c r="O1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="P1" t="s">
+        <v>378</v>
+      </c>
+      <c r="Q1" t="s">
         <v>379</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>380</v>
       </c>
       <c r="R1" t="s">
         <v>21</v>
@@ -4578,10 +4580,10 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
+        <v>380</v>
+      </c>
+      <c r="U1" t="s">
         <v>381</v>
-      </c>
-      <c r="U1" t="s">
-        <v>382</v>
       </c>
       <c r="V1" t="s">
         <v>19</v>
@@ -4595,13 +4597,13 @@
         <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>284</v>
-      </c>
       <c r="E2" s="24" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -4613,7 +4615,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>15</v>
@@ -4631,13 +4633,13 @@
         <v>14</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>6</v>
@@ -4663,25 +4665,25 @@
         <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>151</v>
-      </c>
       <c r="E3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G3" t="s">
         <v>175</v>
       </c>
-      <c r="G3" t="s">
-        <v>176</v>
-      </c>
       <c r="H3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K3">
         <v>100</v>
@@ -4701,28 +4703,28 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>277</v>
-      </c>
       <c r="E4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G4" t="s">
         <v>175</v>
       </c>
-      <c r="G4" t="s">
-        <v>176</v>
-      </c>
       <c r="H4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K4">
         <v>10</v>
@@ -4733,19 +4735,19 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>151</v>
-      </c>
       <c r="H5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -4786,7 +4788,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4794,19 +4796,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H1" t="s">
+        <v>378</v>
+      </c>
+      <c r="I1" t="s">
         <v>379</v>
-      </c>
-      <c r="I1" t="s">
-        <v>380</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -4815,7 +4817,7 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -4838,13 +4840,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -4892,7 +4894,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -4927,7 +4929,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -4939,7 +4941,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
@@ -5199,23 +5201,23 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G1" t="s">
         <v>187</v>
-      </c>
-      <c r="G1" t="s">
-        <v>188</v>
       </c>
       <c r="H1" t="s">
         <v>20</v>
@@ -5224,19 +5226,19 @@
         <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K1" t="s">
         <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M1" t="s">
+        <v>382</v>
+      </c>
+      <c r="N1" t="s">
         <v>383</v>
-      </c>
-      <c r="N1" t="s">
-        <v>384</v>
       </c>
       <c r="O1" t="s">
         <v>21</v>
@@ -5245,28 +5247,28 @@
         <v>24</v>
       </c>
       <c r="Q1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="R1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S1" t="s">
         <v>111</v>
       </c>
       <c r="T1" t="s">
+        <v>316</v>
+      </c>
+      <c r="U1" t="s">
         <v>317</v>
       </c>
-      <c r="U1" t="s">
-        <v>318</v>
-      </c>
       <c r="V1" t="s">
+        <v>200</v>
+      </c>
+      <c r="W1" t="s">
         <v>201</v>
       </c>
-      <c r="W1" t="s">
-        <v>202</v>
-      </c>
       <c r="X1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5277,7 +5279,7 @@
         <v>125</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>110</v>
@@ -5304,13 +5306,13 @@
         <v>14</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M2" s="24" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O2" s="24" t="s">
         <v>6</v>
@@ -5348,20 +5350,20 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F3" s="47"/>
       <c r="G3" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H3">
         <v>100</v>
@@ -5388,20 +5390,20 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H4">
         <v>100</v>
@@ -5415,20 +5417,20 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H5">
         <v>200</v>
@@ -5442,33 +5444,33 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="C7" s="47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G7" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H7">
         <v>10</v>
@@ -5501,399 +5503,399 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" t="s">
         <v>194</v>
       </c>
-      <c r="C3" t="s">
-        <v>195</v>
-      </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B4" s="25">
         <v>44594</v>
       </c>
       <c r="C4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B5" s="25">
         <v>44595</v>
       </c>
       <c r="C5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B6" s="25">
         <v>44600</v>
       </c>
       <c r="C6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B7" s="25">
         <v>44602</v>
       </c>
       <c r="C7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B8" s="25">
         <v>44602</v>
       </c>
       <c r="C8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B9" s="25">
         <v>44602</v>
       </c>
       <c r="C9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B10" s="25">
         <v>44602</v>
       </c>
       <c r="C10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B11" s="25">
         <v>44603</v>
       </c>
       <c r="C11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B12" s="25">
         <v>44605</v>
       </c>
       <c r="C12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B13" s="25">
         <v>44605</v>
       </c>
       <c r="C13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B14" s="25">
         <v>44605</v>
       </c>
       <c r="C14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B15" s="25">
         <v>44635</v>
       </c>
       <c r="C15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B16" s="25">
         <v>44643</v>
       </c>
       <c r="C16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B17" s="25">
         <v>44643</v>
       </c>
       <c r="C17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B18" s="25">
         <v>44643</v>
       </c>
       <c r="C18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D18" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B19" s="25">
         <v>44656</v>
       </c>
       <c r="C19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D19" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B20" s="25">
         <v>44657</v>
       </c>
       <c r="C20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B21" s="25">
         <v>44657</v>
       </c>
       <c r="C21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D21" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B22" s="25">
         <v>44680</v>
       </c>
       <c r="C22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B23" s="25">
         <v>44680</v>
       </c>
       <c r="C23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D23" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B24" s="25">
         <v>44690</v>
       </c>
       <c r="C24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D24" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B25" s="25">
         <v>44695</v>
       </c>
       <c r="C25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D25" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B26" s="25">
         <v>44701</v>
       </c>
       <c r="C26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D26" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B27" s="25">
         <v>44701</v>
       </c>
       <c r="C27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D27" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B28" s="25">
         <v>44712</v>
       </c>
       <c r="C28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D28" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B29" s="25">
         <v>44727</v>
       </c>
       <c r="C29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D29" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B30" s="25">
         <v>44734</v>
       </c>
       <c r="C30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D30" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -5932,7 +5934,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5940,19 +5942,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H1" t="s">
+        <v>382</v>
+      </c>
+      <c r="I1" t="s">
         <v>383</v>
-      </c>
-      <c r="I1" t="s">
-        <v>384</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -5961,10 +5963,10 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="M1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5987,13 +5989,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -6013,7 +6015,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>79</v>
@@ -6027,7 +6029,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>80</v>
@@ -6041,10 +6043,10 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D5">
         <v>75</v>
@@ -6079,7 +6081,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6091,7 +6093,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
@@ -6105,7 +6107,7 @@
         <v>125</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -6343,28 +6345,28 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I1" t="s">
         <v>120</v>
       </c>
       <c r="J1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K1" t="s">
         <v>122</v>
@@ -6373,7 +6375,7 @@
         <v>124</v>
       </c>
       <c r="M1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -6390,7 +6392,7 @@
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>142</v>
@@ -6399,7 +6401,7 @@
         <v>18</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>113</v>
@@ -6417,7 +6419,7 @@
         <v>123</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -6428,13 +6430,13 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -6451,13 +6453,13 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -6471,13 +6473,13 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -6488,13 +6490,13 @@
         <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6508,33 +6510,33 @@
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -6542,16 +6544,16 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -6559,16 +6561,16 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -6603,7 +6605,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6615,7 +6617,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>18</v>
@@ -6627,7 +6629,7 @@
         <v>125</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -6636,7 +6638,7 @@
         <v>58</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -6644,10 +6646,10 @@
         <v>28</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>344</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -6872,7 +6874,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6887,7 +6889,7 @@
         <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6895,19 +6897,19 @@
         <v>28</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7346,12 +7348,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7362,10 +7364,10 @@
         <v>58</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -7379,13 +7381,13 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>278</v>
-      </c>
       <c r="D3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -7418,12 +7420,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7434,10 +7436,10 @@
         <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -7454,10 +7456,10 @@
         <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -7491,13 +7493,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -7511,10 +7513,10 @@
         <v>58</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -7528,16 +7530,16 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -7545,16 +7547,16 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C4" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>414</v>
-      </c>
       <c r="E4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -7586,15 +7588,15 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -7608,16 +7610,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>158</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>159</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -7631,13 +7633,13 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>181</v>
-      </c>
       <c r="D3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -7645,16 +7647,16 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>409</v>
-      </c>
       <c r="D4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -7672,11 +7674,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA1124C-4BD2-46D2-BD33-99ED754CAC73}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7686,20 +7688,20 @@
     <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="20" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
     <col min="7" max="10" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -7719,13 +7721,13 @@
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>143</v>
+        <v>426</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -7739,16 +7741,16 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -7759,16 +7761,16 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F4">
         <v>-0.1</v>
@@ -7776,19 +7778,19 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>407</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>345</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>408</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -7796,19 +7798,19 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>407</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>345</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>408</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -7841,10 +7843,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7853,42 +7855,42 @@
         <v>29</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>326</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>393</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>29</v>
@@ -7929,91 +7931,91 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="F4" t="s">
         <v>325</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>327</v>
-      </c>
-      <c r="F4" t="s">
-        <v>326</v>
-      </c>
       <c r="G4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="M4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B5" s="14"/>
       <c r="G5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J5" t="s">
+        <v>391</v>
+      </c>
+      <c r="K5" t="s">
         <v>392</v>
-      </c>
-      <c r="K5" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B11" s="14"/>
     </row>
@@ -8061,11 +8063,11 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D1" t="s">
         <v>41</v>
@@ -8074,7 +8076,7 @@
         <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G1" t="s">
         <v>43</v>
@@ -8083,7 +8085,7 @@
         <v>47</v>
       </c>
       <c r="I1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J1" t="s">
         <v>45</v>
@@ -8092,7 +8094,7 @@
         <v>55</v>
       </c>
       <c r="L1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M1" t="s">
         <v>39</v>
@@ -8104,16 +8106,16 @@
         <v>53</v>
       </c>
       <c r="P1" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q1" t="s">
         <v>349</v>
       </c>
-      <c r="Q1" t="s">
-        <v>350</v>
-      </c>
       <c r="R1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -8124,7 +8126,7 @@
         <v>57</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>40</v>
@@ -8133,7 +8135,7 @@
         <v>36</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>42</v>
@@ -8151,7 +8153,7 @@
         <v>54</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>38</v>
@@ -8163,16 +8165,16 @@
         <v>52</v>
       </c>
       <c r="P2" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q2" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="Q2" s="9" t="s">
-        <v>348</v>
-      </c>
       <c r="R2" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="S2" s="9" t="s">
         <v>364</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -8180,7 +8182,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -8191,7 +8193,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H4">
         <v>200</v>
@@ -8208,24 +8210,24 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="P6">
         <v>40</v>
@@ -8239,10 +8241,10 @@
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -8281,7 +8283,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -8304,16 +8306,16 @@
         <v>51</v>
       </c>
       <c r="J1" t="s">
+        <v>348</v>
+      </c>
+      <c r="K1" t="s">
         <v>349</v>
       </c>
-      <c r="K1" t="s">
-        <v>350</v>
-      </c>
       <c r="L1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -8345,16 +8347,16 @@
         <v>50</v>
       </c>
       <c r="J2" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>348</v>
-      </c>
       <c r="L2" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>364</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -8362,7 +8364,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>79</v>
@@ -8376,7 +8378,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>80</v>
@@ -8390,10 +8392,10 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -8522,42 +8524,42 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -8642,24 +8644,24 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -8696,14 +8698,14 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G1" t="s">
         <v>130</v>
@@ -8741,7 +8743,7 @@
         <v>58</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>129</v>
@@ -8764,22 +8766,22 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>32</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -8822,22 +8824,22 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F1" t="s">
         <v>138</v>
       </c>
       <c r="G1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -8880,19 +8882,19 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>289</v>
-      </c>
       <c r="E3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -8933,7 +8935,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -8962,7 +8964,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -9123,15 +9125,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" t="s">
         <v>167</v>
-      </c>
-      <c r="E1" t="s">
-        <v>168</v>
       </c>
       <c r="F1" t="s">
         <v>77</v>
@@ -9151,16 +9153,16 @@
         <v>33</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>208</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -9174,16 +9176,16 @@
         <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -9197,18 +9199,18 @@
         <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>34</v>
@@ -9217,18 +9219,18 @@
         <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
@@ -9237,38 +9239,38 @@
         <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>35</v>
@@ -9277,53 +9279,53 @@
         <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E9">
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -9367,14 +9369,14 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G1" t="s">
         <v>130</v>
@@ -9412,7 +9414,7 @@
         <v>58</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>129</v>
@@ -9435,22 +9437,22 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I3">
         <v>0.5</v>
@@ -9461,22 +9463,22 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -9487,22 +9489,22 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I5">
         <v>0.01</v>
@@ -9513,22 +9515,22 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I6">
         <v>0.5</v>
@@ -9539,22 +9541,22 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I7">
         <v>0.01</v>
@@ -9594,14 +9596,14 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -9612,10 +9614,10 @@
         <v>78</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9629,13 +9631,13 @@
         <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>34</v>
@@ -9644,26 +9646,26 @@
         <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>35</v>
@@ -9672,65 +9674,65 @@
         <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" t="s">
         <v>403</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D9" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D11" t="s">
         <v>403</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D11" t="s">
-        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -9764,7 +9766,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -9777,13 +9779,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>83</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -9791,7 +9793,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -9805,7 +9807,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>30</v>
@@ -9845,12 +9847,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -9861,10 +9863,10 @@
         <v>106</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -10236,7 +10238,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -10293,7 +10295,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>106</v>
@@ -10301,7 +10303,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>107</v>
@@ -10309,7 +10311,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>107</v>

</xml_diff>